<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@afafaaa8028a0df3789659a11dc8a323898920b7 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B56B0B-9D0B-4844-A69C-A42440E24106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D9C5D8-FCC2-46FA-9895-9F52A5DC6DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5810" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5810" uniqueCount="693">
   <si>
     <t>name</t>
   </si>
@@ -1761,14 +1761,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>../../assets/img/octocat.png</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/马娆.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>MP</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1789,34 +1781,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>../../assets/img/members/faculty/qym_square.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/陈哲怀.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/谢其哲.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/贺天行.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/郑达.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/王帅.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/胡虎.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>杨景凯</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1829,61 +1793,340 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>../../assets/img/members/student/杨景凯.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/王瀚坤.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/张思拓.jpg</t>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/罗丹宇.jpg</t>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/王鹏宇.jpg</t>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/陈思远.jpg</t>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/宋哲书.jpg</t>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/韩杨.jpg</t>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/黎井漂.jpg</t>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/靳秉睿.jpg</t>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/张熙灼.jpg</t>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/申振南.jpg</t>
-  </si>
-  <si>
-    <t>../../assets/img/members/student/郭思佳.jpg</t>
-  </si>
-  <si>
     <t>殷国航</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>../../assets/img/members/student/殷国航.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>万一</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>../../assets/img/members/student/万一.jpg</t>
+    <t>张熙灼</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>octocat.png</t>
+  </si>
+  <si>
+    <t>members/student/刘媛.jpg</t>
+  </si>
+  <si>
+    <t>members/student/邓威.jpg</t>
+  </si>
+  <si>
+    <t>members/student/王佩璐.jpg</t>
+  </si>
+  <si>
+    <t>members/student/贺天行.jpg</t>
+  </si>
+  <si>
+    <t>members/student/符天凡.jpg</t>
+  </si>
+  <si>
+    <t>members/student/陈博.jpg</t>
+  </si>
+  <si>
+    <t>members/student/万一.jpg</t>
+  </si>
+  <si>
+    <t>members/student/郑达.jpg</t>
+  </si>
+  <si>
+    <t>members/student/陈哲怀.jpg</t>
+  </si>
+  <si>
+    <t>members/student/毕梦霄.jpg</t>
+  </si>
+  <si>
+    <t>members/student/谢其哲.jpg</t>
+  </si>
+  <si>
+    <t>members/student/王帅.jpg</t>
+  </si>
+  <si>
+    <t>members/student/吴学阳.jpg</t>
+  </si>
+  <si>
+    <t>members/student/李翰正.jpg</t>
+  </si>
+  <si>
+    <t>members/student/丁文.jpg</t>
+  </si>
+  <si>
+    <t>members/student/石开宇.jpg</t>
+  </si>
+  <si>
+    <t>members/student/杨叶新.jpg</t>
+  </si>
+  <si>
+    <t>members/student/胡虎.jpg</t>
+  </si>
+  <si>
+    <t>members/student/郭嘉祺.jpg</t>
+  </si>
+  <si>
+    <t>members/student/杜晨鹏.jpg</t>
+  </si>
+  <si>
+    <t>members/student/曹瑞升.jpg</t>
+  </si>
+  <si>
+    <t>members/student/王鸿基.jpg</t>
+  </si>
+  <si>
+    <t>members/student/陈正阳.jpg</t>
+  </si>
+  <si>
+    <t>members/student/许洪深.jpg</t>
+  </si>
+  <si>
+    <t>members/student/李杰宇.jpg</t>
+  </si>
+  <si>
+    <t>members/student/陈星宇.jpg</t>
+  </si>
+  <si>
+    <t>members/student/马达.jpg</t>
+  </si>
+  <si>
+    <t>members/student/吕波尔.jpg</t>
+  </si>
+  <si>
+    <t>members/student/徐薛楠.jpg</t>
+  </si>
+  <si>
+    <t>members/student/徐子涵.jpg</t>
+  </si>
+  <si>
+    <t>members/student/赵梓涵.jpg</t>
+  </si>
+  <si>
+    <t>members/student/奚彧.jpg</t>
+  </si>
+  <si>
+    <t>members/student/吴逸飞.jpg</t>
+  </si>
+  <si>
+    <t>members/student/张丹阳.jpg</t>
+  </si>
+  <si>
+    <t>members/student/刘涛.jpg</t>
+  </si>
+  <si>
+    <t>members/student/兰焜耀.jpg</t>
+  </si>
+  <si>
+    <t>members/student/刘森.jpg</t>
+  </si>
+  <si>
+    <t>members/student/谢泽宇.jpg</t>
+  </si>
+  <si>
+    <t>members/student/徐晓航.jpg</t>
+  </si>
+  <si>
+    <t>members/student/张思拓.jpg</t>
+  </si>
+  <si>
+    <t>members/student/卢葛威.jpg</t>
+  </si>
+  <si>
+    <t>members/student/罗丹宇.jpg</t>
+  </si>
+  <si>
+    <t>members/student/王鹏宇.jpg</t>
+  </si>
+  <si>
+    <t>members/student/朱梓臣.jpg</t>
+  </si>
+  <si>
+    <t>members/student/罗嘉鸣.jpg</t>
+  </si>
+  <si>
+    <t>members/student/卓建衡.jpg</t>
+  </si>
+  <si>
+    <t>members/student/陈思远.jpg</t>
+  </si>
+  <si>
+    <t>members/student/王瀚坤.jpg</t>
+  </si>
+  <si>
+    <t>members/student/马子阳.jpg</t>
+  </si>
+  <si>
+    <t>members/student/杨冠柔.jpg</t>
+  </si>
+  <si>
+    <t>members/student/宋哲书.jpg</t>
+  </si>
+  <si>
+    <t>members/student/张淳皓.jpg</t>
+  </si>
+  <si>
+    <t>members/student/李柏涵.jpg</t>
+  </si>
+  <si>
+    <t>members/student/郭奕玮.jpg</t>
+  </si>
+  <si>
+    <t>members/student/李浩宇.jpg</t>
+  </si>
+  <si>
+    <t>members/student/张耀匀.jpg</t>
+  </si>
+  <si>
+    <t>members/student/肖云冲.jpg</t>
+  </si>
+  <si>
+    <t>members/student/吕铭浩.jpg</t>
+  </si>
+  <si>
+    <t>members/student/宋秀杰.jpg</t>
+  </si>
+  <si>
+    <t>members/student/张晗翀.jpg</t>
+  </si>
+  <si>
+    <t>members/student/韩杨.jpg</t>
+  </si>
+  <si>
+    <t>members/student/韩森宇.jpg</t>
+  </si>
+  <si>
+    <t>members/student/黎井漂.jpg</t>
+  </si>
+  <si>
+    <t>members/student/孙良泰.jpg</t>
+  </si>
+  <si>
+    <t>members/student/杨亦凡.jpg</t>
+  </si>
+  <si>
+    <t>members/student/何朝帆.jpg</t>
+  </si>
+  <si>
+    <t>members/student/杨飞.jpg</t>
+  </si>
+  <si>
+    <t>members/student/李星源.jpg</t>
+  </si>
+  <si>
+    <t>members/student/曾泓川.JPG</t>
+  </si>
+  <si>
+    <t>members/student/牛志康.jpg</t>
+  </si>
+  <si>
+    <t>members/student/沈飞宇.jpg</t>
+  </si>
+  <si>
+    <t>members/student/林少雄.jpg</t>
+  </si>
+  <si>
+    <t>members/student/任立椋.jpg</t>
+  </si>
+  <si>
+    <t>members/student/王浩然.jpg</t>
+  </si>
+  <si>
+    <t>members/student/罗逸杰.jpg</t>
+  </si>
+  <si>
+    <t>members/student/李梓源.jpg</t>
+  </si>
+  <si>
+    <t>members/student/王辰润.jpg</t>
+  </si>
+  <si>
+    <t>members/student/万恬溪.jpg</t>
+  </si>
+  <si>
+    <t>members/student/靳秉睿.jpg</t>
+  </si>
+  <si>
+    <t>members/student/文雯.jpg</t>
+  </si>
+  <si>
+    <t>members/student/周鼎.jpg</t>
+  </si>
+  <si>
+    <t>members/student/李之涵.jpg</t>
+  </si>
+  <si>
+    <t>members/student/张熙灼.jpg</t>
+  </si>
+  <si>
+    <t>members/student/申振南.jpg</t>
+  </si>
+  <si>
+    <t>members/student/陈文熙.jpg</t>
+  </si>
+  <si>
+    <t>members/student/郑航.jpg</t>
+  </si>
+  <si>
+    <t>members/student/郑棋曦.jpg</t>
+  </si>
+  <si>
+    <t>members/student/陈逸恒.jpg</t>
+  </si>
+  <si>
+    <t>members/student/徐瑞阳.jpg</t>
+  </si>
+  <si>
+    <t>members/student/郭思佳.jpg</t>
+  </si>
+  <si>
+    <t>members/student/王熠笑.jpg</t>
+  </si>
+  <si>
+    <t>members/student/黄天呈.jpg</t>
+  </si>
+  <si>
+    <t>members/student/彭景.jpg</t>
+  </si>
+  <si>
+    <t>members/student/杨子越.jpg</t>
+  </si>
+  <si>
+    <t>members/student/谢睿.jpg</t>
+  </si>
+  <si>
+    <t>members/student/曹义路.jpg</t>
+  </si>
+  <si>
+    <t>members/student/苗语洵.jpg</t>
+  </si>
+  <si>
+    <t>members/student/李贻瑄.jpg</t>
+  </si>
+  <si>
+    <t>members/student/汪子翔.jpg</t>
+  </si>
+  <si>
+    <t>members/student/孙羽恒.jpg</t>
+  </si>
+  <si>
+    <t>members/student/冯草林.jpg</t>
+  </si>
+  <si>
+    <t>members/student/殷国航.jpg</t>
+  </si>
+  <si>
+    <t>members/student/单奕佳.jpg</t>
+  </si>
+  <si>
+    <t>members/student/陶也.jpg</t>
+  </si>
+  <si>
+    <t>members/student/马娆.jpg</t>
+  </si>
+  <si>
+    <t>members/faculty/qym_square.jpg</t>
+  </si>
+  <si>
+    <t>members/student/杨景凯.jpg</t>
   </si>
 </sst>
 </file>
@@ -2256,8 +2499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="L179" sqref="L179"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -2303,7 +2546,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -2323,7 +2566,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -2343,7 +2586,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>586</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -2363,7 +2606,7 @@
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -2383,7 +2626,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -2403,7 +2646,7 @@
         <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>587</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -2423,7 +2666,7 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -2443,7 +2686,7 @@
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
@@ -2463,7 +2706,7 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>588</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
@@ -2483,7 +2726,7 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F11" t="s">
         <v>10</v>
@@ -2503,7 +2746,7 @@
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -2523,7 +2766,7 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>
@@ -2543,7 +2786,7 @@
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
@@ -2563,7 +2806,7 @@
         <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="F15" t="s">
         <v>10</v>
@@ -2583,7 +2826,7 @@
         <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>590</v>
       </c>
       <c r="F16" t="s">
         <v>10</v>
@@ -2603,7 +2846,7 @@
         <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>591</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
@@ -2623,7 +2866,7 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
@@ -2643,7 +2886,7 @@
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
@@ -2663,7 +2906,7 @@
         <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
@@ -2683,7 +2926,7 @@
         <v>15</v>
       </c>
       <c r="E21" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F21" t="s">
         <v>10</v>
@@ -2691,7 +2934,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>606</v>
+        <v>583</v>
       </c>
       <c r="B22" t="s">
         <v>61</v>
@@ -2703,7 +2946,7 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>607</v>
+        <v>592</v>
       </c>
       <c r="F22" t="s">
         <v>10</v>
@@ -2723,7 +2966,7 @@
         <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>585</v>
+        <v>593</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
@@ -2743,7 +2986,7 @@
         <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>582</v>
+        <v>594</v>
       </c>
       <c r="F24" t="s">
         <v>10</v>
@@ -2763,7 +3006,7 @@
         <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>71</v>
+        <v>595</v>
       </c>
       <c r="F25" t="s">
         <v>10</v>
@@ -2783,7 +3026,7 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F26" t="s">
         <v>10</v>
@@ -2803,7 +3046,7 @@
         <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
@@ -2823,7 +3066,7 @@
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F28" t="s">
         <v>10</v>
@@ -2843,7 +3086,7 @@
         <v>19</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F29" t="s">
         <v>10</v>
@@ -2863,7 +3106,7 @@
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F30" t="s">
         <v>10</v>
@@ -2883,7 +3126,7 @@
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
@@ -2903,7 +3146,7 @@
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>583</v>
+        <v>596</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
@@ -2923,7 +3166,7 @@
         <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
@@ -2943,7 +3186,7 @@
         <v>19</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F34" t="s">
         <v>10</v>
@@ -2963,7 +3206,7 @@
         <v>15</v>
       </c>
       <c r="E35" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F35" t="s">
         <v>10</v>
@@ -2983,7 +3226,7 @@
         <v>19</v>
       </c>
       <c r="E36" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F36" t="s">
         <v>10</v>
@@ -3003,7 +3246,7 @@
         <v>19</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F37" t="s">
         <v>10</v>
@@ -3023,7 +3266,7 @@
         <v>8</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F38" t="s">
         <v>10</v>
@@ -3043,7 +3286,7 @@
         <v>49</v>
       </c>
       <c r="E39" t="s">
-        <v>586</v>
+        <v>597</v>
       </c>
       <c r="F39" t="s">
         <v>10</v>
@@ -3063,7 +3306,7 @@
         <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F40" t="s">
         <v>10</v>
@@ -3083,7 +3326,7 @@
         <v>104</v>
       </c>
       <c r="E41" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F41" t="s">
         <v>10</v>
@@ -3103,7 +3346,7 @@
         <v>19</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F42" t="s">
         <v>10</v>
@@ -3123,7 +3366,7 @@
         <v>37</v>
       </c>
       <c r="E43" t="s">
-        <v>109</v>
+        <v>598</v>
       </c>
       <c r="F43" t="s">
         <v>10</v>
@@ -3143,7 +3386,7 @@
         <v>15</v>
       </c>
       <c r="E44" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F44" t="s">
         <v>10</v>
@@ -3163,7 +3406,7 @@
         <v>37</v>
       </c>
       <c r="E45" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F45" t="s">
         <v>10</v>
@@ -3183,7 +3426,7 @@
         <v>19</v>
       </c>
       <c r="E46" t="s">
-        <v>116</v>
+        <v>599</v>
       </c>
       <c r="F46" t="s">
         <v>10</v>
@@ -3203,7 +3446,7 @@
         <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F47" t="s">
         <v>10</v>
@@ -3223,7 +3466,7 @@
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F48" t="s">
         <v>10</v>
@@ -3243,7 +3486,7 @@
         <v>15</v>
       </c>
       <c r="E49" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F49" t="s">
         <v>10</v>
@@ -3263,7 +3506,7 @@
         <v>19</v>
       </c>
       <c r="E50" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F50" t="s">
         <v>10</v>
@@ -3283,7 +3526,7 @@
         <v>19</v>
       </c>
       <c r="E51" t="s">
-        <v>127</v>
+        <v>600</v>
       </c>
       <c r="F51" t="s">
         <v>10</v>
@@ -3303,7 +3546,7 @@
         <v>19</v>
       </c>
       <c r="E52" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F52" t="s">
         <v>10</v>
@@ -3323,7 +3566,7 @@
         <v>19</v>
       </c>
       <c r="E53" t="s">
-        <v>132</v>
+        <v>601</v>
       </c>
       <c r="F53" t="s">
         <v>10</v>
@@ -3343,7 +3586,7 @@
         <v>8</v>
       </c>
       <c r="E54" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F54" t="s">
         <v>10</v>
@@ -3363,7 +3606,7 @@
         <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F55" t="s">
         <v>10</v>
@@ -3383,7 +3626,7 @@
         <v>15</v>
       </c>
       <c r="E56" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F56" t="s">
         <v>10</v>
@@ -3403,7 +3646,7 @@
         <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F57" t="s">
         <v>10</v>
@@ -3423,7 +3666,7 @@
         <v>8</v>
       </c>
       <c r="E58" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F58" t="s">
         <v>10</v>
@@ -3443,7 +3686,7 @@
         <v>19</v>
       </c>
       <c r="E59" t="s">
-        <v>145</v>
+        <v>602</v>
       </c>
       <c r="F59" t="s">
         <v>10</v>
@@ -3463,7 +3706,7 @@
         <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>587</v>
+        <v>603</v>
       </c>
       <c r="F60" t="s">
         <v>10</v>
@@ -3483,7 +3726,7 @@
         <v>15</v>
       </c>
       <c r="E61" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F61" t="s">
         <v>10</v>
@@ -3503,7 +3746,7 @@
         <v>15</v>
       </c>
       <c r="E62" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F62" t="s">
         <v>10</v>
@@ -3523,7 +3766,7 @@
         <v>15</v>
       </c>
       <c r="E63" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F63" t="s">
         <v>154</v>
@@ -3543,7 +3786,7 @@
         <v>8</v>
       </c>
       <c r="E64" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F64" t="s">
         <v>10</v>
@@ -3563,7 +3806,7 @@
         <v>37</v>
       </c>
       <c r="E65" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F65" t="s">
         <v>10</v>
@@ -3583,7 +3826,7 @@
         <v>19</v>
       </c>
       <c r="E66" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F66" t="s">
         <v>10</v>
@@ -3603,7 +3846,7 @@
         <v>15</v>
       </c>
       <c r="E67" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F67" t="s">
         <v>10</v>
@@ -3623,7 +3866,7 @@
         <v>15</v>
       </c>
       <c r="E68" t="s">
-        <v>165</v>
+        <v>604</v>
       </c>
       <c r="F68" t="s">
         <v>10</v>
@@ -3643,7 +3886,7 @@
         <v>15</v>
       </c>
       <c r="E69" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F69" t="s">
         <v>10</v>
@@ -3663,7 +3906,7 @@
         <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F70" t="s">
         <v>10</v>
@@ -3683,7 +3926,7 @@
         <v>8</v>
       </c>
       <c r="E71" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F71" t="s">
         <v>10</v>
@@ -3703,7 +3946,7 @@
         <v>15</v>
       </c>
       <c r="E72" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F72" t="s">
         <v>10</v>
@@ -3723,7 +3966,7 @@
         <v>49</v>
       </c>
       <c r="E73" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F73" t="s">
         <v>10</v>
@@ -3743,7 +3986,7 @@
         <v>49</v>
       </c>
       <c r="E74" t="s">
-        <v>178</v>
+        <v>605</v>
       </c>
       <c r="F74" t="s">
         <v>10</v>
@@ -3763,7 +4006,7 @@
         <v>15</v>
       </c>
       <c r="E75" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F75" t="s">
         <v>10</v>
@@ -3783,7 +4026,7 @@
         <v>15</v>
       </c>
       <c r="E76" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F76" t="s">
         <v>10</v>
@@ -3803,7 +4046,7 @@
         <v>15</v>
       </c>
       <c r="E77" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F77" t="s">
         <v>10</v>
@@ -3823,7 +4066,7 @@
         <v>15</v>
       </c>
       <c r="E78" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F78" t="s">
         <v>10</v>
@@ -3843,7 +4086,7 @@
         <v>68</v>
       </c>
       <c r="E79" t="s">
-        <v>189</v>
+        <v>606</v>
       </c>
       <c r="F79" t="s">
         <v>10</v>
@@ -3863,7 +4106,7 @@
         <v>15</v>
       </c>
       <c r="E80" t="s">
-        <v>192</v>
+        <v>607</v>
       </c>
       <c r="F80" t="s">
         <v>10</v>
@@ -3883,7 +4126,7 @@
         <v>8</v>
       </c>
       <c r="E81" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F81" t="s">
         <v>10</v>
@@ -3903,7 +4146,7 @@
         <v>8</v>
       </c>
       <c r="E82" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F82" t="s">
         <v>10</v>
@@ -3923,7 +4166,7 @@
         <v>8</v>
       </c>
       <c r="E83" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F83" t="s">
         <v>10</v>
@@ -3943,7 +4186,7 @@
         <v>8</v>
       </c>
       <c r="E84" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F84" t="s">
         <v>10</v>
@@ -3963,7 +4206,7 @@
         <v>49</v>
       </c>
       <c r="E85" t="s">
-        <v>203</v>
+        <v>608</v>
       </c>
       <c r="F85" t="s">
         <v>10</v>
@@ -3983,7 +4226,7 @@
         <v>49</v>
       </c>
       <c r="E86" t="s">
-        <v>206</v>
+        <v>609</v>
       </c>
       <c r="F86" t="s">
         <v>154</v>
@@ -4003,7 +4246,7 @@
         <v>19</v>
       </c>
       <c r="E87" t="s">
-        <v>209</v>
+        <v>610</v>
       </c>
       <c r="F87" t="s">
         <v>10</v>
@@ -4023,7 +4266,7 @@
         <v>68</v>
       </c>
       <c r="E88" t="s">
-        <v>212</v>
+        <v>611</v>
       </c>
       <c r="F88" t="s">
         <v>154</v>
@@ -4043,7 +4286,7 @@
         <v>68</v>
       </c>
       <c r="E89" t="s">
-        <v>215</v>
+        <v>612</v>
       </c>
       <c r="F89" t="s">
         <v>154</v>
@@ -4063,7 +4306,7 @@
         <v>15</v>
       </c>
       <c r="E90" t="s">
-        <v>218</v>
+        <v>613</v>
       </c>
       <c r="F90" t="s">
         <v>10</v>
@@ -4083,7 +4326,7 @@
         <v>8</v>
       </c>
       <c r="E91" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F91" t="s">
         <v>10</v>
@@ -4103,7 +4346,7 @@
         <v>15</v>
       </c>
       <c r="E92" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F92" t="s">
         <v>10</v>
@@ -4123,7 +4366,7 @@
         <v>68</v>
       </c>
       <c r="E93" t="s">
-        <v>225</v>
+        <v>614</v>
       </c>
       <c r="F93" t="s">
         <v>154</v>
@@ -4143,7 +4386,7 @@
         <v>15</v>
       </c>
       <c r="E94" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F94" t="s">
         <v>10</v>
@@ -4163,7 +4406,7 @@
         <v>15</v>
       </c>
       <c r="E95" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F95" t="s">
         <v>10</v>
@@ -4183,7 +4426,7 @@
         <v>8</v>
       </c>
       <c r="E96" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F96" t="s">
         <v>10</v>
@@ -4203,7 +4446,7 @@
         <v>8</v>
       </c>
       <c r="E97" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F97" t="s">
         <v>10</v>
@@ -4223,7 +4466,7 @@
         <v>19</v>
       </c>
       <c r="E98" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F98" t="s">
         <v>10</v>
@@ -4243,7 +4486,7 @@
         <v>8</v>
       </c>
       <c r="E99" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
@@ -4263,7 +4506,7 @@
         <v>8</v>
       </c>
       <c r="E100" t="s">
-        <v>240</v>
+        <v>615</v>
       </c>
       <c r="F100" t="s">
         <v>10</v>
@@ -4283,7 +4526,7 @@
         <v>49</v>
       </c>
       <c r="E101" t="s">
-        <v>243</v>
+        <v>616</v>
       </c>
       <c r="F101" t="s">
         <v>154</v>
@@ -4303,7 +4546,7 @@
         <v>49</v>
       </c>
       <c r="E102" t="s">
-        <v>246</v>
+        <v>617</v>
       </c>
       <c r="F102" t="s">
         <v>154</v>
@@ -4323,7 +4566,7 @@
         <v>15</v>
       </c>
       <c r="E103" t="s">
-        <v>249</v>
+        <v>618</v>
       </c>
       <c r="F103" t="s">
         <v>10</v>
@@ -4343,7 +4586,7 @@
         <v>15</v>
       </c>
       <c r="E104" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F104" t="s">
         <v>10</v>
@@ -4363,7 +4606,7 @@
         <v>15</v>
       </c>
       <c r="E105" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F105" t="s">
         <v>10</v>
@@ -4383,7 +4626,7 @@
         <v>15</v>
       </c>
       <c r="E106" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F106" t="s">
         <v>10</v>
@@ -4403,7 +4646,7 @@
         <v>49</v>
       </c>
       <c r="E107" t="s">
-        <v>258</v>
+        <v>619</v>
       </c>
       <c r="F107" t="s">
         <v>154</v>
@@ -4423,7 +4666,7 @@
         <v>104</v>
       </c>
       <c r="E108" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F108" t="s">
         <v>10</v>
@@ -4443,7 +4686,7 @@
         <v>49</v>
       </c>
       <c r="E109" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F109" t="s">
         <v>10</v>
@@ -4463,7 +4706,7 @@
         <v>49</v>
       </c>
       <c r="E110" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F110" t="s">
         <v>10</v>
@@ -4483,7 +4726,7 @@
         <v>68</v>
       </c>
       <c r="E111" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F111" t="s">
         <v>10</v>
@@ -4503,7 +4746,7 @@
         <v>49</v>
       </c>
       <c r="E112" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F112" t="s">
         <v>10</v>
@@ -4523,7 +4766,7 @@
         <v>15</v>
       </c>
       <c r="E113" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F113" t="s">
         <v>10</v>
@@ -4543,7 +4786,7 @@
         <v>15</v>
       </c>
       <c r="E114" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F114" t="s">
         <v>10</v>
@@ -4563,7 +4806,7 @@
         <v>15</v>
       </c>
       <c r="E115" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F115" t="s">
         <v>10</v>
@@ -4583,7 +4826,7 @@
         <v>15</v>
       </c>
       <c r="E116" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F116" t="s">
         <v>10</v>
@@ -4603,7 +4846,7 @@
         <v>15</v>
       </c>
       <c r="E117" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F117" t="s">
         <v>10</v>
@@ -4623,7 +4866,7 @@
         <v>15</v>
       </c>
       <c r="E118" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F118" t="s">
         <v>10</v>
@@ -4643,7 +4886,7 @@
         <v>104</v>
       </c>
       <c r="E119" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F119" t="s">
         <v>10</v>
@@ -4663,7 +4906,7 @@
         <v>15</v>
       </c>
       <c r="E120" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F120" t="s">
         <v>10</v>
@@ -4683,7 +4926,7 @@
         <v>15</v>
       </c>
       <c r="E121" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F121" t="s">
         <v>10</v>
@@ -4703,7 +4946,7 @@
         <v>15</v>
       </c>
       <c r="E122" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F122" t="s">
         <v>10</v>
@@ -4723,7 +4966,7 @@
         <v>49</v>
       </c>
       <c r="E123" t="s">
-        <v>291</v>
+        <v>620</v>
       </c>
       <c r="F123" t="s">
         <v>154</v>
@@ -4743,7 +4986,7 @@
         <v>49</v>
       </c>
       <c r="E124" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F124" t="s">
         <v>10</v>
@@ -4763,7 +5006,7 @@
         <v>68</v>
       </c>
       <c r="E125" t="s">
-        <v>296</v>
+        <v>621</v>
       </c>
       <c r="F125" t="s">
         <v>154</v>
@@ -4783,7 +5026,7 @@
         <v>15</v>
       </c>
       <c r="E126" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F126" t="s">
         <v>10</v>
@@ -4803,7 +5046,7 @@
         <v>49</v>
       </c>
       <c r="E127" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F127" t="s">
         <v>10</v>
@@ -4823,7 +5066,7 @@
         <v>15</v>
       </c>
       <c r="E128" t="s">
-        <v>303</v>
+        <v>622</v>
       </c>
       <c r="F128" t="s">
         <v>10</v>
@@ -4843,7 +5086,7 @@
         <v>15</v>
       </c>
       <c r="E129" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F129" t="s">
         <v>10</v>
@@ -4863,7 +5106,7 @@
         <v>15</v>
       </c>
       <c r="E130" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F130" t="s">
         <v>10</v>
@@ -4883,7 +5126,7 @@
         <v>19</v>
       </c>
       <c r="E131" t="s">
-        <v>310</v>
+        <v>623</v>
       </c>
       <c r="F131" t="s">
         <v>10</v>
@@ -4903,7 +5146,7 @@
         <v>15</v>
       </c>
       <c r="E132" t="s">
-        <v>313</v>
+        <v>624</v>
       </c>
       <c r="F132" t="s">
         <v>154</v>
@@ -4923,7 +5166,7 @@
         <v>49</v>
       </c>
       <c r="E133" t="s">
-        <v>593</v>
+        <v>625</v>
       </c>
       <c r="F133" t="s">
         <v>154</v>
@@ -4943,7 +5186,7 @@
         <v>8</v>
       </c>
       <c r="E134" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F134" t="s">
         <v>154</v>
@@ -4963,7 +5206,7 @@
         <v>8</v>
       </c>
       <c r="E135" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F135" t="s">
         <v>154</v>
@@ -4983,7 +5226,7 @@
         <v>15</v>
       </c>
       <c r="E136" t="s">
-        <v>323</v>
+        <v>626</v>
       </c>
       <c r="F136" t="s">
         <v>154</v>
@@ -5003,7 +5246,7 @@
         <v>19</v>
       </c>
       <c r="E137" t="s">
-        <v>594</v>
+        <v>627</v>
       </c>
       <c r="F137" t="s">
         <v>154</v>
@@ -5023,7 +5266,7 @@
         <v>49</v>
       </c>
       <c r="E138" t="s">
-        <v>595</v>
+        <v>628</v>
       </c>
       <c r="F138" t="s">
         <v>154</v>
@@ -5043,7 +5286,7 @@
         <v>37</v>
       </c>
       <c r="E139" t="s">
-        <v>332</v>
+        <v>629</v>
       </c>
       <c r="F139" t="s">
         <v>154</v>
@@ -5063,7 +5306,7 @@
         <v>49</v>
       </c>
       <c r="E140" t="s">
-        <v>335</v>
+        <v>630</v>
       </c>
       <c r="F140" t="s">
         <v>154</v>
@@ -5083,7 +5326,7 @@
         <v>15</v>
       </c>
       <c r="E141" t="s">
-        <v>338</v>
+        <v>631</v>
       </c>
       <c r="F141" t="s">
         <v>154</v>
@@ -5103,7 +5346,7 @@
         <v>15</v>
       </c>
       <c r="E142" t="s">
-        <v>596</v>
+        <v>632</v>
       </c>
       <c r="F142" t="s">
         <v>10</v>
@@ -5123,7 +5366,7 @@
         <v>49</v>
       </c>
       <c r="E143" t="s">
-        <v>592</v>
+        <v>633</v>
       </c>
       <c r="F143" t="s">
         <v>154</v>
@@ -5143,7 +5386,7 @@
         <v>49</v>
       </c>
       <c r="E144" t="s">
-        <v>346</v>
+        <v>634</v>
       </c>
       <c r="F144" t="s">
         <v>154</v>
@@ -5163,7 +5406,7 @@
         <v>15</v>
       </c>
       <c r="E145" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F145" t="s">
         <v>154</v>
@@ -5183,7 +5426,7 @@
         <v>68</v>
       </c>
       <c r="E146" t="s">
-        <v>351</v>
+        <v>635</v>
       </c>
       <c r="F146" t="s">
         <v>154</v>
@@ -5203,7 +5446,7 @@
         <v>15</v>
       </c>
       <c r="E147" t="s">
-        <v>597</v>
+        <v>636</v>
       </c>
       <c r="F147" t="s">
         <v>10</v>
@@ -5223,7 +5466,7 @@
         <v>15</v>
       </c>
       <c r="E148" t="s">
-        <v>357</v>
+        <v>637</v>
       </c>
       <c r="F148" t="s">
         <v>10</v>
@@ -5243,7 +5486,7 @@
         <v>15</v>
       </c>
       <c r="E149" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F149" t="s">
         <v>154</v>
@@ -5263,7 +5506,7 @@
         <v>8</v>
       </c>
       <c r="E150" t="s">
-        <v>362</v>
+        <v>638</v>
       </c>
       <c r="F150" t="s">
         <v>154</v>
@@ -5283,7 +5526,7 @@
         <v>49</v>
       </c>
       <c r="E151" t="s">
-        <v>365</v>
+        <v>639</v>
       </c>
       <c r="F151" t="s">
         <v>154</v>
@@ -5303,7 +5546,7 @@
         <v>15</v>
       </c>
       <c r="E152" t="s">
-        <v>368</v>
+        <v>640</v>
       </c>
       <c r="F152" t="s">
         <v>154</v>
@@ -5323,7 +5566,7 @@
         <v>49</v>
       </c>
       <c r="E153" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F153" t="s">
         <v>154</v>
@@ -5343,7 +5586,7 @@
         <v>15</v>
       </c>
       <c r="E154" t="s">
-        <v>373</v>
+        <v>641</v>
       </c>
       <c r="F154" t="s">
         <v>154</v>
@@ -5363,7 +5606,7 @@
         <v>15</v>
       </c>
       <c r="E155" t="s">
-        <v>376</v>
+        <v>642</v>
       </c>
       <c r="F155" t="s">
         <v>154</v>
@@ -5383,7 +5626,7 @@
         <v>15</v>
       </c>
       <c r="E156" t="s">
-        <v>379</v>
+        <v>643</v>
       </c>
       <c r="F156" t="s">
         <v>154</v>
@@ -5403,7 +5646,7 @@
         <v>49</v>
       </c>
       <c r="E157" t="s">
-        <v>382</v>
+        <v>644</v>
       </c>
       <c r="F157" t="s">
         <v>154</v>
@@ -5423,7 +5666,7 @@
         <v>15</v>
       </c>
       <c r="E158" t="s">
-        <v>385</v>
+        <v>645</v>
       </c>
       <c r="F158" t="s">
         <v>10</v>
@@ -5443,7 +5686,7 @@
         <v>49</v>
       </c>
       <c r="E159" t="s">
-        <v>598</v>
+        <v>646</v>
       </c>
       <c r="F159" t="s">
         <v>154</v>
@@ -5463,7 +5706,7 @@
         <v>15</v>
       </c>
       <c r="E160" t="s">
-        <v>391</v>
+        <v>647</v>
       </c>
       <c r="F160" t="s">
         <v>154</v>
@@ -5483,7 +5726,7 @@
         <v>15</v>
       </c>
       <c r="E161" t="s">
-        <v>599</v>
+        <v>648</v>
       </c>
       <c r="F161" t="s">
         <v>10</v>
@@ -5503,7 +5746,7 @@
         <v>15</v>
       </c>
       <c r="E162" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F162" t="s">
         <v>154</v>
@@ -5523,7 +5766,7 @@
         <v>15</v>
       </c>
       <c r="E163" t="s">
-        <v>399</v>
+        <v>649</v>
       </c>
       <c r="F163" t="s">
         <v>10</v>
@@ -5543,7 +5786,7 @@
         <v>49</v>
       </c>
       <c r="E164" t="s">
-        <v>402</v>
+        <v>650</v>
       </c>
       <c r="F164" t="s">
         <v>154</v>
@@ -5563,7 +5806,7 @@
         <v>15</v>
       </c>
       <c r="E165" t="s">
-        <v>405</v>
+        <v>651</v>
       </c>
       <c r="F165" t="s">
         <v>10</v>
@@ -5583,7 +5826,7 @@
         <v>15</v>
       </c>
       <c r="E166" t="s">
-        <v>408</v>
+        <v>652</v>
       </c>
       <c r="F166" t="s">
         <v>154</v>
@@ -5603,7 +5846,7 @@
         <v>15</v>
       </c>
       <c r="E167" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F167" t="s">
         <v>154</v>
@@ -5623,7 +5866,7 @@
         <v>15</v>
       </c>
       <c r="E168" t="s">
-        <v>413</v>
+        <v>653</v>
       </c>
       <c r="F168" t="s">
         <v>154</v>
@@ -5643,7 +5886,7 @@
         <v>15</v>
       </c>
       <c r="E169" t="s">
-        <v>416</v>
+        <v>654</v>
       </c>
       <c r="F169" t="s">
         <v>10</v>
@@ -5663,7 +5906,7 @@
         <v>37</v>
       </c>
       <c r="E170" t="s">
-        <v>419</v>
+        <v>655</v>
       </c>
       <c r="F170" t="s">
         <v>154</v>
@@ -5683,7 +5926,7 @@
         <v>15</v>
       </c>
       <c r="E171" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F171" t="s">
         <v>154</v>
@@ -5703,7 +5946,7 @@
         <v>15</v>
       </c>
       <c r="E172" t="s">
-        <v>424</v>
+        <v>656</v>
       </c>
       <c r="F172" t="s">
         <v>10</v>
@@ -5723,7 +5966,7 @@
         <v>8</v>
       </c>
       <c r="E173" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F173" t="s">
         <v>10</v>
@@ -5743,7 +5986,7 @@
         <v>8</v>
       </c>
       <c r="E174" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F174" t="s">
         <v>10</v>
@@ -5763,7 +6006,7 @@
         <v>15</v>
       </c>
       <c r="E175" t="s">
-        <v>431</v>
+        <v>657</v>
       </c>
       <c r="F175" t="s">
         <v>10</v>
@@ -5783,7 +6026,7 @@
         <v>49</v>
       </c>
       <c r="E176" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F176" t="s">
         <v>154</v>
@@ -5803,7 +6046,7 @@
         <v>37</v>
       </c>
       <c r="E177" t="s">
-        <v>436</v>
+        <v>658</v>
       </c>
       <c r="F177" t="s">
         <v>10</v>
@@ -5823,7 +6066,7 @@
         <v>104</v>
       </c>
       <c r="E178" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F178" t="s">
         <v>154</v>
@@ -5843,7 +6086,7 @@
         <v>19</v>
       </c>
       <c r="E179" t="s">
-        <v>441</v>
+        <v>659</v>
       </c>
       <c r="F179" t="s">
         <v>154</v>
@@ -5863,7 +6106,7 @@
         <v>15</v>
       </c>
       <c r="E180" t="s">
-        <v>444</v>
+        <v>660</v>
       </c>
       <c r="F180" t="s">
         <v>154</v>
@@ -5883,7 +6126,7 @@
         <v>15</v>
       </c>
       <c r="E181" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F181" t="s">
         <v>154</v>
@@ -5903,7 +6146,7 @@
         <v>49</v>
       </c>
       <c r="E182" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F182" t="s">
         <v>154</v>
@@ -5923,7 +6166,7 @@
         <v>8</v>
       </c>
       <c r="E183" t="s">
-        <v>449</v>
+        <v>661</v>
       </c>
       <c r="F183" t="s">
         <v>10</v>
@@ -5943,7 +6186,7 @@
         <v>8</v>
       </c>
       <c r="E184" t="s">
-        <v>452</v>
+        <v>662</v>
       </c>
       <c r="F184" t="s">
         <v>154</v>
@@ -5963,7 +6206,7 @@
         <v>8</v>
       </c>
       <c r="E185" t="s">
-        <v>455</v>
+        <v>663</v>
       </c>
       <c r="F185" t="s">
         <v>154</v>
@@ -5983,7 +6226,7 @@
         <v>8</v>
       </c>
       <c r="E186" t="s">
-        <v>600</v>
+        <v>664</v>
       </c>
       <c r="F186" t="s">
         <v>154</v>
@@ -6003,7 +6246,7 @@
         <v>8</v>
       </c>
       <c r="E187" t="s">
-        <v>461</v>
+        <v>665</v>
       </c>
       <c r="F187" t="s">
         <v>154</v>
@@ -6023,7 +6266,7 @@
         <v>8</v>
       </c>
       <c r="E188" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F188" t="s">
         <v>154</v>
@@ -6043,7 +6286,7 @@
         <v>19</v>
       </c>
       <c r="E189" t="s">
-        <v>466</v>
+        <v>666</v>
       </c>
       <c r="F189" t="s">
         <v>154</v>
@@ -6063,7 +6306,7 @@
         <v>15</v>
       </c>
       <c r="E190" t="s">
-        <v>469</v>
+        <v>667</v>
       </c>
       <c r="F190" t="s">
         <v>10</v>
@@ -6083,7 +6326,7 @@
         <v>15</v>
       </c>
       <c r="E191" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F191" t="s">
         <v>10</v>
@@ -6103,7 +6346,7 @@
         <v>8</v>
       </c>
       <c r="E192" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F192" t="s">
         <v>154</v>
@@ -6120,7 +6363,7 @@
         <v>15</v>
       </c>
       <c r="E193" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F193" t="s">
         <v>154</v>
@@ -6137,7 +6380,7 @@
         <v>15</v>
       </c>
       <c r="E194" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F194" t="s">
         <v>154</v>
@@ -6154,7 +6397,7 @@
         <v>15</v>
       </c>
       <c r="E195" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F195" t="s">
         <v>154</v>
@@ -6171,7 +6414,7 @@
         <v>8</v>
       </c>
       <c r="E196" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F196" t="s">
         <v>154</v>
@@ -6179,7 +6422,7 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>482</v>
+        <v>584</v>
       </c>
       <c r="B197" t="s">
         <v>483</v>
@@ -6188,7 +6431,7 @@
         <v>8</v>
       </c>
       <c r="E197" t="s">
-        <v>601</v>
+        <v>668</v>
       </c>
       <c r="F197" t="s">
         <v>154</v>
@@ -6205,7 +6448,7 @@
         <v>8</v>
       </c>
       <c r="E198" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F198" t="s">
         <v>154</v>
@@ -6222,7 +6465,7 @@
         <v>8</v>
       </c>
       <c r="E199" t="s">
-        <v>602</v>
+        <v>669</v>
       </c>
       <c r="F199" t="s">
         <v>154</v>
@@ -6239,7 +6482,7 @@
         <v>8</v>
       </c>
       <c r="E200" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F200" t="s">
         <v>154</v>
@@ -6256,7 +6499,7 @@
         <v>8</v>
       </c>
       <c r="E201" t="s">
-        <v>494</v>
+        <v>670</v>
       </c>
       <c r="F201" t="s">
         <v>154</v>
@@ -6273,7 +6516,7 @@
         <v>8</v>
       </c>
       <c r="E202" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F202" t="s">
         <v>154</v>
@@ -6290,7 +6533,7 @@
         <v>19</v>
       </c>
       <c r="E203" t="s">
-        <v>499</v>
+        <v>671</v>
       </c>
       <c r="F203" t="s">
         <v>154</v>
@@ -6307,7 +6550,7 @@
         <v>8</v>
       </c>
       <c r="E204" t="s">
-        <v>502</v>
+        <v>672</v>
       </c>
       <c r="F204" t="s">
         <v>154</v>
@@ -6324,7 +6567,7 @@
         <v>8</v>
       </c>
       <c r="E205" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F205" t="s">
         <v>154</v>
@@ -6341,7 +6584,7 @@
         <v>8</v>
       </c>
       <c r="E206" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F206" t="s">
         <v>154</v>
@@ -6358,7 +6601,7 @@
         <v>8</v>
       </c>
       <c r="E207" t="s">
-        <v>509</v>
+        <v>673</v>
       </c>
       <c r="F207" t="s">
         <v>154</v>
@@ -6375,10 +6618,10 @@
         <v>8</v>
       </c>
       <c r="E208" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F208" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
@@ -6392,7 +6635,7 @@
         <v>8</v>
       </c>
       <c r="E209" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F209" t="s">
         <v>154</v>
@@ -6409,7 +6652,7 @@
         <v>8</v>
       </c>
       <c r="E210" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F210" t="s">
         <v>154</v>
@@ -6426,7 +6669,7 @@
         <v>8</v>
       </c>
       <c r="E211" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F211" t="s">
         <v>154</v>
@@ -6443,7 +6686,7 @@
         <v>8</v>
       </c>
       <c r="E212" t="s">
-        <v>520</v>
+        <v>674</v>
       </c>
       <c r="F212" t="s">
         <v>154</v>
@@ -6460,7 +6703,7 @@
         <v>8</v>
       </c>
       <c r="E213" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F213" t="s">
         <v>154</v>
@@ -6477,7 +6720,7 @@
         <v>8</v>
       </c>
       <c r="E214" t="s">
-        <v>603</v>
+        <v>675</v>
       </c>
       <c r="F214" t="s">
         <v>154</v>
@@ -6494,10 +6737,10 @@
         <v>8</v>
       </c>
       <c r="E215" t="s">
-        <v>528</v>
+        <v>676</v>
       </c>
       <c r="F215" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.3">
@@ -6511,7 +6754,7 @@
         <v>8</v>
       </c>
       <c r="E216" t="s">
-        <v>531</v>
+        <v>677</v>
       </c>
       <c r="F216" t="s">
         <v>154</v>
@@ -6528,7 +6771,7 @@
         <v>8</v>
       </c>
       <c r="E217" t="s">
-        <v>534</v>
+        <v>678</v>
       </c>
       <c r="F217" t="s">
         <v>154</v>
@@ -6545,7 +6788,7 @@
         <v>8</v>
       </c>
       <c r="E218" t="s">
-        <v>537</v>
+        <v>679</v>
       </c>
       <c r="F218" t="s">
         <v>154</v>
@@ -6562,7 +6805,7 @@
         <v>8</v>
       </c>
       <c r="E219" t="s">
-        <v>540</v>
+        <v>680</v>
       </c>
       <c r="F219" t="s">
         <v>154</v>
@@ -6579,7 +6822,7 @@
         <v>8</v>
       </c>
       <c r="E220" t="s">
-        <v>543</v>
+        <v>681</v>
       </c>
       <c r="F220" t="s">
         <v>154</v>
@@ -6596,7 +6839,7 @@
         <v>8</v>
       </c>
       <c r="E221" t="s">
-        <v>546</v>
+        <v>682</v>
       </c>
       <c r="F221" t="s">
         <v>154</v>
@@ -6613,7 +6856,7 @@
         <v>8</v>
       </c>
       <c r="E222" t="s">
-        <v>549</v>
+        <v>683</v>
       </c>
       <c r="F222" t="s">
         <v>154</v>
@@ -6630,10 +6873,10 @@
         <v>27</v>
       </c>
       <c r="D223" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E223" t="s">
-        <v>574</v>
+        <v>585</v>
       </c>
       <c r="F223" t="s">
         <v>10</v>
@@ -6650,7 +6893,7 @@
         <v>8</v>
       </c>
       <c r="E224" t="s">
-        <v>553</v>
+        <v>684</v>
       </c>
       <c r="F224" t="s">
         <v>154</v>
@@ -6667,7 +6910,7 @@
         <v>8</v>
       </c>
       <c r="E225" t="s">
-        <v>556</v>
+        <v>685</v>
       </c>
       <c r="F225" t="s">
         <v>154</v>
@@ -6684,7 +6927,7 @@
         <v>8</v>
       </c>
       <c r="E226" t="s">
-        <v>559</v>
+        <v>686</v>
       </c>
       <c r="F226" t="s">
         <v>154</v>
@@ -6692,7 +6935,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>604</v>
+        <v>582</v>
       </c>
       <c r="B227" t="s">
         <v>156</v>
@@ -6704,7 +6947,7 @@
         <v>8</v>
       </c>
       <c r="E227" t="s">
-        <v>605</v>
+        <v>687</v>
       </c>
       <c r="F227" t="s">
         <v>10</v>
@@ -6721,7 +6964,7 @@
         <v>8</v>
       </c>
       <c r="E228" t="s">
-        <v>563</v>
+        <v>688</v>
       </c>
       <c r="F228" t="s">
         <v>154</v>
@@ -6738,7 +6981,7 @@
         <v>8</v>
       </c>
       <c r="E229" t="s">
-        <v>566</v>
+        <v>689</v>
       </c>
       <c r="F229" t="s">
         <v>154</v>
@@ -6755,7 +6998,7 @@
         <v>8</v>
       </c>
       <c r="E230" t="s">
-        <v>9</v>
+        <v>585</v>
       </c>
       <c r="F230" t="s">
         <v>154</v>
@@ -6775,7 +7018,7 @@
         <v>15</v>
       </c>
       <c r="E231" t="s">
-        <v>575</v>
+        <v>690</v>
       </c>
       <c r="F231" t="s">
         <v>10</v>
@@ -6783,39 +7026,39 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B232" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C232">
         <v>11</v>
       </c>
       <c r="D232" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E232" t="s">
-        <v>581</v>
+        <v>691</v>
       </c>
       <c r="F232" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="B233" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
       <c r="D233" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
       <c r="E233" t="s">
-        <v>591</v>
+        <v>692</v>
       </c>
       <c r="F233" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@bc4ffbc37fc6d8a995cde60637f755d1c12a9fb2 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9EE188-42FF-4DA8-B921-AAE53CA34AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DF57E0-57C8-48E3-8443-549A5400F868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="18000" windowHeight="10432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1663,157 +1663,158 @@
     <t>/assets/img/members/student/张耀匀.jpg</t>
   </si>
   <si>
+    <t>/assets/img/members/student/吕铭浩.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/宋秀杰.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/张晗翀.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/韩杨.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/韩森宇.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/黎井漂.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/孙良泰.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/杨亦凡.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/何朝帆.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/杨飞.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/李星源.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/曾泓川.JPG</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/牛志康.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/沈飞宇.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/林少雄.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/任立椋.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/王浩然.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/罗逸杰.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/李梓源.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/王辰润.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/万恬溪.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/靳秉睿.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/文雯.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/周鼎.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/李之涵.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/张熙灼.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/申振南.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/陈文熙.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/郑航.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/郑棋曦.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/陈逸恒.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/徐瑞阳.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/郭思佳.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/王熠笑.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/黄天呈.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/彭景.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/杨子越.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/谢睿.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/曹义路.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/苗语洵.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/李贻瑄.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/汪子翔.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/孙羽恒.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/冯草林.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/殷国航.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/单奕佳.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/陶也.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/马娆.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/faculty/qym_square.jpg</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/杨景凯.jpg</t>
+  </si>
+  <si>
     <t>/assets/img/members/student/肖云冲.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/吕铭浩.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/宋秀杰.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/张晗翀.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/韩杨.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/韩森宇.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/黎井漂.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/孙良泰.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/杨亦凡.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/何朝帆.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/杨飞.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李星源.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/曾泓川.JPG</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/牛志康.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/沈飞宇.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/林少雄.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/任立椋.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/王浩然.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/罗逸杰.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李梓源.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/王辰润.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/万恬溪.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/靳秉睿.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/文雯.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/周鼎.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李之涵.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/张熙灼.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/申振南.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/陈文熙.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/郑航.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/郑棋曦.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/陈逸恒.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/徐瑞阳.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/郭思佳.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/王熠笑.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/黄天呈.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/彭景.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/杨子越.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/谢睿.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/曹义路.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/苗语洵.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李贻瑄.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/汪子翔.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/孙羽恒.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/冯草林.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/殷国航.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/单奕佳.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/陶也.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/马娆.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/faculty/qym_square.jpg</t>
-  </si>
-  <si>
-    <t>/assets/img/members/student/杨景凯.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2186,8 +2187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="E245" sqref="E245"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="E155" sqref="E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -5293,7 +5294,7 @@
         <v>14</v>
       </c>
       <c r="E155" t="s">
-        <v>539</v>
+        <v>589</v>
       </c>
       <c r="F155" t="s">
         <v>139</v>
@@ -5313,7 +5314,7 @@
         <v>14</v>
       </c>
       <c r="E156" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F156" t="s">
         <v>139</v>
@@ -5333,7 +5334,7 @@
         <v>44</v>
       </c>
       <c r="E157" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F157" t="s">
         <v>139</v>
@@ -5353,7 +5354,7 @@
         <v>14</v>
       </c>
       <c r="E158" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F158" t="s">
         <v>9</v>
@@ -5373,7 +5374,7 @@
         <v>44</v>
       </c>
       <c r="E159" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F159" t="s">
         <v>139</v>
@@ -5393,7 +5394,7 @@
         <v>14</v>
       </c>
       <c r="E160" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F160" t="s">
         <v>139</v>
@@ -5413,7 +5414,7 @@
         <v>14</v>
       </c>
       <c r="E161" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F161" t="s">
         <v>9</v>
@@ -5453,7 +5454,7 @@
         <v>14</v>
       </c>
       <c r="E163" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F163" t="s">
         <v>9</v>
@@ -5473,7 +5474,7 @@
         <v>44</v>
       </c>
       <c r="E164" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F164" t="s">
         <v>139</v>
@@ -5493,7 +5494,7 @@
         <v>14</v>
       </c>
       <c r="E165" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F165" t="s">
         <v>9</v>
@@ -5513,7 +5514,7 @@
         <v>14</v>
       </c>
       <c r="E166" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F166" t="s">
         <v>139</v>
@@ -5553,7 +5554,7 @@
         <v>14</v>
       </c>
       <c r="E168" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F168" t="s">
         <v>139</v>
@@ -5573,7 +5574,7 @@
         <v>14</v>
       </c>
       <c r="E169" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F169" t="s">
         <v>9</v>
@@ -5593,7 +5594,7 @@
         <v>33</v>
       </c>
       <c r="E170" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F170" t="s">
         <v>139</v>
@@ -5633,7 +5634,7 @@
         <v>14</v>
       </c>
       <c r="E172" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F172" t="s">
         <v>9</v>
@@ -5693,7 +5694,7 @@
         <v>14</v>
       </c>
       <c r="E175" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F175" t="s">
         <v>9</v>
@@ -5733,7 +5734,7 @@
         <v>33</v>
       </c>
       <c r="E177" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F177" t="s">
         <v>9</v>
@@ -5773,7 +5774,7 @@
         <v>17</v>
       </c>
       <c r="E179" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F179" t="s">
         <v>139</v>
@@ -5793,7 +5794,7 @@
         <v>14</v>
       </c>
       <c r="E180" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F180" t="s">
         <v>139</v>
@@ -5853,7 +5854,7 @@
         <v>8</v>
       </c>
       <c r="E183" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F183" t="s">
         <v>9</v>
@@ -5873,7 +5874,7 @@
         <v>8</v>
       </c>
       <c r="E184" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F184" t="s">
         <v>139</v>
@@ -5893,7 +5894,7 @@
         <v>8</v>
       </c>
       <c r="E185" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F185" t="s">
         <v>139</v>
@@ -5913,7 +5914,7 @@
         <v>8</v>
       </c>
       <c r="E186" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F186" t="s">
         <v>139</v>
@@ -5933,7 +5934,7 @@
         <v>8</v>
       </c>
       <c r="E187" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F187" t="s">
         <v>139</v>
@@ -5973,7 +5974,7 @@
         <v>17</v>
       </c>
       <c r="E189" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F189" t="s">
         <v>139</v>
@@ -5993,7 +5994,7 @@
         <v>14</v>
       </c>
       <c r="E190" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F190" t="s">
         <v>9</v>
@@ -6118,7 +6119,7 @@
         <v>8</v>
       </c>
       <c r="E197" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F197" t="s">
         <v>139</v>
@@ -6152,7 +6153,7 @@
         <v>8</v>
       </c>
       <c r="E199" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F199" t="s">
         <v>139</v>
@@ -6186,7 +6187,7 @@
         <v>8</v>
       </c>
       <c r="E201" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F201" t="s">
         <v>139</v>
@@ -6220,7 +6221,7 @@
         <v>17</v>
       </c>
       <c r="E203" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F203" t="s">
         <v>139</v>
@@ -6237,7 +6238,7 @@
         <v>8</v>
       </c>
       <c r="E204" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F204" t="s">
         <v>139</v>
@@ -6288,7 +6289,7 @@
         <v>8</v>
       </c>
       <c r="E207" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F207" t="s">
         <v>139</v>
@@ -6373,7 +6374,7 @@
         <v>8</v>
       </c>
       <c r="E212" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F212" t="s">
         <v>139</v>
@@ -6407,7 +6408,7 @@
         <v>8</v>
       </c>
       <c r="E214" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F214" t="s">
         <v>139</v>
@@ -6424,7 +6425,7 @@
         <v>8</v>
       </c>
       <c r="E215" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F215" t="s">
         <v>475</v>
@@ -6441,7 +6442,7 @@
         <v>8</v>
       </c>
       <c r="E216" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F216" t="s">
         <v>139</v>
@@ -6458,7 +6459,7 @@
         <v>8</v>
       </c>
       <c r="E217" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F217" t="s">
         <v>139</v>
@@ -6475,7 +6476,7 @@
         <v>8</v>
       </c>
       <c r="E218" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F218" t="s">
         <v>139</v>
@@ -6492,7 +6493,7 @@
         <v>8</v>
       </c>
       <c r="E219" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F219" t="s">
         <v>139</v>
@@ -6509,7 +6510,7 @@
         <v>8</v>
       </c>
       <c r="E220" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F220" t="s">
         <v>139</v>
@@ -6526,7 +6527,7 @@
         <v>8</v>
       </c>
       <c r="E221" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F221" t="s">
         <v>139</v>
@@ -6543,7 +6544,7 @@
         <v>8</v>
       </c>
       <c r="E222" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F222" t="s">
         <v>139</v>
@@ -6580,7 +6581,7 @@
         <v>8</v>
       </c>
       <c r="E224" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F224" t="s">
         <v>139</v>
@@ -6597,7 +6598,7 @@
         <v>8</v>
       </c>
       <c r="E225" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F225" t="s">
         <v>139</v>
@@ -6614,7 +6615,7 @@
         <v>8</v>
       </c>
       <c r="E226" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F226" t="s">
         <v>139</v>
@@ -6634,7 +6635,7 @@
         <v>8</v>
       </c>
       <c r="E227" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F227" t="s">
         <v>9</v>
@@ -6651,7 +6652,7 @@
         <v>8</v>
       </c>
       <c r="E228" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F228" t="s">
         <v>139</v>
@@ -6668,7 +6669,7 @@
         <v>8</v>
       </c>
       <c r="E229" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F229" t="s">
         <v>139</v>
@@ -6705,7 +6706,7 @@
         <v>14</v>
       </c>
       <c r="E231" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F231" t="s">
         <v>9</v>
@@ -6725,7 +6726,7 @@
         <v>474</v>
       </c>
       <c r="E232" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F232" t="s">
         <v>475</v>
@@ -6742,7 +6743,7 @@
         <v>478</v>
       </c>
       <c r="E233" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F233" t="s">
         <v>475</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@fb54664199e110dfcea445a04f4e44e2ed9f8dd9 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DF57E0-57C8-48E3-8443-549A5400F868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F46C65-3475-4267-9250-8F8A2948CE71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1103" yWindow="1103" windowWidth="18000" windowHeight="10432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="591">
   <si>
     <t>name</t>
   </si>
@@ -1814,6 +1814,10 @@
   </si>
   <si>
     <t>/assets/img/members/student/肖云冲.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UP</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2187,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E155" sqref="E155"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="D178" sqref="D178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -6031,7 +6035,7 @@
         <v>200</v>
       </c>
       <c r="D192" t="s">
-        <v>8</v>
+        <v>590</v>
       </c>
       <c r="E192" t="s">
         <v>482</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@c72625c88a000fddd6be8df167be24d0c5876fa1 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8F4167-7244-470A-A17B-CD8E25AB84EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B38F59-9772-4952-8D0F-298F84ABB668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11918" yWindow="0" windowWidth="12165" windowHeight="14362" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1166" uniqueCount="593">
   <si>
     <t>name</t>
   </si>
@@ -1821,6 +1821,14 @@
   </si>
   <si>
     <t>UP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/刘丁烨.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MP</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1840,6 +1848,7 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2194,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B199" sqref="B199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -5901,7 +5910,7 @@
         <v>14</v>
       </c>
       <c r="E185" t="s">
-        <v>482</v>
+        <v>591</v>
       </c>
       <c r="F185" t="s">
         <v>139</v>
@@ -6203,7 +6212,7 @@
         <v>399</v>
       </c>
       <c r="D201" t="s">
-        <v>14</v>
+        <v>592</v>
       </c>
       <c r="E201" t="s">
         <v>482</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@7377a0098f7d4a5b62fbbf22aff5259d33884219 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB7A7B2-E102-45AA-A8EF-B8004E546A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1FC737-B4A2-467A-BE80-BB0DBEA2F4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21710" yWindow="-110" windowWidth="21820" windowHeight="38620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1201" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="641">
   <si>
     <t>name</t>
   </si>
@@ -1009,16 +1009,10 @@
     <t>Sen Liu</t>
   </si>
   <si>
-    <t>/assets/img/members/student/刘森.jpg</t>
-  </si>
-  <si>
     <t>李广鹏</t>
   </si>
   <si>
     <t>Guangpeng Li</t>
-  </si>
-  <si>
-    <t>杨宝琛</t>
   </si>
   <si>
     <t>Baochen Yang</t>
@@ -1906,6 +1900,70 @@
   </si>
   <si>
     <t>/assets/img/members/student/李波含.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/陈博2.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>马英梓</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yingzi Ma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/马英梓.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>杨宝琛</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/刘森.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/杨宝琛.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/刘韫聪.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/李广鹏.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/陈琦.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/龚勋.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/张王优.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/李晨达.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/王巍.jpg</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2277,13 +2335,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F240"/>
+  <dimension ref="A1:F241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="N194" sqref="N194"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="95.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3799,7 +3860,7 @@
         <v>52</v>
       </c>
       <c r="E76" t="s">
-        <v>13</v>
+        <v>638</v>
       </c>
       <c r="F76" t="s">
         <v>10</v>
@@ -3859,7 +3920,7 @@
         <v>16</v>
       </c>
       <c r="E79" t="s">
-        <v>13</v>
+        <v>639</v>
       </c>
       <c r="F79" t="s">
         <v>10</v>
@@ -4122,7 +4183,7 @@
         <v>232</v>
       </c>
       <c r="F92" t="s">
-        <v>226</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -4259,7 +4320,7 @@
         <v>16</v>
       </c>
       <c r="E99" t="s">
-        <v>13</v>
+        <v>640</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
@@ -4442,7 +4503,7 @@
         <v>272</v>
       </c>
       <c r="F108" t="s">
-        <v>226</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -4839,7 +4900,7 @@
         <v>52</v>
       </c>
       <c r="E128" t="s">
-        <v>13</v>
+        <v>637</v>
       </c>
       <c r="F128" t="s">
         <v>10</v>
@@ -4899,7 +4960,7 @@
         <v>52</v>
       </c>
       <c r="E131" t="s">
-        <v>13</v>
+        <v>634</v>
       </c>
       <c r="F131" t="s">
         <v>10</v>
@@ -4919,7 +4980,7 @@
         <v>16</v>
       </c>
       <c r="E132" t="s">
-        <v>329</v>
+        <v>632</v>
       </c>
       <c r="F132" t="s">
         <v>10</v>
@@ -4927,10 +4988,10 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>329</v>
+      </c>
+      <c r="B133" t="s">
         <v>330</v>
-      </c>
-      <c r="B133" t="s">
-        <v>331</v>
       </c>
       <c r="C133">
         <v>135</v>
@@ -4939,7 +5000,7 @@
         <v>16</v>
       </c>
       <c r="E133" t="s">
-        <v>13</v>
+        <v>635</v>
       </c>
       <c r="F133" t="s">
         <v>10</v>
@@ -4947,10 +5008,10 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>332</v>
+        <v>631</v>
       </c>
       <c r="B134" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C134">
         <v>136</v>
@@ -4959,7 +5020,7 @@
         <v>16</v>
       </c>
       <c r="E134" t="s">
-        <v>13</v>
+        <v>633</v>
       </c>
       <c r="F134" t="s">
         <v>10</v>
@@ -4967,10 +5028,10 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B135" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C135">
         <v>138</v>
@@ -4979,7 +5040,7 @@
         <v>20</v>
       </c>
       <c r="E135" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F135" t="s">
         <v>10</v>
@@ -4987,10 +5048,10 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B136" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C136">
         <v>139</v>
@@ -4999,7 +5060,7 @@
         <v>16</v>
       </c>
       <c r="E136" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F136" t="s">
         <v>226</v>
@@ -5007,10 +5068,10 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B137" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C137">
         <v>140</v>
@@ -5019,7 +5080,7 @@
         <v>52</v>
       </c>
       <c r="E137" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F137" t="s">
         <v>226</v>
@@ -5027,10 +5088,10 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B138" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C138">
         <v>141</v>
@@ -5047,19 +5108,19 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B139" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C139">
         <v>142</v>
       </c>
       <c r="D139" t="s">
-        <v>8</v>
+        <v>621</v>
       </c>
       <c r="E139" t="s">
-        <v>13</v>
+        <v>636</v>
       </c>
       <c r="F139" t="s">
         <v>226</v>
@@ -5067,10 +5128,10 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B140" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C140">
         <v>143</v>
@@ -5079,7 +5140,7 @@
         <v>16</v>
       </c>
       <c r="E140" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F140" t="s">
         <v>226</v>
@@ -5087,10 +5148,10 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B141" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C141">
         <v>144</v>
@@ -5099,7 +5160,7 @@
         <v>20</v>
       </c>
       <c r="E141" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F141" t="s">
         <v>226</v>
@@ -5107,10 +5168,10 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B142" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C142">
         <v>145</v>
@@ -5119,7 +5180,7 @@
         <v>52</v>
       </c>
       <c r="E142" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F142" t="s">
         <v>226</v>
@@ -5127,10 +5188,10 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B143" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C143">
         <v>146</v>
@@ -5139,7 +5200,7 @@
         <v>42</v>
       </c>
       <c r="E143" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F143" t="s">
         <v>226</v>
@@ -5147,10 +5208,10 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B144" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C144">
         <v>147</v>
@@ -5159,7 +5220,7 @@
         <v>52</v>
       </c>
       <c r="E144" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F144" t="s">
         <v>226</v>
@@ -5167,10 +5228,10 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B145" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C145">
         <v>148</v>
@@ -5179,7 +5240,7 @@
         <v>16</v>
       </c>
       <c r="E145" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F145" t="s">
         <v>226</v>
@@ -5187,10 +5248,10 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B146" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C146">
         <v>149</v>
@@ -5199,7 +5260,7 @@
         <v>16</v>
       </c>
       <c r="E146" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F146" t="s">
         <v>10</v>
@@ -5207,10 +5268,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B147" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C147">
         <v>150</v>
@@ -5219,7 +5280,7 @@
         <v>52</v>
       </c>
       <c r="E147" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F147" t="s">
         <v>226</v>
@@ -5227,10 +5288,10 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B148" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C148">
         <v>151</v>
@@ -5239,7 +5300,7 @@
         <v>52</v>
       </c>
       <c r="E148" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F148" t="s">
         <v>226</v>
@@ -5247,10 +5308,10 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B149" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C149">
         <v>152</v>
@@ -5267,19 +5328,19 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B150" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C150">
         <v>153</v>
       </c>
       <c r="D150" t="s">
-        <v>77</v>
+        <v>625</v>
       </c>
       <c r="E150" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F150" t="s">
         <v>226</v>
@@ -5287,10 +5348,10 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B151" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C151">
         <v>154</v>
@@ -5299,7 +5360,7 @@
         <v>16</v>
       </c>
       <c r="E151" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F151" t="s">
         <v>10</v>
@@ -5307,10 +5368,10 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B152" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C152">
         <v>155</v>
@@ -5319,7 +5380,7 @@
         <v>16</v>
       </c>
       <c r="E152" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F152" t="s">
         <v>10</v>
@@ -5327,10 +5388,10 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B153" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C153">
         <v>156</v>
@@ -5339,7 +5400,7 @@
         <v>16</v>
       </c>
       <c r="E153" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F153" t="s">
         <v>226</v>
@@ -5347,10 +5408,10 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B154" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C154">
         <v>157</v>
@@ -5359,7 +5420,7 @@
         <v>8</v>
       </c>
       <c r="E154" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F154" t="s">
         <v>226</v>
@@ -5367,10 +5428,10 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B155" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C155">
         <v>158</v>
@@ -5379,7 +5440,7 @@
         <v>52</v>
       </c>
       <c r="E155" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="F155" t="s">
         <v>226</v>
@@ -5387,10 +5448,10 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B156" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C156">
         <v>159</v>
@@ -5399,7 +5460,7 @@
         <v>16</v>
       </c>
       <c r="E156" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F156" t="s">
         <v>226</v>
@@ -5407,10 +5468,10 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B157" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C157">
         <v>160</v>
@@ -5419,7 +5480,7 @@
         <v>52</v>
       </c>
       <c r="E157" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F157" t="s">
         <v>226</v>
@@ -5427,10 +5488,10 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B158" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C158">
         <v>161</v>
@@ -5439,7 +5500,7 @@
         <v>16</v>
       </c>
       <c r="E158" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F158" t="s">
         <v>226</v>
@@ -5447,10 +5508,10 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B159" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C159">
         <v>162</v>
@@ -5459,7 +5520,7 @@
         <v>16</v>
       </c>
       <c r="E159" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F159" t="s">
         <v>226</v>
@@ -5467,10 +5528,10 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B160" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C160">
         <v>163</v>
@@ -5479,7 +5540,7 @@
         <v>16</v>
       </c>
       <c r="E160" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F160" t="s">
         <v>226</v>
@@ -5487,10 +5548,10 @@
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B161" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C161">
         <v>164</v>
@@ -5499,7 +5560,7 @@
         <v>52</v>
       </c>
       <c r="E161" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F161" t="s">
         <v>226</v>
@@ -5507,10 +5568,10 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B162" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C162">
         <v>165</v>
@@ -5519,7 +5580,7 @@
         <v>16</v>
       </c>
       <c r="E162" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F162" t="s">
         <v>10</v>
@@ -5527,10 +5588,10 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B163" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C163">
         <v>166</v>
@@ -5539,7 +5600,7 @@
         <v>52</v>
       </c>
       <c r="E163" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F163" t="s">
         <v>226</v>
@@ -5547,10 +5608,10 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B164" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C164">
         <v>167</v>
@@ -5559,7 +5620,7 @@
         <v>16</v>
       </c>
       <c r="E164" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F164" t="s">
         <v>226</v>
@@ -5567,10 +5628,10 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B165" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C165">
         <v>168</v>
@@ -5579,7 +5640,7 @@
         <v>16</v>
       </c>
       <c r="E165" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F165" t="s">
         <v>10</v>
@@ -5587,19 +5648,19 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B166" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C166">
         <v>169</v>
       </c>
       <c r="D166" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E166" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="F166" t="s">
         <v>226</v>
@@ -5607,10 +5668,10 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B167" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C167">
         <v>170</v>
@@ -5619,7 +5680,7 @@
         <v>16</v>
       </c>
       <c r="E167" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F167" t="s">
         <v>10</v>
@@ -5627,10 +5688,10 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B168" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C168">
         <v>171</v>
@@ -5639,7 +5700,7 @@
         <v>52</v>
       </c>
       <c r="E168" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F168" t="s">
         <v>226</v>
@@ -5647,10 +5708,10 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B169" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C169">
         <v>172</v>
@@ -5659,7 +5720,7 @@
         <v>16</v>
       </c>
       <c r="E169" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F169" t="s">
         <v>10</v>
@@ -5667,10 +5728,10 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B170" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C170">
         <v>173</v>
@@ -5679,7 +5740,7 @@
         <v>16</v>
       </c>
       <c r="E170" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F170" t="s">
         <v>226</v>
@@ -5687,10 +5748,10 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B171" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C171">
         <v>174</v>
@@ -5707,10 +5768,10 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B172" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C172">
         <v>175</v>
@@ -5719,7 +5780,7 @@
         <v>16</v>
       </c>
       <c r="E172" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F172" t="s">
         <v>226</v>
@@ -5727,10 +5788,10 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B173" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C173">
         <v>176</v>
@@ -5739,7 +5800,7 @@
         <v>16</v>
       </c>
       <c r="E173" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F173" t="s">
         <v>10</v>
@@ -5747,10 +5808,10 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B174" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C174">
         <v>177</v>
@@ -5759,7 +5820,7 @@
         <v>42</v>
       </c>
       <c r="E174" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F174" t="s">
         <v>226</v>
@@ -5767,10 +5828,10 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B175" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C175">
         <v>178</v>
@@ -5787,10 +5848,10 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B176" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C176">
         <v>179</v>
@@ -5799,7 +5860,7 @@
         <v>16</v>
       </c>
       <c r="E176" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F176" t="s">
         <v>10</v>
@@ -5807,10 +5868,10 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B177" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C177">
         <v>180</v>
@@ -5827,10 +5888,10 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B178" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C178">
         <v>181</v>
@@ -5847,10 +5908,10 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B179" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C179">
         <v>182</v>
@@ -5859,7 +5920,7 @@
         <v>16</v>
       </c>
       <c r="E179" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F179" t="s">
         <v>10</v>
@@ -5867,10 +5928,10 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B180" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C180">
         <v>183</v>
@@ -5879,7 +5940,7 @@
         <v>52</v>
       </c>
       <c r="E180" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F180" t="s">
         <v>226</v>
@@ -5887,10 +5948,10 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B181" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C181">
         <v>184</v>
@@ -5899,7 +5960,7 @@
         <v>42</v>
       </c>
       <c r="E181" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F181" t="s">
         <v>10</v>
@@ -5907,10 +5968,10 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B182" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C182">
         <v>185</v>
@@ -5927,10 +5988,10 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B183" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C183">
         <v>186</v>
@@ -5939,7 +6000,7 @@
         <v>20</v>
       </c>
       <c r="E183" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F183" t="s">
         <v>226</v>
@@ -5947,10 +6008,10 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B184" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C184">
         <v>187</v>
@@ -5959,7 +6020,7 @@
         <v>16</v>
       </c>
       <c r="E184" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F184" t="s">
         <v>226</v>
@@ -5967,10 +6028,10 @@
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B185" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C185">
         <v>189</v>
@@ -5979,7 +6040,7 @@
         <v>16</v>
       </c>
       <c r="E185" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F185" t="s">
         <v>226</v>
@@ -5996,10 +6057,10 @@
         <v>190</v>
       </c>
       <c r="D186" t="s">
-        <v>52</v>
+        <v>625</v>
       </c>
       <c r="E186" t="s">
-        <v>13</v>
+        <v>626</v>
       </c>
       <c r="F186" t="s">
         <v>10</v>
@@ -6007,10 +6068,10 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B187" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C187">
         <v>191</v>
@@ -6019,7 +6080,7 @@
         <v>8</v>
       </c>
       <c r="E187" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F187" t="s">
         <v>10</v>
@@ -6027,10 +6088,10 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B188" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C188">
         <v>192</v>
@@ -6039,7 +6100,7 @@
         <v>8</v>
       </c>
       <c r="E188" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F188" t="s">
         <v>226</v>
@@ -6047,10 +6108,10 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B189" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C189">
         <v>193</v>
@@ -6059,7 +6120,7 @@
         <v>8</v>
       </c>
       <c r="E189" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F189" t="s">
         <v>226</v>
@@ -6067,10 +6128,10 @@
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B190" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C190">
         <v>194</v>
@@ -6079,7 +6140,7 @@
         <v>8</v>
       </c>
       <c r="E190" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F190" t="s">
         <v>226</v>
@@ -6087,10 +6148,10 @@
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B191" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C191">
         <v>195</v>
@@ -6099,7 +6160,7 @@
         <v>8</v>
       </c>
       <c r="E191" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F191" t="s">
         <v>226</v>
@@ -6107,10 +6168,10 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B192" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C192">
         <v>196</v>
@@ -6127,10 +6188,10 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B193" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C193">
         <v>197</v>
@@ -6139,7 +6200,7 @@
         <v>20</v>
       </c>
       <c r="E193" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F193" t="s">
         <v>226</v>
@@ -6147,10 +6208,10 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B194" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C194">
         <v>198</v>
@@ -6159,7 +6220,7 @@
         <v>16</v>
       </c>
       <c r="E194" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="F194" t="s">
         <v>226</v>
@@ -6167,10 +6228,10 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B195" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C195">
         <v>199</v>
@@ -6179,7 +6240,7 @@
         <v>16</v>
       </c>
       <c r="E195" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F195" t="s">
         <v>10</v>
@@ -6187,10 +6248,10 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B196" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C196">
         <v>200</v>
@@ -6199,7 +6260,7 @@
         <v>42</v>
       </c>
       <c r="E196" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="F196" t="s">
         <v>226</v>
@@ -6207,16 +6268,16 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>501</v>
+      </c>
+      <c r="B197" t="s">
+        <v>502</v>
+      </c>
+      <c r="D197" t="s">
+        <v>8</v>
+      </c>
+      <c r="E197" t="s">
         <v>503</v>
-      </c>
-      <c r="B197" t="s">
-        <v>504</v>
-      </c>
-      <c r="D197" t="s">
-        <v>8</v>
-      </c>
-      <c r="E197" t="s">
-        <v>505</v>
       </c>
       <c r="F197" t="s">
         <v>226</v>
@@ -6224,10 +6285,10 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B198" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D198" t="s">
         <v>8</v>
@@ -6241,16 +6302,16 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>506</v>
+      </c>
+      <c r="B199" t="s">
+        <v>507</v>
+      </c>
+      <c r="D199" t="s">
+        <v>8</v>
+      </c>
+      <c r="E199" t="s">
         <v>508</v>
-      </c>
-      <c r="B199" t="s">
-        <v>509</v>
-      </c>
-      <c r="D199" t="s">
-        <v>8</v>
-      </c>
-      <c r="E199" t="s">
-        <v>510</v>
       </c>
       <c r="F199" t="s">
         <v>226</v>
@@ -6258,16 +6319,16 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
+        <v>509</v>
+      </c>
+      <c r="B200" t="s">
+        <v>510</v>
+      </c>
+      <c r="D200" t="s">
+        <v>8</v>
+      </c>
+      <c r="E200" t="s">
         <v>511</v>
-      </c>
-      <c r="B200" t="s">
-        <v>512</v>
-      </c>
-      <c r="D200" t="s">
-        <v>8</v>
-      </c>
-      <c r="E200" t="s">
-        <v>513</v>
       </c>
       <c r="F200" t="s">
         <v>226</v>
@@ -6275,16 +6336,16 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B201" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D201" t="s">
         <v>77</v>
       </c>
       <c r="E201" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F201" t="s">
         <v>226</v>
@@ -6292,10 +6353,10 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B202" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D202" t="s">
         <v>8</v>
@@ -6309,16 +6370,16 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>517</v>
+      </c>
+      <c r="B203" t="s">
+        <v>518</v>
+      </c>
+      <c r="D203" t="s">
+        <v>8</v>
+      </c>
+      <c r="E203" t="s">
         <v>519</v>
-      </c>
-      <c r="B203" t="s">
-        <v>520</v>
-      </c>
-      <c r="D203" t="s">
-        <v>8</v>
-      </c>
-      <c r="E203" t="s">
-        <v>521</v>
       </c>
       <c r="F203" t="s">
         <v>226</v>
@@ -6326,16 +6387,16 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
+        <v>520</v>
+      </c>
+      <c r="B204" t="s">
+        <v>521</v>
+      </c>
+      <c r="D204" t="s">
+        <v>8</v>
+      </c>
+      <c r="E204" t="s">
         <v>522</v>
-      </c>
-      <c r="B204" t="s">
-        <v>523</v>
-      </c>
-      <c r="D204" t="s">
-        <v>8</v>
-      </c>
-      <c r="E204" t="s">
-        <v>524</v>
       </c>
       <c r="F204" t="s">
         <v>226</v>
@@ -6343,16 +6404,16 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
+        <v>523</v>
+      </c>
+      <c r="B205" t="s">
+        <v>524</v>
+      </c>
+      <c r="D205" t="s">
+        <v>8</v>
+      </c>
+      <c r="E205" t="s">
         <v>525</v>
-      </c>
-      <c r="B205" t="s">
-        <v>526</v>
-      </c>
-      <c r="D205" t="s">
-        <v>8</v>
-      </c>
-      <c r="E205" t="s">
-        <v>527</v>
       </c>
       <c r="F205" t="s">
         <v>226</v>
@@ -6360,10 +6421,10 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B206" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D206" t="s">
         <v>16</v>
@@ -6377,16 +6438,16 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
+        <v>528</v>
+      </c>
+      <c r="B207" t="s">
+        <v>529</v>
+      </c>
+      <c r="D207" t="s">
+        <v>8</v>
+      </c>
+      <c r="E207" t="s">
         <v>530</v>
-      </c>
-      <c r="B207" t="s">
-        <v>531</v>
-      </c>
-      <c r="D207" t="s">
-        <v>8</v>
-      </c>
-      <c r="E207" t="s">
-        <v>532</v>
       </c>
       <c r="F207" t="s">
         <v>226</v>
@@ -6394,10 +6455,10 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B208" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D208" t="s">
         <v>8</v>
@@ -6411,10 +6472,10 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B209" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D209" t="s">
         <v>8</v>
@@ -6428,16 +6489,16 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
+        <v>535</v>
+      </c>
+      <c r="B210" t="s">
+        <v>536</v>
+      </c>
+      <c r="D210" t="s">
+        <v>8</v>
+      </c>
+      <c r="E210" t="s">
         <v>537</v>
-      </c>
-      <c r="B210" t="s">
-        <v>538</v>
-      </c>
-      <c r="D210" t="s">
-        <v>8</v>
-      </c>
-      <c r="E210" t="s">
-        <v>539</v>
       </c>
       <c r="F210" t="s">
         <v>226</v>
@@ -6445,10 +6506,10 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B211" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D211" t="s">
         <v>8</v>
@@ -6462,10 +6523,10 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B212" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D212" t="s">
         <v>8</v>
@@ -6479,16 +6540,16 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
+        <v>542</v>
+      </c>
+      <c r="B213" t="s">
+        <v>543</v>
+      </c>
+      <c r="D213" t="s">
+        <v>8</v>
+      </c>
+      <c r="E213" t="s">
         <v>544</v>
-      </c>
-      <c r="B213" t="s">
-        <v>545</v>
-      </c>
-      <c r="D213" t="s">
-        <v>8</v>
-      </c>
-      <c r="E213" t="s">
-        <v>546</v>
       </c>
       <c r="F213" t="s">
         <v>226</v>
@@ -6496,16 +6557,16 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
+        <v>545</v>
+      </c>
+      <c r="B214" t="s">
+        <v>546</v>
+      </c>
+      <c r="D214" t="s">
+        <v>8</v>
+      </c>
+      <c r="E214" t="s">
         <v>547</v>
-      </c>
-      <c r="B214" t="s">
-        <v>548</v>
-      </c>
-      <c r="D214" t="s">
-        <v>8</v>
-      </c>
-      <c r="E214" t="s">
-        <v>549</v>
       </c>
       <c r="F214" t="s">
         <v>226</v>
@@ -6513,16 +6574,16 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B215" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D215" t="s">
         <v>20</v>
       </c>
       <c r="E215" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F215" t="s">
         <v>226</v>
@@ -6530,16 +6591,16 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
+        <v>551</v>
+      </c>
+      <c r="B216" t="s">
+        <v>552</v>
+      </c>
+      <c r="D216" t="s">
+        <v>8</v>
+      </c>
+      <c r="E216" t="s">
         <v>553</v>
-      </c>
-      <c r="B216" t="s">
-        <v>554</v>
-      </c>
-      <c r="D216" t="s">
-        <v>8</v>
-      </c>
-      <c r="E216" t="s">
-        <v>555</v>
       </c>
       <c r="F216" t="s">
         <v>226</v>
@@ -6547,10 +6608,10 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B217" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D217" t="s">
         <v>8</v>
@@ -6564,16 +6625,16 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
+        <v>556</v>
+      </c>
+      <c r="B218" t="s">
+        <v>557</v>
+      </c>
+      <c r="D218" t="s">
+        <v>8</v>
+      </c>
+      <c r="E218" t="s">
         <v>558</v>
-      </c>
-      <c r="B218" t="s">
-        <v>559</v>
-      </c>
-      <c r="D218" t="s">
-        <v>8</v>
-      </c>
-      <c r="E218" t="s">
-        <v>560</v>
       </c>
       <c r="F218" t="s">
         <v>226</v>
@@ -6581,16 +6642,16 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
+        <v>559</v>
+      </c>
+      <c r="B219" t="s">
+        <v>560</v>
+      </c>
+      <c r="D219" t="s">
+        <v>8</v>
+      </c>
+      <c r="E219" t="s">
         <v>561</v>
-      </c>
-      <c r="B219" t="s">
-        <v>562</v>
-      </c>
-      <c r="D219" t="s">
-        <v>8</v>
-      </c>
-      <c r="E219" t="s">
-        <v>563</v>
       </c>
       <c r="F219" t="s">
         <v>226</v>
@@ -6598,16 +6659,16 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
+        <v>562</v>
+      </c>
+      <c r="B220" t="s">
+        <v>563</v>
+      </c>
+      <c r="D220" t="s">
+        <v>8</v>
+      </c>
+      <c r="E220" t="s">
         <v>564</v>
-      </c>
-      <c r="B220" t="s">
-        <v>565</v>
-      </c>
-      <c r="D220" t="s">
-        <v>8</v>
-      </c>
-      <c r="E220" t="s">
-        <v>566</v>
       </c>
       <c r="F220" t="s">
         <v>226</v>
@@ -6615,16 +6676,16 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
+        <v>565</v>
+      </c>
+      <c r="B221" t="s">
+        <v>566</v>
+      </c>
+      <c r="D221" t="s">
+        <v>8</v>
+      </c>
+      <c r="E221" t="s">
         <v>567</v>
-      </c>
-      <c r="B221" t="s">
-        <v>568</v>
-      </c>
-      <c r="D221" t="s">
-        <v>8</v>
-      </c>
-      <c r="E221" t="s">
-        <v>569</v>
       </c>
       <c r="F221" t="s">
         <v>10</v>
@@ -6632,10 +6693,10 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B222" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="D222" t="s">
         <v>8</v>
@@ -6649,16 +6710,16 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
+        <v>570</v>
+      </c>
+      <c r="B223" t="s">
+        <v>571</v>
+      </c>
+      <c r="D223" t="s">
+        <v>8</v>
+      </c>
+      <c r="E223" t="s">
         <v>572</v>
-      </c>
-      <c r="B223" t="s">
-        <v>573</v>
-      </c>
-      <c r="D223" t="s">
-        <v>8</v>
-      </c>
-      <c r="E223" t="s">
-        <v>574</v>
       </c>
       <c r="F223" t="s">
         <v>226</v>
@@ -6666,16 +6727,16 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
+        <v>573</v>
+      </c>
+      <c r="B224" t="s">
+        <v>574</v>
+      </c>
+      <c r="D224" t="s">
+        <v>8</v>
+      </c>
+      <c r="E224" t="s">
         <v>575</v>
-      </c>
-      <c r="B224" t="s">
-        <v>576</v>
-      </c>
-      <c r="D224" t="s">
-        <v>8</v>
-      </c>
-      <c r="E224" t="s">
-        <v>577</v>
       </c>
       <c r="F224" t="s">
         <v>226</v>
@@ -6683,16 +6744,16 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
+        <v>576</v>
+      </c>
+      <c r="B225" t="s">
+        <v>577</v>
+      </c>
+      <c r="D225" t="s">
+        <v>8</v>
+      </c>
+      <c r="E225" t="s">
         <v>578</v>
-      </c>
-      <c r="B225" t="s">
-        <v>579</v>
-      </c>
-      <c r="D225" t="s">
-        <v>8</v>
-      </c>
-      <c r="E225" t="s">
-        <v>580</v>
       </c>
       <c r="F225" t="s">
         <v>10</v>
@@ -6700,16 +6761,16 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
+        <v>579</v>
+      </c>
+      <c r="B226" t="s">
+        <v>580</v>
+      </c>
+      <c r="D226" t="s">
+        <v>8</v>
+      </c>
+      <c r="E226" t="s">
         <v>581</v>
-      </c>
-      <c r="B226" t="s">
-        <v>582</v>
-      </c>
-      <c r="D226" t="s">
-        <v>8</v>
-      </c>
-      <c r="E226" t="s">
-        <v>583</v>
       </c>
       <c r="F226" t="s">
         <v>226</v>
@@ -6717,10 +6778,10 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B227" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D227" t="s">
         <v>8</v>
@@ -6734,16 +6795,16 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
+        <v>584</v>
+      </c>
+      <c r="B228" t="s">
+        <v>585</v>
+      </c>
+      <c r="D228" t="s">
+        <v>8</v>
+      </c>
+      <c r="E228" t="s">
         <v>586</v>
-      </c>
-      <c r="B228" t="s">
-        <v>587</v>
-      </c>
-      <c r="D228" t="s">
-        <v>8</v>
-      </c>
-      <c r="E228" t="s">
-        <v>588</v>
       </c>
       <c r="F228" t="s">
         <v>226</v>
@@ -6751,10 +6812,10 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B229" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="D229" t="s">
         <v>8</v>
@@ -6768,10 +6829,10 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B230" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="D230" t="s">
         <v>8</v>
@@ -6785,16 +6846,16 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B231" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="D231" t="s">
         <v>20</v>
       </c>
       <c r="E231" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F231" t="s">
         <v>226</v>
@@ -6802,16 +6863,16 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
+        <v>594</v>
+      </c>
+      <c r="B232" t="s">
+        <v>595</v>
+      </c>
+      <c r="D232" t="s">
+        <v>8</v>
+      </c>
+      <c r="E232" t="s">
         <v>596</v>
-      </c>
-      <c r="B232" t="s">
-        <v>597</v>
-      </c>
-      <c r="D232" t="s">
-        <v>8</v>
-      </c>
-      <c r="E232" t="s">
-        <v>598</v>
       </c>
       <c r="F232" t="s">
         <v>226</v>
@@ -6819,10 +6880,10 @@
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B233" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D233" t="s">
         <v>8</v>
@@ -6836,16 +6897,16 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
+        <v>599</v>
+      </c>
+      <c r="B234" t="s">
+        <v>600</v>
+      </c>
+      <c r="D234" t="s">
+        <v>8</v>
+      </c>
+      <c r="E234" t="s">
         <v>601</v>
-      </c>
-      <c r="B234" t="s">
-        <v>602</v>
-      </c>
-      <c r="D234" t="s">
-        <v>8</v>
-      </c>
-      <c r="E234" t="s">
-        <v>603</v>
       </c>
       <c r="F234" t="s">
         <v>226</v>
@@ -6853,16 +6914,16 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
+        <v>602</v>
+      </c>
+      <c r="B235" t="s">
+        <v>603</v>
+      </c>
+      <c r="D235" t="s">
+        <v>8</v>
+      </c>
+      <c r="E235" t="s">
         <v>604</v>
-      </c>
-      <c r="B235" t="s">
-        <v>605</v>
-      </c>
-      <c r="D235" t="s">
-        <v>8</v>
-      </c>
-      <c r="E235" t="s">
-        <v>606</v>
       </c>
       <c r="F235" t="s">
         <v>226</v>
@@ -6870,7 +6931,7 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B236" t="s">
         <v>285</v>
@@ -6879,7 +6940,7 @@
         <v>8</v>
       </c>
       <c r="E236" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F236" t="s">
         <v>226</v>
@@ -6887,16 +6948,16 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
+        <v>607</v>
+      </c>
+      <c r="B237" t="s">
+        <v>608</v>
+      </c>
+      <c r="D237" t="s">
+        <v>8</v>
+      </c>
+      <c r="E237" t="s">
         <v>609</v>
-      </c>
-      <c r="B237" t="s">
-        <v>610</v>
-      </c>
-      <c r="D237" t="s">
-        <v>8</v>
-      </c>
-      <c r="E237" t="s">
-        <v>611</v>
       </c>
       <c r="F237" t="s">
         <v>226</v>
@@ -6904,16 +6965,16 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
+        <v>610</v>
+      </c>
+      <c r="B238" t="s">
+        <v>611</v>
+      </c>
+      <c r="D238" t="s">
+        <v>8</v>
+      </c>
+      <c r="E238" t="s">
         <v>612</v>
-      </c>
-      <c r="B238" t="s">
-        <v>613</v>
-      </c>
-      <c r="D238" t="s">
-        <v>8</v>
-      </c>
-      <c r="E238" t="s">
-        <v>614</v>
       </c>
       <c r="F238" t="s">
         <v>226</v>
@@ -6921,16 +6982,16 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
+        <v>613</v>
+      </c>
+      <c r="B239" t="s">
+        <v>614</v>
+      </c>
+      <c r="D239" t="s">
+        <v>8</v>
+      </c>
+      <c r="E239" t="s">
         <v>615</v>
-      </c>
-      <c r="B239" t="s">
-        <v>616</v>
-      </c>
-      <c r="D239" t="s">
-        <v>8</v>
-      </c>
-      <c r="E239" t="s">
-        <v>617</v>
       </c>
       <c r="F239" t="s">
         <v>226</v>
@@ -6938,19 +6999,36 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
+        <v>616</v>
+      </c>
+      <c r="B240" t="s">
+        <v>617</v>
+      </c>
+      <c r="D240" t="s">
+        <v>8</v>
+      </c>
+      <c r="E240" t="s">
         <v>618</v>
       </c>
-      <c r="B240" t="s">
-        <v>619</v>
-      </c>
-      <c r="D240" t="s">
-        <v>8</v>
-      </c>
-      <c r="E240" t="s">
-        <v>620</v>
-      </c>
       <c r="F240" t="s">
         <v>226</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>627</v>
+      </c>
+      <c r="B241" t="s">
+        <v>628</v>
+      </c>
+      <c r="D241" t="s">
+        <v>629</v>
+      </c>
+      <c r="E241" t="s">
+        <v>630</v>
+      </c>
+      <c r="F241" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@a50e919bed854152731300c93755d4dcc340107b 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C1FC737-B4A2-467A-BE80-BB0DBEA2F4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F6BA38-D817-454F-9311-651664BF21C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21710" yWindow="-110" windowWidth="21820" windowHeight="38620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="642">
   <si>
     <t>name</t>
   </si>
@@ -1964,6 +1964,10 @@
   </si>
   <si>
     <t>/assets/img/members/student/王巍.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/樊帅.jpg</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2337,8 +2341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="E183" sqref="E183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -5980,7 +5984,7 @@
         <v>36</v>
       </c>
       <c r="E182" t="s">
-        <v>13</v>
+        <v>641</v>
       </c>
       <c r="F182" t="s">
         <v>226</v>

</xml_diff>

<commit_message>
update: 1. profile of Lu Chen 2. logo 3. several avatars
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F6BA38-D817-454F-9311-651664BF21C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465F157A-1BB7-4AF0-BF35-00D9D75DE064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="662">
   <si>
     <t>name</t>
   </si>
@@ -598,6 +598,9 @@
     <t>Wangyou Zhang</t>
   </si>
   <si>
+    <t>/assets/img/members/student/张王优.jpg</t>
+  </si>
+  <si>
     <t>杜晨鹏</t>
   </si>
   <si>
@@ -622,6 +625,9 @@
     <t>Chenda Li</t>
   </si>
   <si>
+    <t>/assets/img/members/student/李晨达.jpg</t>
+  </si>
+  <si>
     <t>卢怡宙</t>
   </si>
   <si>
@@ -772,6 +778,9 @@
     <t>Wei Wang</t>
   </si>
   <si>
+    <t>/assets/img/members/student/王巍.jpg</t>
+  </si>
+  <si>
     <t>吴章昊</t>
   </si>
   <si>
@@ -982,6 +991,9 @@
     <t>Xun Gong</t>
   </si>
   <si>
+    <t>/assets/img/members/student/龚勋.jpg</t>
+  </si>
+  <si>
     <t>兰焜耀</t>
   </si>
   <si>
@@ -1003,21 +1015,36 @@
     <t>Yuncong Liu</t>
   </si>
   <si>
+    <t>/assets/img/members/student/刘韫聪.jpg</t>
+  </si>
+  <si>
     <t>刘森</t>
   </si>
   <si>
     <t>Sen Liu</t>
   </si>
   <si>
+    <t>/assets/img/members/student/刘森.jpg</t>
+  </si>
+  <si>
     <t>李广鹏</t>
   </si>
   <si>
     <t>Guangpeng Li</t>
   </si>
   <si>
+    <t>/assets/img/members/student/李广鹏.jpg</t>
+  </si>
+  <si>
+    <t>杨宝琛</t>
+  </si>
+  <si>
     <t>Baochen Yang</t>
   </si>
   <si>
+    <t>/assets/img/members/student/杨宝琛.jpg</t>
+  </si>
+  <si>
     <t>谢泽宇</t>
   </si>
   <si>
@@ -1057,6 +1084,9 @@
     <t>Qi Chen</t>
   </si>
   <si>
+    <t>/assets/img/members/student/陈琦.jpg</t>
+  </si>
+  <si>
     <t>卢葛威</t>
   </si>
   <si>
@@ -1288,9 +1318,15 @@
     <t>/assets/img/members/student/黎井漂.jpg</t>
   </si>
   <si>
+    <t>李翰奇</t>
+  </si>
+  <si>
     <t>Hanqi Li</t>
   </si>
   <si>
+    <t>/assets/img/members/student/李翰奇.jpg</t>
+  </si>
+  <si>
     <t>孙良泰</t>
   </si>
   <si>
@@ -1420,6 +1456,9 @@
     <t>Shuai Fan</t>
   </si>
   <si>
+    <t>/assets/img/members/student/樊帅.jpg</t>
+  </si>
+  <si>
     <t>王浩然</t>
   </si>
   <si>
@@ -1447,6 +1486,9 @@
     <t>/assets/img/members/student/刘丁烨.jpg</t>
   </si>
   <si>
+    <t>/assets/img/members/student/陈博2.jpg</t>
+  </si>
+  <si>
     <t>李梓源</t>
   </si>
   <si>
@@ -1513,6 +1555,9 @@
     <t>Zhihan Li</t>
   </si>
   <si>
+    <t>/assets/img/members/student/李之涵.jpg</t>
+  </si>
+  <si>
     <t>张怡天</t>
   </si>
   <si>
@@ -1525,6 +1570,9 @@
     <t>Bohan Li</t>
   </si>
   <si>
+    <t>/assets/img/members/student/李波含.jpg</t>
+  </si>
+  <si>
     <t>曹义路</t>
   </si>
   <si>
@@ -1879,95 +1927,85 @@
     <t>/assets/img/members/student/江楠.jpg</t>
   </si>
   <si>
-    <t>李翰奇</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李翰奇.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/octocat.png</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李之涵.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李波含.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>P</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/陈博2.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>马英梓</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Yingzi Ma</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>U</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>/assets/img/members/student/马英梓.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>杨宝琛</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/刘森.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/杨宝琛.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/刘韫聪.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李广鹏.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/陈琦.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/龚勋.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/张王优.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李晨达.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/王巍.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/樊帅.jpg</t>
+  </si>
+  <si>
+    <t>涂文明</t>
+  </si>
+  <si>
+    <t>Wenming Tu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/涂文明.jpg</t>
+  </si>
+  <si>
+    <t>梅嘉豪</t>
+  </si>
+  <si>
+    <t>Jiahao Mei</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/梅嘉豪.jpg</t>
+  </si>
+  <si>
+    <t>吴媚</t>
+  </si>
+  <si>
+    <t>WuMei</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/吴媚.jpg</t>
+  </si>
+  <si>
+    <t>王哲祥</t>
+  </si>
+  <si>
+    <t>Zhexiang Wang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/王哲祥.jpg</t>
+  </si>
+  <si>
+    <t>Chonghao Cai</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/蔡崇皓.jpg</t>
+  </si>
+  <si>
+    <t>朱轩宇</t>
+  </si>
+  <si>
+    <t>Xuanyu Zhu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/朱轩宇.jpg</t>
+  </si>
+  <si>
+    <t>陈冠豫</t>
+  </si>
+  <si>
+    <t>Guanyu Chen</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/陈冠豫.jpg</t>
+  </si>
+  <si>
+    <t>刘峻希</t>
+  </si>
+  <si>
+    <t>Junxi Liu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/刘峻希.jpg</t>
+  </si>
+  <si>
+    <t>蔡崇皓</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2339,16 +2377,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F241"/>
+  <dimension ref="A1:F249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="E183" sqref="E183"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="M231" sqref="M231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="95.08984375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3864,7 +3899,7 @@
         <v>52</v>
       </c>
       <c r="E76" t="s">
-        <v>638</v>
+        <v>192</v>
       </c>
       <c r="F76" t="s">
         <v>10</v>
@@ -3872,10 +3907,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B77" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C77">
         <v>78</v>
@@ -3884,7 +3919,7 @@
         <v>52</v>
       </c>
       <c r="E77" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F77" t="s">
         <v>10</v>
@@ -3892,10 +3927,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B78" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C78">
         <v>79</v>
@@ -3904,7 +3939,7 @@
         <v>16</v>
       </c>
       <c r="E78" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F78" t="s">
         <v>10</v>
@@ -3912,10 +3947,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B79" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C79">
         <v>80</v>
@@ -3924,7 +3959,7 @@
         <v>16</v>
       </c>
       <c r="E79" t="s">
-        <v>639</v>
+        <v>201</v>
       </c>
       <c r="F79" t="s">
         <v>10</v>
@@ -3932,10 +3967,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B80" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C80">
         <v>81</v>
@@ -3952,10 +3987,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B81" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C81">
         <v>82</v>
@@ -3972,10 +4007,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B82" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C82">
         <v>83</v>
@@ -3992,10 +4027,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B83" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C83">
         <v>84</v>
@@ -4004,7 +4039,7 @@
         <v>77</v>
       </c>
       <c r="E83" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F83" t="s">
         <v>10</v>
@@ -4012,10 +4047,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B84" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C84">
         <v>85</v>
@@ -4024,7 +4059,7 @@
         <v>16</v>
       </c>
       <c r="E84" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F84" t="s">
         <v>10</v>
@@ -4032,10 +4067,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B85" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C85">
         <v>86</v>
@@ -4052,10 +4087,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B86" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C86">
         <v>87</v>
@@ -4072,10 +4107,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B87" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C87">
         <v>88</v>
@@ -4092,10 +4127,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B88" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C88">
         <v>89</v>
@@ -4112,10 +4147,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B89" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C89">
         <v>90</v>
@@ -4124,7 +4159,7 @@
         <v>52</v>
       </c>
       <c r="E89" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F89" t="s">
         <v>10</v>
@@ -4132,10 +4167,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B90" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C90">
         <v>91</v>
@@ -4144,18 +4179,18 @@
         <v>52</v>
       </c>
       <c r="E90" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F90" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B91" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C91">
         <v>92</v>
@@ -4164,7 +4199,7 @@
         <v>20</v>
       </c>
       <c r="E91" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F91" t="s">
         <v>10</v>
@@ -4172,10 +4207,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B92" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C92">
         <v>93</v>
@@ -4184,7 +4219,7 @@
         <v>77</v>
       </c>
       <c r="E92" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F92" t="s">
         <v>10</v>
@@ -4192,10 +4227,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B93" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C93">
         <v>94</v>
@@ -4204,18 +4239,18 @@
         <v>77</v>
       </c>
       <c r="E93" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F93" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B94" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C94">
         <v>95</v>
@@ -4224,7 +4259,7 @@
         <v>16</v>
       </c>
       <c r="E94" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F94" t="s">
         <v>10</v>
@@ -4232,10 +4267,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B95" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C95">
         <v>96</v>
@@ -4252,10 +4287,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B96" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C96">
         <v>97</v>
@@ -4272,10 +4307,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B97" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C97">
         <v>98</v>
@@ -4284,18 +4319,18 @@
         <v>77</v>
       </c>
       <c r="E97" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F97" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B98" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C98">
         <v>99</v>
@@ -4312,10 +4347,10 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B99" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C99">
         <v>100</v>
@@ -4324,7 +4359,7 @@
         <v>16</v>
       </c>
       <c r="E99" t="s">
-        <v>640</v>
+        <v>252</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
@@ -4332,10 +4367,10 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B100" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C100">
         <v>101</v>
@@ -4352,10 +4387,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B101" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C101">
         <v>102</v>
@@ -4372,10 +4407,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B102" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C102">
         <v>103</v>
@@ -4392,10 +4427,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B103" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C103">
         <v>104</v>
@@ -4412,10 +4447,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B104" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C104">
         <v>105</v>
@@ -4424,7 +4459,7 @@
         <v>8</v>
       </c>
       <c r="E104" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F104" t="s">
         <v>10</v>
@@ -4432,10 +4467,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B105" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C105">
         <v>106</v>
@@ -4444,18 +4479,18 @@
         <v>52</v>
       </c>
       <c r="E105" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F105" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B106" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C106">
         <v>107</v>
@@ -4464,18 +4499,18 @@
         <v>52</v>
       </c>
       <c r="E106" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F106" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B107" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C107">
         <v>108</v>
@@ -4484,7 +4519,7 @@
         <v>16</v>
       </c>
       <c r="E107" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F107" t="s">
         <v>10</v>
@@ -4492,10 +4527,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B108" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C108">
         <v>109</v>
@@ -4504,7 +4539,7 @@
         <v>77</v>
       </c>
       <c r="E108" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F108" t="s">
         <v>10</v>
@@ -4512,10 +4547,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B109" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C109">
         <v>110</v>
@@ -4524,7 +4559,7 @@
         <v>16</v>
       </c>
       <c r="E109" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F109" t="s">
         <v>10</v>
@@ -4532,10 +4567,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B110" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C110">
         <v>111</v>
@@ -4544,7 +4579,7 @@
         <v>16</v>
       </c>
       <c r="E110" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F110" t="s">
         <v>10</v>
@@ -4552,10 +4587,10 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B111" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C111">
         <v>112</v>
@@ -4564,18 +4599,18 @@
         <v>52</v>
       </c>
       <c r="E111" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F111" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B112" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C112">
         <v>114</v>
@@ -4592,10 +4627,10 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B113" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C113">
         <v>115</v>
@@ -4612,10 +4647,10 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B114" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C114">
         <v>116</v>
@@ -4632,10 +4667,10 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B115" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C115">
         <v>117</v>
@@ -4652,10 +4687,10 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B116" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C116">
         <v>118</v>
@@ -4672,10 +4707,10 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B117" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C117">
         <v>119</v>
@@ -4692,10 +4727,10 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B118" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C118">
         <v>120</v>
@@ -4712,10 +4747,10 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B119" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C119">
         <v>121</v>
@@ -4732,10 +4767,10 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B120" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C120">
         <v>122</v>
@@ -4752,10 +4787,10 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B121" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C121">
         <v>123</v>
@@ -4772,10 +4807,10 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B122" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C122">
         <v>124</v>
@@ -4784,7 +4819,7 @@
         <v>16</v>
       </c>
       <c r="E122" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F122" t="s">
         <v>10</v>
@@ -4792,10 +4827,10 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B123" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C123">
         <v>125</v>
@@ -4812,10 +4847,10 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B124" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C124">
         <v>126</v>
@@ -4824,7 +4859,7 @@
         <v>16</v>
       </c>
       <c r="E124" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="F124" t="s">
         <v>10</v>
@@ -4832,10 +4867,10 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B125" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C125">
         <v>127</v>
@@ -4852,10 +4887,10 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B126" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C126">
         <v>128</v>
@@ -4864,7 +4899,7 @@
         <v>16</v>
       </c>
       <c r="E126" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F126" t="s">
         <v>10</v>
@@ -4872,10 +4907,10 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B127" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C127">
         <v>129</v>
@@ -4884,18 +4919,18 @@
         <v>52</v>
       </c>
       <c r="E127" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="F127" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B128" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C128">
         <v>130</v>
@@ -4904,7 +4939,7 @@
         <v>52</v>
       </c>
       <c r="E128" t="s">
-        <v>637</v>
+        <v>323</v>
       </c>
       <c r="F128" t="s">
         <v>10</v>
@@ -4912,10 +4947,10 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B129" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C129">
         <v>131</v>
@@ -4924,18 +4959,18 @@
         <v>77</v>
       </c>
       <c r="E129" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="F129" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B130" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C130">
         <v>132</v>
@@ -4952,10 +4987,10 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B131" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C131">
         <v>133</v>
@@ -4964,7 +4999,7 @@
         <v>52</v>
       </c>
       <c r="E131" t="s">
-        <v>634</v>
+        <v>331</v>
       </c>
       <c r="F131" t="s">
         <v>10</v>
@@ -4972,10 +5007,10 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="B132" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="C132">
         <v>134</v>
@@ -4984,7 +5019,7 @@
         <v>16</v>
       </c>
       <c r="E132" t="s">
-        <v>632</v>
+        <v>334</v>
       </c>
       <c r="F132" t="s">
         <v>10</v>
@@ -4992,10 +5027,10 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B133" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C133">
         <v>135</v>
@@ -5004,7 +5039,7 @@
         <v>16</v>
       </c>
       <c r="E133" t="s">
-        <v>635</v>
+        <v>337</v>
       </c>
       <c r="F133" t="s">
         <v>10</v>
@@ -5012,10 +5047,10 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>631</v>
+        <v>338</v>
       </c>
       <c r="B134" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="C134">
         <v>136</v>
@@ -5024,7 +5059,7 @@
         <v>16</v>
       </c>
       <c r="E134" t="s">
-        <v>633</v>
+        <v>340</v>
       </c>
       <c r="F134" t="s">
         <v>10</v>
@@ -5032,10 +5067,10 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="B135" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="C135">
         <v>138</v>
@@ -5044,7 +5079,7 @@
         <v>20</v>
       </c>
       <c r="E135" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="F135" t="s">
         <v>10</v>
@@ -5052,10 +5087,10 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="B136" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="C136">
         <v>139</v>
@@ -5064,18 +5099,18 @@
         <v>16</v>
       </c>
       <c r="E136" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="F136" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="B137" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="C137">
         <v>140</v>
@@ -5084,18 +5119,18 @@
         <v>52</v>
       </c>
       <c r="E137" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="F137" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="B138" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="C138">
         <v>141</v>
@@ -5107,35 +5142,35 @@
         <v>13</v>
       </c>
       <c r="F138" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="B139" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="C139">
         <v>142</v>
       </c>
       <c r="D139" t="s">
-        <v>621</v>
+        <v>42</v>
       </c>
       <c r="E139" t="s">
-        <v>636</v>
+        <v>354</v>
       </c>
       <c r="F139" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="B140" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="C140">
         <v>143</v>
@@ -5144,18 +5179,18 @@
         <v>16</v>
       </c>
       <c r="E140" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="F140" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="B141" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="C141">
         <v>144</v>
@@ -5164,18 +5199,18 @@
         <v>20</v>
       </c>
       <c r="E141" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="F141" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="B142" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="C142">
         <v>145</v>
@@ -5184,18 +5219,18 @@
         <v>52</v>
       </c>
       <c r="E142" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="F142" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="B143" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="C143">
         <v>146</v>
@@ -5204,18 +5239,18 @@
         <v>42</v>
       </c>
       <c r="E143" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="F143" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="B144" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="C144">
         <v>147</v>
@@ -5224,18 +5259,18 @@
         <v>52</v>
       </c>
       <c r="E144" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="F144" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="B145" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="C145">
         <v>148</v>
@@ -5244,18 +5279,18 @@
         <v>16</v>
       </c>
       <c r="E145" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="F145" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="B146" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="C146">
         <v>149</v>
@@ -5264,7 +5299,7 @@
         <v>16</v>
       </c>
       <c r="E146" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="F146" t="s">
         <v>10</v>
@@ -5272,10 +5307,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="B147" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="C147">
         <v>150</v>
@@ -5284,18 +5319,18 @@
         <v>52</v>
       </c>
       <c r="E147" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="F147" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="B148" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="C148">
         <v>151</v>
@@ -5304,18 +5339,18 @@
         <v>52</v>
       </c>
       <c r="E148" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="F148" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="B149" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="C149">
         <v>152</v>
@@ -5327,35 +5362,35 @@
         <v>13</v>
       </c>
       <c r="F149" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="B150" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="C150">
         <v>153</v>
       </c>
       <c r="D150" t="s">
-        <v>625</v>
+        <v>52</v>
       </c>
       <c r="E150" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="F150" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="B151" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="C151">
         <v>154</v>
@@ -5364,7 +5399,7 @@
         <v>16</v>
       </c>
       <c r="E151" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="F151" t="s">
         <v>10</v>
@@ -5372,10 +5407,10 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="B152" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="C152">
         <v>155</v>
@@ -5384,7 +5419,7 @@
         <v>16</v>
       </c>
       <c r="E152" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="F152" t="s">
         <v>10</v>
@@ -5392,10 +5427,10 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="B153" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C153">
         <v>156</v>
@@ -5404,18 +5439,18 @@
         <v>16</v>
       </c>
       <c r="E153" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="F153" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="B154" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="C154">
         <v>157</v>
@@ -5424,18 +5459,18 @@
         <v>8</v>
       </c>
       <c r="E154" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="F154" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="B155" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C155">
         <v>158</v>
@@ -5444,18 +5479,18 @@
         <v>52</v>
       </c>
       <c r="E155" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="F155" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="B156" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
       <c r="C156">
         <v>159</v>
@@ -5464,18 +5499,18 @@
         <v>16</v>
       </c>
       <c r="E156" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="F156" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
       <c r="B157" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="C157">
         <v>160</v>
@@ -5484,18 +5519,18 @@
         <v>52</v>
       </c>
       <c r="E157" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="F157" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="B158" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="C158">
         <v>161</v>
@@ -5504,18 +5539,18 @@
         <v>16</v>
       </c>
       <c r="E158" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="F158" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="B159" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="C159">
         <v>162</v>
@@ -5524,18 +5559,18 @@
         <v>16</v>
       </c>
       <c r="E159" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="F159" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="B160" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="C160">
         <v>163</v>
@@ -5544,18 +5579,18 @@
         <v>16</v>
       </c>
       <c r="E160" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="F160" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="B161" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="C161">
         <v>164</v>
@@ -5564,18 +5599,18 @@
         <v>52</v>
       </c>
       <c r="E161" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="F161" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="B162" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="C162">
         <v>165</v>
@@ -5584,7 +5619,7 @@
         <v>16</v>
       </c>
       <c r="E162" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="F162" t="s">
         <v>10</v>
@@ -5592,10 +5627,10 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="B163" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="C163">
         <v>166</v>
@@ -5604,18 +5639,18 @@
         <v>52</v>
       </c>
       <c r="E163" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="F163" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="B164" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="C164">
         <v>167</v>
@@ -5624,18 +5659,18 @@
         <v>16</v>
       </c>
       <c r="E164" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="F164" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>419</v>
+        <v>429</v>
       </c>
       <c r="B165" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="C165">
         <v>168</v>
@@ -5644,7 +5679,7 @@
         <v>16</v>
       </c>
       <c r="E165" t="s">
-        <v>421</v>
+        <v>431</v>
       </c>
       <c r="F165" t="s">
         <v>10</v>
@@ -5652,30 +5687,30 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>619</v>
+        <v>432</v>
       </c>
       <c r="B166" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="C166">
         <v>169</v>
       </c>
       <c r="D166" t="s">
-        <v>621</v>
+        <v>42</v>
       </c>
       <c r="E166" t="s">
-        <v>620</v>
+        <v>434</v>
       </c>
       <c r="F166" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="B167" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="C167">
         <v>170</v>
@@ -5684,7 +5719,7 @@
         <v>16</v>
       </c>
       <c r="E167" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="F167" t="s">
         <v>10</v>
@@ -5692,10 +5727,10 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="B168" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="C168">
         <v>171</v>
@@ -5704,18 +5739,18 @@
         <v>52</v>
       </c>
       <c r="E168" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="F168" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="B169" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="C169">
         <v>172</v>
@@ -5724,7 +5759,7 @@
         <v>16</v>
       </c>
       <c r="E169" t="s">
-        <v>431</v>
+        <v>443</v>
       </c>
       <c r="F169" t="s">
         <v>10</v>
@@ -5732,10 +5767,10 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>432</v>
+        <v>444</v>
       </c>
       <c r="B170" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="C170">
         <v>173</v>
@@ -5744,18 +5779,18 @@
         <v>16</v>
       </c>
       <c r="E170" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="F170" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="B171" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="C171">
         <v>174</v>
@@ -5767,15 +5802,15 @@
         <v>13</v>
       </c>
       <c r="F171" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="B172" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="C172">
         <v>175</v>
@@ -5784,18 +5819,18 @@
         <v>16</v>
       </c>
       <c r="E172" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
       <c r="F172" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="B173" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="C173">
         <v>176</v>
@@ -5804,7 +5839,7 @@
         <v>16</v>
       </c>
       <c r="E173" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="F173" t="s">
         <v>10</v>
@@ -5812,10 +5847,10 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="B174" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="C174">
         <v>177</v>
@@ -5824,18 +5859,18 @@
         <v>42</v>
       </c>
       <c r="E174" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="F174" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="B175" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="C175">
         <v>178</v>
@@ -5847,15 +5882,15 @@
         <v>13</v>
       </c>
       <c r="F175" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B176" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="C176">
         <v>179</v>
@@ -5864,7 +5899,7 @@
         <v>16</v>
       </c>
       <c r="E176" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="F176" t="s">
         <v>10</v>
@@ -5872,10 +5907,10 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="B177" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="C177">
         <v>180</v>
@@ -5892,10 +5927,10 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="B178" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="C178">
         <v>181</v>
@@ -5912,10 +5947,10 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
       <c r="B179" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="C179">
         <v>182</v>
@@ -5924,7 +5959,7 @@
         <v>16</v>
       </c>
       <c r="E179" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="F179" t="s">
         <v>10</v>
@@ -5932,10 +5967,10 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="B180" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="C180">
         <v>183</v>
@@ -5944,18 +5979,18 @@
         <v>52</v>
       </c>
       <c r="E180" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="F180" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
       <c r="B181" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="C181">
         <v>184</v>
@@ -5964,7 +5999,7 @@
         <v>42</v>
       </c>
       <c r="E181" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="F181" t="s">
         <v>10</v>
@@ -5972,10 +6007,10 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="B182" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="C182">
         <v>185</v>
@@ -5984,18 +6019,18 @@
         <v>36</v>
       </c>
       <c r="E182" t="s">
-        <v>641</v>
+        <v>478</v>
       </c>
       <c r="F182" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>466</v>
+        <v>479</v>
       </c>
       <c r="B183" t="s">
-        <v>467</v>
+        <v>480</v>
       </c>
       <c r="C183">
         <v>186</v>
@@ -6004,18 +6039,18 @@
         <v>20</v>
       </c>
       <c r="E183" t="s">
-        <v>468</v>
+        <v>481</v>
       </c>
       <c r="F183" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>469</v>
+        <v>482</v>
       </c>
       <c r="B184" t="s">
-        <v>470</v>
+        <v>483</v>
       </c>
       <c r="C184">
         <v>187</v>
@@ -6024,18 +6059,18 @@
         <v>16</v>
       </c>
       <c r="E184" t="s">
-        <v>471</v>
+        <v>484</v>
       </c>
       <c r="F184" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>472</v>
+        <v>485</v>
       </c>
       <c r="B185" t="s">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="C185">
         <v>189</v>
@@ -6044,10 +6079,10 @@
         <v>16</v>
       </c>
       <c r="E185" t="s">
-        <v>474</v>
+        <v>487</v>
       </c>
       <c r="F185" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -6061,10 +6096,10 @@
         <v>190</v>
       </c>
       <c r="D186" t="s">
-        <v>625</v>
+        <v>52</v>
       </c>
       <c r="E186" t="s">
-        <v>626</v>
+        <v>488</v>
       </c>
       <c r="F186" t="s">
         <v>10</v>
@@ -6072,10 +6107,10 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="B187" t="s">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="C187">
         <v>191</v>
@@ -6084,7 +6119,7 @@
         <v>8</v>
       </c>
       <c r="E187" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="F187" t="s">
         <v>10</v>
@@ -6092,10 +6127,10 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>478</v>
+        <v>492</v>
       </c>
       <c r="B188" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="C188">
         <v>192</v>
@@ -6104,18 +6139,18 @@
         <v>8</v>
       </c>
       <c r="E188" t="s">
-        <v>480</v>
+        <v>494</v>
       </c>
       <c r="F188" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="B189" t="s">
-        <v>482</v>
+        <v>496</v>
       </c>
       <c r="C189">
         <v>193</v>
@@ -6124,18 +6159,18 @@
         <v>8</v>
       </c>
       <c r="E189" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="F189" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>484</v>
+        <v>498</v>
       </c>
       <c r="B190" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="C190">
         <v>194</v>
@@ -6144,18 +6179,18 @@
         <v>8</v>
       </c>
       <c r="E190" t="s">
-        <v>486</v>
+        <v>500</v>
       </c>
       <c r="F190" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="B191" t="s">
-        <v>488</v>
+        <v>502</v>
       </c>
       <c r="C191">
         <v>195</v>
@@ -6164,18 +6199,18 @@
         <v>8</v>
       </c>
       <c r="E191" t="s">
-        <v>489</v>
+        <v>503</v>
       </c>
       <c r="F191" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>490</v>
+        <v>504</v>
       </c>
       <c r="B192" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="C192">
         <v>196</v>
@@ -6187,15 +6222,15 @@
         <v>13</v>
       </c>
       <c r="F192" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>492</v>
+        <v>506</v>
       </c>
       <c r="B193" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="C193">
         <v>197</v>
@@ -6204,18 +6239,18 @@
         <v>20</v>
       </c>
       <c r="E193" t="s">
-        <v>494</v>
+        <v>508</v>
       </c>
       <c r="F193" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="B194" t="s">
-        <v>496</v>
+        <v>510</v>
       </c>
       <c r="C194">
         <v>198</v>
@@ -6224,18 +6259,18 @@
         <v>16</v>
       </c>
       <c r="E194" t="s">
-        <v>623</v>
+        <v>511</v>
       </c>
       <c r="F194" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>497</v>
+        <v>512</v>
       </c>
       <c r="B195" t="s">
-        <v>498</v>
+        <v>513</v>
       </c>
       <c r="C195">
         <v>199</v>
@@ -6244,7 +6279,7 @@
         <v>16</v>
       </c>
       <c r="E195" t="s">
-        <v>622</v>
+        <v>13</v>
       </c>
       <c r="F195" t="s">
         <v>10</v>
@@ -6252,10 +6287,10 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>499</v>
+        <v>514</v>
       </c>
       <c r="B196" t="s">
-        <v>500</v>
+        <v>515</v>
       </c>
       <c r="C196">
         <v>200</v>
@@ -6264,35 +6299,35 @@
         <v>42</v>
       </c>
       <c r="E196" t="s">
-        <v>624</v>
+        <v>516</v>
       </c>
       <c r="F196" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>501</v>
+        <v>517</v>
       </c>
       <c r="B197" t="s">
-        <v>502</v>
+        <v>518</v>
       </c>
       <c r="D197" t="s">
         <v>8</v>
       </c>
       <c r="E197" t="s">
-        <v>503</v>
+        <v>519</v>
       </c>
       <c r="F197" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>504</v>
+        <v>520</v>
       </c>
       <c r="B198" t="s">
-        <v>505</v>
+        <v>521</v>
       </c>
       <c r="D198" t="s">
         <v>8</v>
@@ -6301,66 +6336,66 @@
         <v>13</v>
       </c>
       <c r="F198" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>506</v>
+        <v>522</v>
       </c>
       <c r="B199" t="s">
-        <v>507</v>
+        <v>523</v>
       </c>
       <c r="D199" t="s">
         <v>8</v>
       </c>
       <c r="E199" t="s">
-        <v>508</v>
+        <v>524</v>
       </c>
       <c r="F199" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>509</v>
+        <v>525</v>
       </c>
       <c r="B200" t="s">
-        <v>510</v>
+        <v>526</v>
       </c>
       <c r="D200" t="s">
         <v>8</v>
       </c>
       <c r="E200" t="s">
-        <v>511</v>
+        <v>527</v>
       </c>
       <c r="F200" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="B201" t="s">
-        <v>513</v>
+        <v>529</v>
       </c>
       <c r="D201" t="s">
         <v>77</v>
       </c>
       <c r="E201" t="s">
-        <v>514</v>
+        <v>530</v>
       </c>
       <c r="F201" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>515</v>
+        <v>531</v>
       </c>
       <c r="B202" t="s">
-        <v>516</v>
+        <v>532</v>
       </c>
       <c r="D202" t="s">
         <v>8</v>
@@ -6369,66 +6404,66 @@
         <v>13</v>
       </c>
       <c r="F202" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>517</v>
+        <v>533</v>
       </c>
       <c r="B203" t="s">
-        <v>518</v>
+        <v>534</v>
       </c>
       <c r="D203" t="s">
         <v>8</v>
       </c>
       <c r="E203" t="s">
-        <v>519</v>
+        <v>535</v>
       </c>
       <c r="F203" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>520</v>
+        <v>536</v>
       </c>
       <c r="B204" t="s">
-        <v>521</v>
+        <v>537</v>
       </c>
       <c r="D204" t="s">
         <v>8</v>
       </c>
       <c r="E204" t="s">
-        <v>522</v>
+        <v>538</v>
       </c>
       <c r="F204" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>523</v>
+        <v>539</v>
       </c>
       <c r="B205" t="s">
-        <v>524</v>
+        <v>540</v>
       </c>
       <c r="D205" t="s">
         <v>8</v>
       </c>
       <c r="E205" t="s">
-        <v>525</v>
+        <v>541</v>
       </c>
       <c r="F205" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>526</v>
+        <v>542</v>
       </c>
       <c r="B206" t="s">
-        <v>527</v>
+        <v>543</v>
       </c>
       <c r="D206" t="s">
         <v>16</v>
@@ -6437,32 +6472,32 @@
         <v>13</v>
       </c>
       <c r="F206" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>528</v>
+        <v>544</v>
       </c>
       <c r="B207" t="s">
-        <v>529</v>
+        <v>545</v>
       </c>
       <c r="D207" t="s">
         <v>8</v>
       </c>
       <c r="E207" t="s">
-        <v>530</v>
+        <v>546</v>
       </c>
       <c r="F207" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>531</v>
+        <v>547</v>
       </c>
       <c r="B208" t="s">
-        <v>532</v>
+        <v>548</v>
       </c>
       <c r="D208" t="s">
         <v>8</v>
@@ -6471,15 +6506,15 @@
         <v>13</v>
       </c>
       <c r="F208" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>533</v>
+        <v>549</v>
       </c>
       <c r="B209" t="s">
-        <v>534</v>
+        <v>550</v>
       </c>
       <c r="D209" t="s">
         <v>8</v>
@@ -6488,32 +6523,32 @@
         <v>13</v>
       </c>
       <c r="F209" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>535</v>
+        <v>551</v>
       </c>
       <c r="B210" t="s">
-        <v>536</v>
+        <v>552</v>
       </c>
       <c r="D210" t="s">
         <v>8</v>
       </c>
       <c r="E210" t="s">
-        <v>537</v>
+        <v>553</v>
       </c>
       <c r="F210" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>538</v>
+        <v>554</v>
       </c>
       <c r="B211" t="s">
-        <v>539</v>
+        <v>555</v>
       </c>
       <c r="D211" t="s">
         <v>8</v>
@@ -6522,15 +6557,15 @@
         <v>13</v>
       </c>
       <c r="F211" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>540</v>
+        <v>556</v>
       </c>
       <c r="B212" t="s">
-        <v>541</v>
+        <v>557</v>
       </c>
       <c r="D212" t="s">
         <v>8</v>
@@ -6539,83 +6574,83 @@
         <v>13</v>
       </c>
       <c r="F212" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>542</v>
+        <v>558</v>
       </c>
       <c r="B213" t="s">
-        <v>543</v>
+        <v>559</v>
       </c>
       <c r="D213" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E213" t="s">
-        <v>544</v>
+        <v>560</v>
       </c>
       <c r="F213" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>545</v>
+        <v>561</v>
       </c>
       <c r="B214" t="s">
-        <v>546</v>
+        <v>562</v>
       </c>
       <c r="D214" t="s">
         <v>8</v>
       </c>
       <c r="E214" t="s">
-        <v>547</v>
+        <v>563</v>
       </c>
       <c r="F214" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>548</v>
+        <v>564</v>
       </c>
       <c r="B215" t="s">
-        <v>549</v>
+        <v>565</v>
       </c>
       <c r="D215" t="s">
         <v>20</v>
       </c>
       <c r="E215" t="s">
-        <v>550</v>
+        <v>566</v>
       </c>
       <c r="F215" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>551</v>
+        <v>567</v>
       </c>
       <c r="B216" t="s">
-        <v>552</v>
+        <v>568</v>
       </c>
       <c r="D216" t="s">
         <v>8</v>
       </c>
       <c r="E216" t="s">
-        <v>553</v>
+        <v>569</v>
       </c>
       <c r="F216" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>554</v>
+        <v>570</v>
       </c>
       <c r="B217" t="s">
-        <v>555</v>
+        <v>571</v>
       </c>
       <c r="D217" t="s">
         <v>8</v>
@@ -6624,72 +6659,72 @@
         <v>13</v>
       </c>
       <c r="F217" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>556</v>
+        <v>572</v>
       </c>
       <c r="B218" t="s">
-        <v>557</v>
+        <v>573</v>
       </c>
       <c r="D218" t="s">
         <v>8</v>
       </c>
       <c r="E218" t="s">
-        <v>558</v>
+        <v>574</v>
       </c>
       <c r="F218" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>559</v>
+        <v>575</v>
       </c>
       <c r="B219" t="s">
-        <v>560</v>
+        <v>576</v>
       </c>
       <c r="D219" t="s">
         <v>8</v>
       </c>
       <c r="E219" t="s">
-        <v>561</v>
+        <v>577</v>
       </c>
       <c r="F219" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>562</v>
+        <v>578</v>
       </c>
       <c r="B220" t="s">
-        <v>563</v>
+        <v>579</v>
       </c>
       <c r="D220" t="s">
         <v>8</v>
       </c>
       <c r="E220" t="s">
-        <v>564</v>
+        <v>580</v>
       </c>
       <c r="F220" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>565</v>
+        <v>581</v>
       </c>
       <c r="B221" t="s">
-        <v>566</v>
+        <v>582</v>
       </c>
       <c r="D221" t="s">
         <v>8</v>
       </c>
       <c r="E221" t="s">
-        <v>567</v>
+        <v>583</v>
       </c>
       <c r="F221" t="s">
         <v>10</v>
@@ -6697,10 +6732,10 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>568</v>
+        <v>584</v>
       </c>
       <c r="B222" t="s">
-        <v>569</v>
+        <v>585</v>
       </c>
       <c r="D222" t="s">
         <v>8</v>
@@ -6714,50 +6749,50 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>570</v>
+        <v>586</v>
       </c>
       <c r="B223" t="s">
-        <v>571</v>
+        <v>587</v>
       </c>
       <c r="D223" t="s">
         <v>8</v>
       </c>
       <c r="E223" t="s">
-        <v>572</v>
+        <v>588</v>
       </c>
       <c r="F223" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>573</v>
+        <v>589</v>
       </c>
       <c r="B224" t="s">
-        <v>574</v>
+        <v>590</v>
       </c>
       <c r="D224" t="s">
         <v>8</v>
       </c>
       <c r="E224" t="s">
-        <v>575</v>
+        <v>591</v>
       </c>
       <c r="F224" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>576</v>
+        <v>592</v>
       </c>
       <c r="B225" t="s">
-        <v>577</v>
+        <v>593</v>
       </c>
       <c r="D225" t="s">
         <v>8</v>
       </c>
       <c r="E225" t="s">
-        <v>578</v>
+        <v>594</v>
       </c>
       <c r="F225" t="s">
         <v>10</v>
@@ -6765,27 +6800,27 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>579</v>
+        <v>595</v>
       </c>
       <c r="B226" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="D226" t="s">
         <v>8</v>
       </c>
       <c r="E226" t="s">
-        <v>581</v>
+        <v>597</v>
       </c>
       <c r="F226" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>582</v>
+        <v>598</v>
       </c>
       <c r="B227" t="s">
-        <v>583</v>
+        <v>599</v>
       </c>
       <c r="D227" t="s">
         <v>8</v>
@@ -6794,32 +6829,32 @@
         <v>13</v>
       </c>
       <c r="F227" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>584</v>
+        <v>600</v>
       </c>
       <c r="B228" t="s">
-        <v>585</v>
+        <v>601</v>
       </c>
       <c r="D228" t="s">
         <v>8</v>
       </c>
       <c r="E228" t="s">
-        <v>586</v>
+        <v>602</v>
       </c>
       <c r="F228" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>587</v>
+        <v>603</v>
       </c>
       <c r="B229" t="s">
-        <v>588</v>
+        <v>604</v>
       </c>
       <c r="D229" t="s">
         <v>8</v>
@@ -6828,15 +6863,15 @@
         <v>13</v>
       </c>
       <c r="F229" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>589</v>
+        <v>605</v>
       </c>
       <c r="B230" t="s">
-        <v>590</v>
+        <v>606</v>
       </c>
       <c r="D230" t="s">
         <v>8</v>
@@ -6845,49 +6880,49 @@
         <v>13</v>
       </c>
       <c r="F230" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>591</v>
+        <v>607</v>
       </c>
       <c r="B231" t="s">
-        <v>592</v>
+        <v>608</v>
       </c>
       <c r="D231" t="s">
         <v>20</v>
       </c>
       <c r="E231" t="s">
-        <v>593</v>
+        <v>609</v>
       </c>
       <c r="F231" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>594</v>
+        <v>610</v>
       </c>
       <c r="B232" t="s">
-        <v>595</v>
+        <v>611</v>
       </c>
       <c r="D232" t="s">
         <v>8</v>
       </c>
       <c r="E232" t="s">
-        <v>596</v>
+        <v>612</v>
       </c>
       <c r="F232" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>597</v>
+        <v>613</v>
       </c>
       <c r="B233" t="s">
-        <v>598</v>
+        <v>614</v>
       </c>
       <c r="D233" t="s">
         <v>8</v>
@@ -6896,143 +6931,279 @@
         <v>13</v>
       </c>
       <c r="F233" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>599</v>
+        <v>615</v>
       </c>
       <c r="B234" t="s">
-        <v>600</v>
+        <v>616</v>
       </c>
       <c r="D234" t="s">
         <v>8</v>
       </c>
       <c r="E234" t="s">
-        <v>601</v>
+        <v>617</v>
       </c>
       <c r="F234" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>602</v>
+        <v>618</v>
       </c>
       <c r="B235" t="s">
-        <v>603</v>
+        <v>619</v>
       </c>
       <c r="D235" t="s">
         <v>8</v>
       </c>
       <c r="E235" t="s">
-        <v>604</v>
+        <v>620</v>
       </c>
       <c r="F235" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>605</v>
+        <v>621</v>
       </c>
       <c r="B236" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D236" t="s">
         <v>8</v>
       </c>
       <c r="E236" t="s">
-        <v>606</v>
+        <v>622</v>
       </c>
       <c r="F236" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>607</v>
+        <v>623</v>
       </c>
       <c r="B237" t="s">
-        <v>608</v>
+        <v>624</v>
       </c>
       <c r="D237" t="s">
         <v>8</v>
       </c>
       <c r="E237" t="s">
-        <v>609</v>
+        <v>625</v>
       </c>
       <c r="F237" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>610</v>
+        <v>626</v>
       </c>
       <c r="B238" t="s">
-        <v>611</v>
+        <v>627</v>
       </c>
       <c r="D238" t="s">
         <v>8</v>
       </c>
       <c r="E238" t="s">
-        <v>612</v>
+        <v>628</v>
       </c>
       <c r="F238" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>613</v>
+        <v>629</v>
       </c>
       <c r="B239" t="s">
-        <v>614</v>
+        <v>630</v>
       </c>
       <c r="D239" t="s">
         <v>8</v>
       </c>
       <c r="E239" t="s">
-        <v>615</v>
+        <v>631</v>
       </c>
       <c r="F239" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>616</v>
+        <v>632</v>
       </c>
       <c r="B240" t="s">
-        <v>617</v>
+        <v>633</v>
       </c>
       <c r="D240" t="s">
         <v>8</v>
       </c>
       <c r="E240" t="s">
-        <v>618</v>
+        <v>634</v>
       </c>
       <c r="F240" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="B241" t="s">
-        <v>628</v>
+        <v>636</v>
       </c>
       <c r="D241" t="s">
-        <v>629</v>
+        <v>8</v>
       </c>
       <c r="E241" t="s">
-        <v>630</v>
+        <v>637</v>
       </c>
       <c r="F241" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>638</v>
+      </c>
+      <c r="B242" t="s">
+        <v>639</v>
+      </c>
+      <c r="D242" t="s">
+        <v>52</v>
+      </c>
+      <c r="E242" t="s">
+        <v>640</v>
+      </c>
+      <c r="F242" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>641</v>
+      </c>
+      <c r="B243" t="s">
+        <v>642</v>
+      </c>
+      <c r="D243" t="s">
+        <v>16</v>
+      </c>
+      <c r="E243" t="s">
+        <v>643</v>
+      </c>
+      <c r="F243" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>644</v>
+      </c>
+      <c r="B244" t="s">
+        <v>645</v>
+      </c>
+      <c r="D244" t="s">
+        <v>52</v>
+      </c>
+      <c r="E244" t="s">
+        <v>646</v>
+      </c>
+      <c r="F244" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>647</v>
+      </c>
+      <c r="B245" t="s">
+        <v>648</v>
+      </c>
+      <c r="D245" t="s">
+        <v>16</v>
+      </c>
+      <c r="E245" t="s">
+        <v>649</v>
+      </c>
+      <c r="F245" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>661</v>
+      </c>
+      <c r="B246" t="s">
+        <v>650</v>
+      </c>
+      <c r="D246" t="s">
+        <v>16</v>
+      </c>
+      <c r="E246" t="s">
+        <v>651</v>
+      </c>
+      <c r="F246" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>652</v>
+      </c>
+      <c r="B247" t="s">
+        <v>653</v>
+      </c>
+      <c r="D247" t="s">
+        <v>52</v>
+      </c>
+      <c r="E247" t="s">
+        <v>654</v>
+      </c>
+      <c r="F247" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>655</v>
+      </c>
+      <c r="B248" t="s">
+        <v>656</v>
+      </c>
+      <c r="D248" t="s">
+        <v>16</v>
+      </c>
+      <c r="E248" t="s">
+        <v>657</v>
+      </c>
+      <c r="F248" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>658</v>
+      </c>
+      <c r="B249" t="s">
+        <v>659</v>
+      </c>
+      <c r="D249" t="s">
+        <v>8</v>
+      </c>
+      <c r="E249" t="s">
+        <v>660</v>
+      </c>
+      <c r="F249" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@cc0d4d1870abbd962080f27ce9b86951edd09256 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F6BA38-D817-454F-9311-651664BF21C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465F157A-1BB7-4AF0-BF35-00D9D75DE064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="662">
   <si>
     <t>name</t>
   </si>
@@ -598,6 +598,9 @@
     <t>Wangyou Zhang</t>
   </si>
   <si>
+    <t>/assets/img/members/student/张王优.jpg</t>
+  </si>
+  <si>
     <t>杜晨鹏</t>
   </si>
   <si>
@@ -622,6 +625,9 @@
     <t>Chenda Li</t>
   </si>
   <si>
+    <t>/assets/img/members/student/李晨达.jpg</t>
+  </si>
+  <si>
     <t>卢怡宙</t>
   </si>
   <si>
@@ -772,6 +778,9 @@
     <t>Wei Wang</t>
   </si>
   <si>
+    <t>/assets/img/members/student/王巍.jpg</t>
+  </si>
+  <si>
     <t>吴章昊</t>
   </si>
   <si>
@@ -982,6 +991,9 @@
     <t>Xun Gong</t>
   </si>
   <si>
+    <t>/assets/img/members/student/龚勋.jpg</t>
+  </si>
+  <si>
     <t>兰焜耀</t>
   </si>
   <si>
@@ -1003,21 +1015,36 @@
     <t>Yuncong Liu</t>
   </si>
   <si>
+    <t>/assets/img/members/student/刘韫聪.jpg</t>
+  </si>
+  <si>
     <t>刘森</t>
   </si>
   <si>
     <t>Sen Liu</t>
   </si>
   <si>
+    <t>/assets/img/members/student/刘森.jpg</t>
+  </si>
+  <si>
     <t>李广鹏</t>
   </si>
   <si>
     <t>Guangpeng Li</t>
   </si>
   <si>
+    <t>/assets/img/members/student/李广鹏.jpg</t>
+  </si>
+  <si>
+    <t>杨宝琛</t>
+  </si>
+  <si>
     <t>Baochen Yang</t>
   </si>
   <si>
+    <t>/assets/img/members/student/杨宝琛.jpg</t>
+  </si>
+  <si>
     <t>谢泽宇</t>
   </si>
   <si>
@@ -1057,6 +1084,9 @@
     <t>Qi Chen</t>
   </si>
   <si>
+    <t>/assets/img/members/student/陈琦.jpg</t>
+  </si>
+  <si>
     <t>卢葛威</t>
   </si>
   <si>
@@ -1288,9 +1318,15 @@
     <t>/assets/img/members/student/黎井漂.jpg</t>
   </si>
   <si>
+    <t>李翰奇</t>
+  </si>
+  <si>
     <t>Hanqi Li</t>
   </si>
   <si>
+    <t>/assets/img/members/student/李翰奇.jpg</t>
+  </si>
+  <si>
     <t>孙良泰</t>
   </si>
   <si>
@@ -1420,6 +1456,9 @@
     <t>Shuai Fan</t>
   </si>
   <si>
+    <t>/assets/img/members/student/樊帅.jpg</t>
+  </si>
+  <si>
     <t>王浩然</t>
   </si>
   <si>
@@ -1447,6 +1486,9 @@
     <t>/assets/img/members/student/刘丁烨.jpg</t>
   </si>
   <si>
+    <t>/assets/img/members/student/陈博2.jpg</t>
+  </si>
+  <si>
     <t>李梓源</t>
   </si>
   <si>
@@ -1513,6 +1555,9 @@
     <t>Zhihan Li</t>
   </si>
   <si>
+    <t>/assets/img/members/student/李之涵.jpg</t>
+  </si>
+  <si>
     <t>张怡天</t>
   </si>
   <si>
@@ -1525,6 +1570,9 @@
     <t>Bohan Li</t>
   </si>
   <si>
+    <t>/assets/img/members/student/李波含.jpg</t>
+  </si>
+  <si>
     <t>曹义路</t>
   </si>
   <si>
@@ -1879,95 +1927,85 @@
     <t>/assets/img/members/student/江楠.jpg</t>
   </si>
   <si>
-    <t>李翰奇</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李翰奇.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/octocat.png</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李之涵.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李波含.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>P</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/陈博2.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>马英梓</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Yingzi Ma</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>U</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>/assets/img/members/student/马英梓.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>杨宝琛</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/刘森.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/杨宝琛.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/刘韫聪.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李广鹏.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/陈琦.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/龚勋.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/张王优.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/李晨达.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/王巍.jpg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/assets/img/members/student/樊帅.jpg</t>
+  </si>
+  <si>
+    <t>涂文明</t>
+  </si>
+  <si>
+    <t>Wenming Tu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/涂文明.jpg</t>
+  </si>
+  <si>
+    <t>梅嘉豪</t>
+  </si>
+  <si>
+    <t>Jiahao Mei</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/梅嘉豪.jpg</t>
+  </si>
+  <si>
+    <t>吴媚</t>
+  </si>
+  <si>
+    <t>WuMei</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/吴媚.jpg</t>
+  </si>
+  <si>
+    <t>王哲祥</t>
+  </si>
+  <si>
+    <t>Zhexiang Wang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/王哲祥.jpg</t>
+  </si>
+  <si>
+    <t>Chonghao Cai</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/蔡崇皓.jpg</t>
+  </si>
+  <si>
+    <t>朱轩宇</t>
+  </si>
+  <si>
+    <t>Xuanyu Zhu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/朱轩宇.jpg</t>
+  </si>
+  <si>
+    <t>陈冠豫</t>
+  </si>
+  <si>
+    <t>Guanyu Chen</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/陈冠豫.jpg</t>
+  </si>
+  <si>
+    <t>刘峻希</t>
+  </si>
+  <si>
+    <t>Junxi Liu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/刘峻希.jpg</t>
+  </si>
+  <si>
+    <t>蔡崇皓</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2339,16 +2377,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F241"/>
+  <dimension ref="A1:F249"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="E183" sqref="E183"/>
+    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
+      <selection activeCell="M231" sqref="M231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="5" max="5" width="95.08984375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3864,7 +3899,7 @@
         <v>52</v>
       </c>
       <c r="E76" t="s">
-        <v>638</v>
+        <v>192</v>
       </c>
       <c r="F76" t="s">
         <v>10</v>
@@ -3872,10 +3907,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B77" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C77">
         <v>78</v>
@@ -3884,7 +3919,7 @@
         <v>52</v>
       </c>
       <c r="E77" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F77" t="s">
         <v>10</v>
@@ -3892,10 +3927,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B78" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C78">
         <v>79</v>
@@ -3904,7 +3939,7 @@
         <v>16</v>
       </c>
       <c r="E78" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F78" t="s">
         <v>10</v>
@@ -3912,10 +3947,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B79" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C79">
         <v>80</v>
@@ -3924,7 +3959,7 @@
         <v>16</v>
       </c>
       <c r="E79" t="s">
-        <v>639</v>
+        <v>201</v>
       </c>
       <c r="F79" t="s">
         <v>10</v>
@@ -3932,10 +3967,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B80" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C80">
         <v>81</v>
@@ -3952,10 +3987,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B81" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C81">
         <v>82</v>
@@ -3972,10 +4007,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B82" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C82">
         <v>83</v>
@@ -3992,10 +4027,10 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B83" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C83">
         <v>84</v>
@@ -4004,7 +4039,7 @@
         <v>77</v>
       </c>
       <c r="E83" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F83" t="s">
         <v>10</v>
@@ -4012,10 +4047,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B84" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C84">
         <v>85</v>
@@ -4024,7 +4059,7 @@
         <v>16</v>
       </c>
       <c r="E84" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F84" t="s">
         <v>10</v>
@@ -4032,10 +4067,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B85" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C85">
         <v>86</v>
@@ -4052,10 +4087,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B86" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C86">
         <v>87</v>
@@ -4072,10 +4107,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B87" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C87">
         <v>88</v>
@@ -4092,10 +4127,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B88" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C88">
         <v>89</v>
@@ -4112,10 +4147,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B89" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C89">
         <v>90</v>
@@ -4124,7 +4159,7 @@
         <v>52</v>
       </c>
       <c r="E89" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F89" t="s">
         <v>10</v>
@@ -4132,10 +4167,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B90" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C90">
         <v>91</v>
@@ -4144,18 +4179,18 @@
         <v>52</v>
       </c>
       <c r="E90" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F90" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B91" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C91">
         <v>92</v>
@@ -4164,7 +4199,7 @@
         <v>20</v>
       </c>
       <c r="E91" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F91" t="s">
         <v>10</v>
@@ -4172,10 +4207,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B92" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C92">
         <v>93</v>
@@ -4184,7 +4219,7 @@
         <v>77</v>
       </c>
       <c r="E92" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F92" t="s">
         <v>10</v>
@@ -4192,10 +4227,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B93" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C93">
         <v>94</v>
@@ -4204,18 +4239,18 @@
         <v>77</v>
       </c>
       <c r="E93" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F93" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B94" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C94">
         <v>95</v>
@@ -4224,7 +4259,7 @@
         <v>16</v>
       </c>
       <c r="E94" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F94" t="s">
         <v>10</v>
@@ -4232,10 +4267,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B95" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C95">
         <v>96</v>
@@ -4252,10 +4287,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B96" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C96">
         <v>97</v>
@@ -4272,10 +4307,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B97" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C97">
         <v>98</v>
@@ -4284,18 +4319,18 @@
         <v>77</v>
       </c>
       <c r="E97" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="F97" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B98" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C98">
         <v>99</v>
@@ -4312,10 +4347,10 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B99" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C99">
         <v>100</v>
@@ -4324,7 +4359,7 @@
         <v>16</v>
       </c>
       <c r="E99" t="s">
-        <v>640</v>
+        <v>252</v>
       </c>
       <c r="F99" t="s">
         <v>10</v>
@@ -4332,10 +4367,10 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="B100" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C100">
         <v>101</v>
@@ -4352,10 +4387,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B101" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C101">
         <v>102</v>
@@ -4372,10 +4407,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B102" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="C102">
         <v>103</v>
@@ -4392,10 +4427,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="B103" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C103">
         <v>104</v>
@@ -4412,10 +4447,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="B104" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="C104">
         <v>105</v>
@@ -4424,7 +4459,7 @@
         <v>8</v>
       </c>
       <c r="E104" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F104" t="s">
         <v>10</v>
@@ -4432,10 +4467,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="B105" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C105">
         <v>106</v>
@@ -4444,18 +4479,18 @@
         <v>52</v>
       </c>
       <c r="E105" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F105" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="B106" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C106">
         <v>107</v>
@@ -4464,18 +4499,18 @@
         <v>52</v>
       </c>
       <c r="E106" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F106" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="B107" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C107">
         <v>108</v>
@@ -4484,7 +4519,7 @@
         <v>16</v>
       </c>
       <c r="E107" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F107" t="s">
         <v>10</v>
@@ -4492,10 +4527,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B108" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C108">
         <v>109</v>
@@ -4504,7 +4539,7 @@
         <v>77</v>
       </c>
       <c r="E108" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F108" t="s">
         <v>10</v>
@@ -4512,10 +4547,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="B109" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C109">
         <v>110</v>
@@ -4524,7 +4559,7 @@
         <v>16</v>
       </c>
       <c r="E109" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="F109" t="s">
         <v>10</v>
@@ -4532,10 +4567,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="B110" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C110">
         <v>111</v>
@@ -4544,7 +4579,7 @@
         <v>16</v>
       </c>
       <c r="E110" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="F110" t="s">
         <v>10</v>
@@ -4552,10 +4587,10 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B111" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C111">
         <v>112</v>
@@ -4564,18 +4599,18 @@
         <v>52</v>
       </c>
       <c r="E111" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="F111" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="B112" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C112">
         <v>114</v>
@@ -4592,10 +4627,10 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B113" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C113">
         <v>115</v>
@@ -4612,10 +4647,10 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="B114" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="C114">
         <v>116</v>
@@ -4632,10 +4667,10 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="B115" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="C115">
         <v>117</v>
@@ -4652,10 +4687,10 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="B116" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C116">
         <v>118</v>
@@ -4672,10 +4707,10 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="B117" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C117">
         <v>119</v>
@@ -4692,10 +4727,10 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B118" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C118">
         <v>120</v>
@@ -4712,10 +4747,10 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B119" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C119">
         <v>121</v>
@@ -4732,10 +4767,10 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="B120" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C120">
         <v>122</v>
@@ -4752,10 +4787,10 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="B121" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="C121">
         <v>123</v>
@@ -4772,10 +4807,10 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="B122" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="C122">
         <v>124</v>
@@ -4784,7 +4819,7 @@
         <v>16</v>
       </c>
       <c r="E122" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F122" t="s">
         <v>10</v>
@@ -4792,10 +4827,10 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B123" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="C123">
         <v>125</v>
@@ -4812,10 +4847,10 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B124" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="C124">
         <v>126</v>
@@ -4824,7 +4859,7 @@
         <v>16</v>
       </c>
       <c r="E124" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="F124" t="s">
         <v>10</v>
@@ -4832,10 +4867,10 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B125" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C125">
         <v>127</v>
@@ -4852,10 +4887,10 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="B126" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C126">
         <v>128</v>
@@ -4864,7 +4899,7 @@
         <v>16</v>
       </c>
       <c r="E126" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="F126" t="s">
         <v>10</v>
@@ -4872,10 +4907,10 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B127" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="C127">
         <v>129</v>
@@ -4884,18 +4919,18 @@
         <v>52</v>
       </c>
       <c r="E127" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="F127" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B128" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="C128">
         <v>130</v>
@@ -4904,7 +4939,7 @@
         <v>52</v>
       </c>
       <c r="E128" t="s">
-        <v>637</v>
+        <v>323</v>
       </c>
       <c r="F128" t="s">
         <v>10</v>
@@ -4912,10 +4947,10 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B129" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C129">
         <v>131</v>
@@ -4924,18 +4959,18 @@
         <v>77</v>
       </c>
       <c r="E129" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="F129" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="B130" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C130">
         <v>132</v>
@@ -4952,10 +4987,10 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B131" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C131">
         <v>133</v>
@@ -4964,7 +4999,7 @@
         <v>52</v>
       </c>
       <c r="E131" t="s">
-        <v>634</v>
+        <v>331</v>
       </c>
       <c r="F131" t="s">
         <v>10</v>
@@ -4972,10 +5007,10 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="B132" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="C132">
         <v>134</v>
@@ -4984,7 +5019,7 @@
         <v>16</v>
       </c>
       <c r="E132" t="s">
-        <v>632</v>
+        <v>334</v>
       </c>
       <c r="F132" t="s">
         <v>10</v>
@@ -4992,10 +5027,10 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B133" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="C133">
         <v>135</v>
@@ -5004,7 +5039,7 @@
         <v>16</v>
       </c>
       <c r="E133" t="s">
-        <v>635</v>
+        <v>337</v>
       </c>
       <c r="F133" t="s">
         <v>10</v>
@@ -5012,10 +5047,10 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>631</v>
+        <v>338</v>
       </c>
       <c r="B134" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="C134">
         <v>136</v>
@@ -5024,7 +5059,7 @@
         <v>16</v>
       </c>
       <c r="E134" t="s">
-        <v>633</v>
+        <v>340</v>
       </c>
       <c r="F134" t="s">
         <v>10</v>
@@ -5032,10 +5067,10 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="B135" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="C135">
         <v>138</v>
@@ -5044,7 +5079,7 @@
         <v>20</v>
       </c>
       <c r="E135" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="F135" t="s">
         <v>10</v>
@@ -5052,10 +5087,10 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="B136" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="C136">
         <v>139</v>
@@ -5064,18 +5099,18 @@
         <v>16</v>
       </c>
       <c r="E136" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="F136" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="B137" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="C137">
         <v>140</v>
@@ -5084,18 +5119,18 @@
         <v>52</v>
       </c>
       <c r="E137" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="F137" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="B138" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="C138">
         <v>141</v>
@@ -5107,35 +5142,35 @@
         <v>13</v>
       </c>
       <c r="F138" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="B139" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="C139">
         <v>142</v>
       </c>
       <c r="D139" t="s">
-        <v>621</v>
+        <v>42</v>
       </c>
       <c r="E139" t="s">
-        <v>636</v>
+        <v>354</v>
       </c>
       <c r="F139" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="B140" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="C140">
         <v>143</v>
@@ -5144,18 +5179,18 @@
         <v>16</v>
       </c>
       <c r="E140" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="F140" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="B141" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="C141">
         <v>144</v>
@@ -5164,18 +5199,18 @@
         <v>20</v>
       </c>
       <c r="E141" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="F141" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="B142" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="C142">
         <v>145</v>
@@ -5184,18 +5219,18 @@
         <v>52</v>
       </c>
       <c r="E142" t="s">
-        <v>353</v>
+        <v>363</v>
       </c>
       <c r="F142" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="B143" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="C143">
         <v>146</v>
@@ -5204,18 +5239,18 @@
         <v>42</v>
       </c>
       <c r="E143" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="F143" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="B144" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="C144">
         <v>147</v>
@@ -5224,18 +5259,18 @@
         <v>52</v>
       </c>
       <c r="E144" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="F144" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="B145" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="C145">
         <v>148</v>
@@ -5244,18 +5279,18 @@
         <v>16</v>
       </c>
       <c r="E145" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="F145" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="B146" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="C146">
         <v>149</v>
@@ -5264,7 +5299,7 @@
         <v>16</v>
       </c>
       <c r="E146" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
       <c r="F146" t="s">
         <v>10</v>
@@ -5272,10 +5307,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="B147" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="C147">
         <v>150</v>
@@ -5284,18 +5319,18 @@
         <v>52</v>
       </c>
       <c r="E147" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="F147" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="B148" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="C148">
         <v>151</v>
@@ -5304,18 +5339,18 @@
         <v>52</v>
       </c>
       <c r="E148" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="F148" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="B149" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="C149">
         <v>152</v>
@@ -5327,35 +5362,35 @@
         <v>13</v>
       </c>
       <c r="F149" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="B150" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="C150">
         <v>153</v>
       </c>
       <c r="D150" t="s">
-        <v>625</v>
+        <v>52</v>
       </c>
       <c r="E150" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="F150" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="B151" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="C151">
         <v>154</v>
@@ -5364,7 +5399,7 @@
         <v>16</v>
       </c>
       <c r="E151" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="F151" t="s">
         <v>10</v>
@@ -5372,10 +5407,10 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="B152" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="C152">
         <v>155</v>
@@ -5384,7 +5419,7 @@
         <v>16</v>
       </c>
       <c r="E152" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="F152" t="s">
         <v>10</v>
@@ -5392,10 +5427,10 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="B153" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C153">
         <v>156</v>
@@ -5404,18 +5439,18 @@
         <v>16</v>
       </c>
       <c r="E153" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="F153" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="B154" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="C154">
         <v>157</v>
@@ -5424,18 +5459,18 @@
         <v>8</v>
       </c>
       <c r="E154" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
       <c r="F154" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="B155" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="C155">
         <v>158</v>
@@ -5444,18 +5479,18 @@
         <v>52</v>
       </c>
       <c r="E155" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="F155" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="B156" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
       <c r="C156">
         <v>159</v>
@@ -5464,18 +5499,18 @@
         <v>16</v>
       </c>
       <c r="E156" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="F156" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
       <c r="B157" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="C157">
         <v>160</v>
@@ -5484,18 +5519,18 @@
         <v>52</v>
       </c>
       <c r="E157" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="F157" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="B158" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
       <c r="C158">
         <v>161</v>
@@ -5504,18 +5539,18 @@
         <v>16</v>
       </c>
       <c r="E158" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="F158" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="B159" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="C159">
         <v>162</v>
@@ -5524,18 +5559,18 @@
         <v>16</v>
       </c>
       <c r="E159" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="F159" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>404</v>
+        <v>414</v>
       </c>
       <c r="B160" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="C160">
         <v>163</v>
@@ -5544,18 +5579,18 @@
         <v>16</v>
       </c>
       <c r="E160" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
       <c r="F160" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="B161" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
       <c r="C161">
         <v>164</v>
@@ -5564,18 +5599,18 @@
         <v>52</v>
       </c>
       <c r="E161" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="F161" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="B162" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="C162">
         <v>165</v>
@@ -5584,7 +5619,7 @@
         <v>16</v>
       </c>
       <c r="E162" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="F162" t="s">
         <v>10</v>
@@ -5592,10 +5627,10 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="B163" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="C163">
         <v>166</v>
@@ -5604,18 +5639,18 @@
         <v>52</v>
       </c>
       <c r="E163" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
       <c r="F163" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="B164" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="C164">
         <v>167</v>
@@ -5624,18 +5659,18 @@
         <v>16</v>
       </c>
       <c r="E164" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="F164" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>419</v>
+        <v>429</v>
       </c>
       <c r="B165" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="C165">
         <v>168</v>
@@ -5644,7 +5679,7 @@
         <v>16</v>
       </c>
       <c r="E165" t="s">
-        <v>421</v>
+        <v>431</v>
       </c>
       <c r="F165" t="s">
         <v>10</v>
@@ -5652,30 +5687,30 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>619</v>
+        <v>432</v>
       </c>
       <c r="B166" t="s">
-        <v>422</v>
+        <v>433</v>
       </c>
       <c r="C166">
         <v>169</v>
       </c>
       <c r="D166" t="s">
-        <v>621</v>
+        <v>42</v>
       </c>
       <c r="E166" t="s">
-        <v>620</v>
+        <v>434</v>
       </c>
       <c r="F166" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>423</v>
+        <v>435</v>
       </c>
       <c r="B167" t="s">
-        <v>424</v>
+        <v>436</v>
       </c>
       <c r="C167">
         <v>170</v>
@@ -5684,7 +5719,7 @@
         <v>16</v>
       </c>
       <c r="E167" t="s">
-        <v>425</v>
+        <v>437</v>
       </c>
       <c r="F167" t="s">
         <v>10</v>
@@ -5692,10 +5727,10 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>426</v>
+        <v>438</v>
       </c>
       <c r="B168" t="s">
-        <v>427</v>
+        <v>439</v>
       </c>
       <c r="C168">
         <v>171</v>
@@ -5704,18 +5739,18 @@
         <v>52</v>
       </c>
       <c r="E168" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="F168" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>429</v>
+        <v>441</v>
       </c>
       <c r="B169" t="s">
-        <v>430</v>
+        <v>442</v>
       </c>
       <c r="C169">
         <v>172</v>
@@ -5724,7 +5759,7 @@
         <v>16</v>
       </c>
       <c r="E169" t="s">
-        <v>431</v>
+        <v>443</v>
       </c>
       <c r="F169" t="s">
         <v>10</v>
@@ -5732,10 +5767,10 @@
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>432</v>
+        <v>444</v>
       </c>
       <c r="B170" t="s">
-        <v>433</v>
+        <v>445</v>
       </c>
       <c r="C170">
         <v>173</v>
@@ -5744,18 +5779,18 @@
         <v>16</v>
       </c>
       <c r="E170" t="s">
-        <v>434</v>
+        <v>446</v>
       </c>
       <c r="F170" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="B171" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="C171">
         <v>174</v>
@@ -5767,15 +5802,15 @@
         <v>13</v>
       </c>
       <c r="F171" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="B172" t="s">
-        <v>438</v>
+        <v>450</v>
       </c>
       <c r="C172">
         <v>175</v>
@@ -5784,18 +5819,18 @@
         <v>16</v>
       </c>
       <c r="E172" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
       <c r="F172" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>440</v>
+        <v>452</v>
       </c>
       <c r="B173" t="s">
-        <v>441</v>
+        <v>453</v>
       </c>
       <c r="C173">
         <v>176</v>
@@ -5804,7 +5839,7 @@
         <v>16</v>
       </c>
       <c r="E173" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="F173" t="s">
         <v>10</v>
@@ -5812,10 +5847,10 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>443</v>
+        <v>455</v>
       </c>
       <c r="B174" t="s">
-        <v>444</v>
+        <v>456</v>
       </c>
       <c r="C174">
         <v>177</v>
@@ -5824,18 +5859,18 @@
         <v>42</v>
       </c>
       <c r="E174" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="F174" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="B175" t="s">
-        <v>447</v>
+        <v>459</v>
       </c>
       <c r="C175">
         <v>178</v>
@@ -5847,15 +5882,15 @@
         <v>13</v>
       </c>
       <c r="F175" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>448</v>
+        <v>460</v>
       </c>
       <c r="B176" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="C176">
         <v>179</v>
@@ -5864,7 +5899,7 @@
         <v>16</v>
       </c>
       <c r="E176" t="s">
-        <v>450</v>
+        <v>462</v>
       </c>
       <c r="F176" t="s">
         <v>10</v>
@@ -5872,10 +5907,10 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>451</v>
+        <v>463</v>
       </c>
       <c r="B177" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
       <c r="C177">
         <v>180</v>
@@ -5892,10 +5927,10 @@
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="B178" t="s">
-        <v>454</v>
+        <v>466</v>
       </c>
       <c r="C178">
         <v>181</v>
@@ -5912,10 +5947,10 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>455</v>
+        <v>467</v>
       </c>
       <c r="B179" t="s">
-        <v>456</v>
+        <v>468</v>
       </c>
       <c r="C179">
         <v>182</v>
@@ -5924,7 +5959,7 @@
         <v>16</v>
       </c>
       <c r="E179" t="s">
-        <v>457</v>
+        <v>469</v>
       </c>
       <c r="F179" t="s">
         <v>10</v>
@@ -5932,10 +5967,10 @@
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>458</v>
+        <v>470</v>
       </c>
       <c r="B180" t="s">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="C180">
         <v>183</v>
@@ -5944,18 +5979,18 @@
         <v>52</v>
       </c>
       <c r="E180" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="F180" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>461</v>
+        <v>473</v>
       </c>
       <c r="B181" t="s">
-        <v>462</v>
+        <v>474</v>
       </c>
       <c r="C181">
         <v>184</v>
@@ -5964,7 +5999,7 @@
         <v>42</v>
       </c>
       <c r="E181" t="s">
-        <v>463</v>
+        <v>475</v>
       </c>
       <c r="F181" t="s">
         <v>10</v>
@@ -5972,10 +6007,10 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="B182" t="s">
-        <v>465</v>
+        <v>477</v>
       </c>
       <c r="C182">
         <v>185</v>
@@ -5984,18 +6019,18 @@
         <v>36</v>
       </c>
       <c r="E182" t="s">
-        <v>641</v>
+        <v>478</v>
       </c>
       <c r="F182" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>466</v>
+        <v>479</v>
       </c>
       <c r="B183" t="s">
-        <v>467</v>
+        <v>480</v>
       </c>
       <c r="C183">
         <v>186</v>
@@ -6004,18 +6039,18 @@
         <v>20</v>
       </c>
       <c r="E183" t="s">
-        <v>468</v>
+        <v>481</v>
       </c>
       <c r="F183" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>469</v>
+        <v>482</v>
       </c>
       <c r="B184" t="s">
-        <v>470</v>
+        <v>483</v>
       </c>
       <c r="C184">
         <v>187</v>
@@ -6024,18 +6059,18 @@
         <v>16</v>
       </c>
       <c r="E184" t="s">
-        <v>471</v>
+        <v>484</v>
       </c>
       <c r="F184" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>472</v>
+        <v>485</v>
       </c>
       <c r="B185" t="s">
-        <v>473</v>
+        <v>486</v>
       </c>
       <c r="C185">
         <v>189</v>
@@ -6044,10 +6079,10 @@
         <v>16</v>
       </c>
       <c r="E185" t="s">
-        <v>474</v>
+        <v>487</v>
       </c>
       <c r="F185" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -6061,10 +6096,10 @@
         <v>190</v>
       </c>
       <c r="D186" t="s">
-        <v>625</v>
+        <v>52</v>
       </c>
       <c r="E186" t="s">
-        <v>626</v>
+        <v>488</v>
       </c>
       <c r="F186" t="s">
         <v>10</v>
@@ -6072,10 +6107,10 @@
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>475</v>
+        <v>489</v>
       </c>
       <c r="B187" t="s">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="C187">
         <v>191</v>
@@ -6084,7 +6119,7 @@
         <v>8</v>
       </c>
       <c r="E187" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="F187" t="s">
         <v>10</v>
@@ -6092,10 +6127,10 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>478</v>
+        <v>492</v>
       </c>
       <c r="B188" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="C188">
         <v>192</v>
@@ -6104,18 +6139,18 @@
         <v>8</v>
       </c>
       <c r="E188" t="s">
-        <v>480</v>
+        <v>494</v>
       </c>
       <c r="F188" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="B189" t="s">
-        <v>482</v>
+        <v>496</v>
       </c>
       <c r="C189">
         <v>193</v>
@@ -6124,18 +6159,18 @@
         <v>8</v>
       </c>
       <c r="E189" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="F189" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>484</v>
+        <v>498</v>
       </c>
       <c r="B190" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="C190">
         <v>194</v>
@@ -6144,18 +6179,18 @@
         <v>8</v>
       </c>
       <c r="E190" t="s">
-        <v>486</v>
+        <v>500</v>
       </c>
       <c r="F190" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="B191" t="s">
-        <v>488</v>
+        <v>502</v>
       </c>
       <c r="C191">
         <v>195</v>
@@ -6164,18 +6199,18 @@
         <v>8</v>
       </c>
       <c r="E191" t="s">
-        <v>489</v>
+        <v>503</v>
       </c>
       <c r="F191" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>490</v>
+        <v>504</v>
       </c>
       <c r="B192" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="C192">
         <v>196</v>
@@ -6187,15 +6222,15 @@
         <v>13</v>
       </c>
       <c r="F192" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>492</v>
+        <v>506</v>
       </c>
       <c r="B193" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="C193">
         <v>197</v>
@@ -6204,18 +6239,18 @@
         <v>20</v>
       </c>
       <c r="E193" t="s">
-        <v>494</v>
+        <v>508</v>
       </c>
       <c r="F193" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="B194" t="s">
-        <v>496</v>
+        <v>510</v>
       </c>
       <c r="C194">
         <v>198</v>
@@ -6224,18 +6259,18 @@
         <v>16</v>
       </c>
       <c r="E194" t="s">
-        <v>623</v>
+        <v>511</v>
       </c>
       <c r="F194" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>497</v>
+        <v>512</v>
       </c>
       <c r="B195" t="s">
-        <v>498</v>
+        <v>513</v>
       </c>
       <c r="C195">
         <v>199</v>
@@ -6244,7 +6279,7 @@
         <v>16</v>
       </c>
       <c r="E195" t="s">
-        <v>622</v>
+        <v>13</v>
       </c>
       <c r="F195" t="s">
         <v>10</v>
@@ -6252,10 +6287,10 @@
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>499</v>
+        <v>514</v>
       </c>
       <c r="B196" t="s">
-        <v>500</v>
+        <v>515</v>
       </c>
       <c r="C196">
         <v>200</v>
@@ -6264,35 +6299,35 @@
         <v>42</v>
       </c>
       <c r="E196" t="s">
-        <v>624</v>
+        <v>516</v>
       </c>
       <c r="F196" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>501</v>
+        <v>517</v>
       </c>
       <c r="B197" t="s">
-        <v>502</v>
+        <v>518</v>
       </c>
       <c r="D197" t="s">
         <v>8</v>
       </c>
       <c r="E197" t="s">
-        <v>503</v>
+        <v>519</v>
       </c>
       <c r="F197" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>504</v>
+        <v>520</v>
       </c>
       <c r="B198" t="s">
-        <v>505</v>
+        <v>521</v>
       </c>
       <c r="D198" t="s">
         <v>8</v>
@@ -6301,66 +6336,66 @@
         <v>13</v>
       </c>
       <c r="F198" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>506</v>
+        <v>522</v>
       </c>
       <c r="B199" t="s">
-        <v>507</v>
+        <v>523</v>
       </c>
       <c r="D199" t="s">
         <v>8</v>
       </c>
       <c r="E199" t="s">
-        <v>508</v>
+        <v>524</v>
       </c>
       <c r="F199" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>509</v>
+        <v>525</v>
       </c>
       <c r="B200" t="s">
-        <v>510</v>
+        <v>526</v>
       </c>
       <c r="D200" t="s">
         <v>8</v>
       </c>
       <c r="E200" t="s">
-        <v>511</v>
+        <v>527</v>
       </c>
       <c r="F200" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="B201" t="s">
-        <v>513</v>
+        <v>529</v>
       </c>
       <c r="D201" t="s">
         <v>77</v>
       </c>
       <c r="E201" t="s">
-        <v>514</v>
+        <v>530</v>
       </c>
       <c r="F201" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>515</v>
+        <v>531</v>
       </c>
       <c r="B202" t="s">
-        <v>516</v>
+        <v>532</v>
       </c>
       <c r="D202" t="s">
         <v>8</v>
@@ -6369,66 +6404,66 @@
         <v>13</v>
       </c>
       <c r="F202" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>517</v>
+        <v>533</v>
       </c>
       <c r="B203" t="s">
-        <v>518</v>
+        <v>534</v>
       </c>
       <c r="D203" t="s">
         <v>8</v>
       </c>
       <c r="E203" t="s">
-        <v>519</v>
+        <v>535</v>
       </c>
       <c r="F203" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>520</v>
+        <v>536</v>
       </c>
       <c r="B204" t="s">
-        <v>521</v>
+        <v>537</v>
       </c>
       <c r="D204" t="s">
         <v>8</v>
       </c>
       <c r="E204" t="s">
-        <v>522</v>
+        <v>538</v>
       </c>
       <c r="F204" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>523</v>
+        <v>539</v>
       </c>
       <c r="B205" t="s">
-        <v>524</v>
+        <v>540</v>
       </c>
       <c r="D205" t="s">
         <v>8</v>
       </c>
       <c r="E205" t="s">
-        <v>525</v>
+        <v>541</v>
       </c>
       <c r="F205" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>526</v>
+        <v>542</v>
       </c>
       <c r="B206" t="s">
-        <v>527</v>
+        <v>543</v>
       </c>
       <c r="D206" t="s">
         <v>16</v>
@@ -6437,32 +6472,32 @@
         <v>13</v>
       </c>
       <c r="F206" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>528</v>
+        <v>544</v>
       </c>
       <c r="B207" t="s">
-        <v>529</v>
+        <v>545</v>
       </c>
       <c r="D207" t="s">
         <v>8</v>
       </c>
       <c r="E207" t="s">
-        <v>530</v>
+        <v>546</v>
       </c>
       <c r="F207" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>531</v>
+        <v>547</v>
       </c>
       <c r="B208" t="s">
-        <v>532</v>
+        <v>548</v>
       </c>
       <c r="D208" t="s">
         <v>8</v>
@@ -6471,15 +6506,15 @@
         <v>13</v>
       </c>
       <c r="F208" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>533</v>
+        <v>549</v>
       </c>
       <c r="B209" t="s">
-        <v>534</v>
+        <v>550</v>
       </c>
       <c r="D209" t="s">
         <v>8</v>
@@ -6488,32 +6523,32 @@
         <v>13</v>
       </c>
       <c r="F209" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>535</v>
+        <v>551</v>
       </c>
       <c r="B210" t="s">
-        <v>536</v>
+        <v>552</v>
       </c>
       <c r="D210" t="s">
         <v>8</v>
       </c>
       <c r="E210" t="s">
-        <v>537</v>
+        <v>553</v>
       </c>
       <c r="F210" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>538</v>
+        <v>554</v>
       </c>
       <c r="B211" t="s">
-        <v>539</v>
+        <v>555</v>
       </c>
       <c r="D211" t="s">
         <v>8</v>
@@ -6522,15 +6557,15 @@
         <v>13</v>
       </c>
       <c r="F211" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>540</v>
+        <v>556</v>
       </c>
       <c r="B212" t="s">
-        <v>541</v>
+        <v>557</v>
       </c>
       <c r="D212" t="s">
         <v>8</v>
@@ -6539,83 +6574,83 @@
         <v>13</v>
       </c>
       <c r="F212" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>542</v>
+        <v>558</v>
       </c>
       <c r="B213" t="s">
-        <v>543</v>
+        <v>559</v>
       </c>
       <c r="D213" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E213" t="s">
-        <v>544</v>
+        <v>560</v>
       </c>
       <c r="F213" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>545</v>
+        <v>561</v>
       </c>
       <c r="B214" t="s">
-        <v>546</v>
+        <v>562</v>
       </c>
       <c r="D214" t="s">
         <v>8</v>
       </c>
       <c r="E214" t="s">
-        <v>547</v>
+        <v>563</v>
       </c>
       <c r="F214" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>548</v>
+        <v>564</v>
       </c>
       <c r="B215" t="s">
-        <v>549</v>
+        <v>565</v>
       </c>
       <c r="D215" t="s">
         <v>20</v>
       </c>
       <c r="E215" t="s">
-        <v>550</v>
+        <v>566</v>
       </c>
       <c r="F215" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>551</v>
+        <v>567</v>
       </c>
       <c r="B216" t="s">
-        <v>552</v>
+        <v>568</v>
       </c>
       <c r="D216" t="s">
         <v>8</v>
       </c>
       <c r="E216" t="s">
-        <v>553</v>
+        <v>569</v>
       </c>
       <c r="F216" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>554</v>
+        <v>570</v>
       </c>
       <c r="B217" t="s">
-        <v>555</v>
+        <v>571</v>
       </c>
       <c r="D217" t="s">
         <v>8</v>
@@ -6624,72 +6659,72 @@
         <v>13</v>
       </c>
       <c r="F217" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>556</v>
+        <v>572</v>
       </c>
       <c r="B218" t="s">
-        <v>557</v>
+        <v>573</v>
       </c>
       <c r="D218" t="s">
         <v>8</v>
       </c>
       <c r="E218" t="s">
-        <v>558</v>
+        <v>574</v>
       </c>
       <c r="F218" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>559</v>
+        <v>575</v>
       </c>
       <c r="B219" t="s">
-        <v>560</v>
+        <v>576</v>
       </c>
       <c r="D219" t="s">
         <v>8</v>
       </c>
       <c r="E219" t="s">
-        <v>561</v>
+        <v>577</v>
       </c>
       <c r="F219" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>562</v>
+        <v>578</v>
       </c>
       <c r="B220" t="s">
-        <v>563</v>
+        <v>579</v>
       </c>
       <c r="D220" t="s">
         <v>8</v>
       </c>
       <c r="E220" t="s">
-        <v>564</v>
+        <v>580</v>
       </c>
       <c r="F220" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>565</v>
+        <v>581</v>
       </c>
       <c r="B221" t="s">
-        <v>566</v>
+        <v>582</v>
       </c>
       <c r="D221" t="s">
         <v>8</v>
       </c>
       <c r="E221" t="s">
-        <v>567</v>
+        <v>583</v>
       </c>
       <c r="F221" t="s">
         <v>10</v>
@@ -6697,10 +6732,10 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>568</v>
+        <v>584</v>
       </c>
       <c r="B222" t="s">
-        <v>569</v>
+        <v>585</v>
       </c>
       <c r="D222" t="s">
         <v>8</v>
@@ -6714,50 +6749,50 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>570</v>
+        <v>586</v>
       </c>
       <c r="B223" t="s">
-        <v>571</v>
+        <v>587</v>
       </c>
       <c r="D223" t="s">
         <v>8</v>
       </c>
       <c r="E223" t="s">
-        <v>572</v>
+        <v>588</v>
       </c>
       <c r="F223" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>573</v>
+        <v>589</v>
       </c>
       <c r="B224" t="s">
-        <v>574</v>
+        <v>590</v>
       </c>
       <c r="D224" t="s">
         <v>8</v>
       </c>
       <c r="E224" t="s">
-        <v>575</v>
+        <v>591</v>
       </c>
       <c r="F224" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>576</v>
+        <v>592</v>
       </c>
       <c r="B225" t="s">
-        <v>577</v>
+        <v>593</v>
       </c>
       <c r="D225" t="s">
         <v>8</v>
       </c>
       <c r="E225" t="s">
-        <v>578</v>
+        <v>594</v>
       </c>
       <c r="F225" t="s">
         <v>10</v>
@@ -6765,27 +6800,27 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>579</v>
+        <v>595</v>
       </c>
       <c r="B226" t="s">
-        <v>580</v>
+        <v>596</v>
       </c>
       <c r="D226" t="s">
         <v>8</v>
       </c>
       <c r="E226" t="s">
-        <v>581</v>
+        <v>597</v>
       </c>
       <c r="F226" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>582</v>
+        <v>598</v>
       </c>
       <c r="B227" t="s">
-        <v>583</v>
+        <v>599</v>
       </c>
       <c r="D227" t="s">
         <v>8</v>
@@ -6794,32 +6829,32 @@
         <v>13</v>
       </c>
       <c r="F227" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>584</v>
+        <v>600</v>
       </c>
       <c r="B228" t="s">
-        <v>585</v>
+        <v>601</v>
       </c>
       <c r="D228" t="s">
         <v>8</v>
       </c>
       <c r="E228" t="s">
-        <v>586</v>
+        <v>602</v>
       </c>
       <c r="F228" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>587</v>
+        <v>603</v>
       </c>
       <c r="B229" t="s">
-        <v>588</v>
+        <v>604</v>
       </c>
       <c r="D229" t="s">
         <v>8</v>
@@ -6828,15 +6863,15 @@
         <v>13</v>
       </c>
       <c r="F229" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>589</v>
+        <v>605</v>
       </c>
       <c r="B230" t="s">
-        <v>590</v>
+        <v>606</v>
       </c>
       <c r="D230" t="s">
         <v>8</v>
@@ -6845,49 +6880,49 @@
         <v>13</v>
       </c>
       <c r="F230" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>591</v>
+        <v>607</v>
       </c>
       <c r="B231" t="s">
-        <v>592</v>
+        <v>608</v>
       </c>
       <c r="D231" t="s">
         <v>20</v>
       </c>
       <c r="E231" t="s">
-        <v>593</v>
+        <v>609</v>
       </c>
       <c r="F231" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>594</v>
+        <v>610</v>
       </c>
       <c r="B232" t="s">
-        <v>595</v>
+        <v>611</v>
       </c>
       <c r="D232" t="s">
         <v>8</v>
       </c>
       <c r="E232" t="s">
-        <v>596</v>
+        <v>612</v>
       </c>
       <c r="F232" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>597</v>
+        <v>613</v>
       </c>
       <c r="B233" t="s">
-        <v>598</v>
+        <v>614</v>
       </c>
       <c r="D233" t="s">
         <v>8</v>
@@ -6896,143 +6931,279 @@
         <v>13</v>
       </c>
       <c r="F233" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>599</v>
+        <v>615</v>
       </c>
       <c r="B234" t="s">
-        <v>600</v>
+        <v>616</v>
       </c>
       <c r="D234" t="s">
         <v>8</v>
       </c>
       <c r="E234" t="s">
-        <v>601</v>
+        <v>617</v>
       </c>
       <c r="F234" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>602</v>
+        <v>618</v>
       </c>
       <c r="B235" t="s">
-        <v>603</v>
+        <v>619</v>
       </c>
       <c r="D235" t="s">
         <v>8</v>
       </c>
       <c r="E235" t="s">
-        <v>604</v>
+        <v>620</v>
       </c>
       <c r="F235" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>605</v>
+        <v>621</v>
       </c>
       <c r="B236" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D236" t="s">
         <v>8</v>
       </c>
       <c r="E236" t="s">
-        <v>606</v>
+        <v>622</v>
       </c>
       <c r="F236" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>607</v>
+        <v>623</v>
       </c>
       <c r="B237" t="s">
-        <v>608</v>
+        <v>624</v>
       </c>
       <c r="D237" t="s">
         <v>8</v>
       </c>
       <c r="E237" t="s">
-        <v>609</v>
+        <v>625</v>
       </c>
       <c r="F237" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>610</v>
+        <v>626</v>
       </c>
       <c r="B238" t="s">
-        <v>611</v>
+        <v>627</v>
       </c>
       <c r="D238" t="s">
         <v>8</v>
       </c>
       <c r="E238" t="s">
-        <v>612</v>
+        <v>628</v>
       </c>
       <c r="F238" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>613</v>
+        <v>629</v>
       </c>
       <c r="B239" t="s">
-        <v>614</v>
+        <v>630</v>
       </c>
       <c r="D239" t="s">
         <v>8</v>
       </c>
       <c r="E239" t="s">
-        <v>615</v>
+        <v>631</v>
       </c>
       <c r="F239" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>616</v>
+        <v>632</v>
       </c>
       <c r="B240" t="s">
-        <v>617</v>
+        <v>633</v>
       </c>
       <c r="D240" t="s">
         <v>8</v>
       </c>
       <c r="E240" t="s">
-        <v>618</v>
+        <v>634</v>
       </c>
       <c r="F240" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>627</v>
+        <v>635</v>
       </c>
       <c r="B241" t="s">
-        <v>628</v>
+        <v>636</v>
       </c>
       <c r="D241" t="s">
-        <v>629</v>
+        <v>8</v>
       </c>
       <c r="E241" t="s">
-        <v>630</v>
+        <v>637</v>
       </c>
       <c r="F241" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>638</v>
+      </c>
+      <c r="B242" t="s">
+        <v>639</v>
+      </c>
+      <c r="D242" t="s">
+        <v>52</v>
+      </c>
+      <c r="E242" t="s">
+        <v>640</v>
+      </c>
+      <c r="F242" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>641</v>
+      </c>
+      <c r="B243" t="s">
+        <v>642</v>
+      </c>
+      <c r="D243" t="s">
+        <v>16</v>
+      </c>
+      <c r="E243" t="s">
+        <v>643</v>
+      </c>
+      <c r="F243" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>644</v>
+      </c>
+      <c r="B244" t="s">
+        <v>645</v>
+      </c>
+      <c r="D244" t="s">
+        <v>52</v>
+      </c>
+      <c r="E244" t="s">
+        <v>646</v>
+      </c>
+      <c r="F244" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>647</v>
+      </c>
+      <c r="B245" t="s">
+        <v>648</v>
+      </c>
+      <c r="D245" t="s">
+        <v>16</v>
+      </c>
+      <c r="E245" t="s">
+        <v>649</v>
+      </c>
+      <c r="F245" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>661</v>
+      </c>
+      <c r="B246" t="s">
+        <v>650</v>
+      </c>
+      <c r="D246" t="s">
+        <v>16</v>
+      </c>
+      <c r="E246" t="s">
+        <v>651</v>
+      </c>
+      <c r="F246" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>652</v>
+      </c>
+      <c r="B247" t="s">
+        <v>653</v>
+      </c>
+      <c r="D247" t="s">
+        <v>52</v>
+      </c>
+      <c r="E247" t="s">
+        <v>654</v>
+      </c>
+      <c r="F247" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>655</v>
+      </c>
+      <c r="B248" t="s">
+        <v>656</v>
+      </c>
+      <c r="D248" t="s">
+        <v>16</v>
+      </c>
+      <c r="E248" t="s">
+        <v>657</v>
+      </c>
+      <c r="F248" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>658</v>
+      </c>
+      <c r="B249" t="s">
+        <v>659</v>
+      </c>
+      <c r="D249" t="s">
+        <v>8</v>
+      </c>
+      <c r="E249" t="s">
+        <v>660</v>
+      </c>
+      <c r="F249" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: 1. new members 2. update group photo
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465F157A-1BB7-4AF0-BF35-00D9D75DE064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C60FA30-4F1D-4CB4-A209-36FE1C679EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="738">
   <si>
     <t>name</t>
   </si>
@@ -1690,6 +1693,9 @@
     <t>Yuzhe Liang</t>
   </si>
   <si>
+    <t>/assets/img/members/student/梁宇哲.jpg</t>
+  </si>
+  <si>
     <t>刘轩丞</t>
   </si>
   <si>
@@ -1957,7 +1963,7 @@
     <t>吴媚</t>
   </si>
   <si>
-    <t>WuMei</t>
+    <t>Mei Wu</t>
   </si>
   <si>
     <t>/assets/img/members/student/吴媚.jpg</t>
@@ -1972,6 +1978,9 @@
     <t>/assets/img/members/student/王哲祥.jpg</t>
   </si>
   <si>
+    <t>蔡崇皓</t>
+  </si>
+  <si>
     <t>Chonghao Cai</t>
   </si>
   <si>
@@ -1981,7 +1990,7 @@
     <t>朱轩宇</t>
   </si>
   <si>
-    <t>Xuanyu Zhu</t>
+    <t>Zhu Xuanyu</t>
   </si>
   <si>
     <t>/assets/img/members/student/朱轩宇.jpg</t>
@@ -2005,7 +2014,235 @@
     <t>/assets/img/members/student/刘峻希.jpg</t>
   </si>
   <si>
-    <t>蔡崇皓</t>
+    <t>孙文杰</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wenjie Sun </t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/孙文杰.jpg</t>
+  </si>
+  <si>
+    <t>刘展勋</t>
+  </si>
+  <si>
+    <t>Zhanxun Liu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/刘展勋.jpg</t>
+  </si>
+  <si>
+    <t>李师萌</t>
+  </si>
+  <si>
+    <t>Shimeng Li</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/李师萌.jpg</t>
+  </si>
+  <si>
+    <t>韩晨烨</t>
+  </si>
+  <si>
+    <t>Chenye Han</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/韩晨烨.jpg</t>
+  </si>
+  <si>
+    <t>涂宇清</t>
+  </si>
+  <si>
+    <t>Yuqing Tu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/涂宇清.jpg</t>
+  </si>
+  <si>
+    <t>张锦维</t>
+  </si>
+  <si>
+    <t>Jinwei Zhang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/张锦维.jpg</t>
+  </si>
+  <si>
+    <t>黄文宾</t>
+  </si>
+  <si>
+    <t>Wenbin Huang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/黄文宾.jpg</t>
+  </si>
+  <si>
+    <t>徐世奇</t>
+  </si>
+  <si>
+    <t>Shiqi Xu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/徐世奇.jpg</t>
+  </si>
+  <si>
+    <t>尹志强</t>
+  </si>
+  <si>
+    <t>zhiqiangyin</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/尹志强.jpg</t>
+  </si>
+  <si>
+    <t>张书畅</t>
+  </si>
+  <si>
+    <t>Shuchang Zhang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/张书畅.jpg</t>
+  </si>
+  <si>
+    <t>陈沛宁</t>
+  </si>
+  <si>
+    <t>Peining Chen</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/陈沛宁.jpg</t>
+  </si>
+  <si>
+    <t>刘翔</t>
+  </si>
+  <si>
+    <t>Xiang Liu</t>
+  </si>
+  <si>
+    <t>../../assets/img/octocat.png</t>
+  </si>
+  <si>
+    <t>王金文</t>
+  </si>
+  <si>
+    <t>JinWen Wang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/王金文.jpg</t>
+  </si>
+  <si>
+    <t>顾笑与</t>
+  </si>
+  <si>
+    <t>Xiaoyu Gu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/顾笑与.jpg</t>
+  </si>
+  <si>
+    <t>杨子董</t>
+  </si>
+  <si>
+    <t>Zidong Yang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/杨子董.jpg</t>
+  </si>
+  <si>
+    <t>姜振宇</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/姜振宇.jpg</t>
+  </si>
+  <si>
+    <t>渡边翔太</t>
+  </si>
+  <si>
+    <t>WATANABE SHOTA</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/渡边翔太.jpg</t>
+  </si>
+  <si>
+    <t>王梓鉴</t>
+  </si>
+  <si>
+    <t>Zijian Wang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/王梓鉴.jpg</t>
+  </si>
+  <si>
+    <t>孙天翼</t>
+  </si>
+  <si>
+    <t>Tianyi Sun</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/孙天翼.jpg</t>
+  </si>
+  <si>
+    <t>罗予</t>
+  </si>
+  <si>
+    <t>Yu Luo</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/罗予.jpg</t>
+  </si>
+  <si>
+    <t>凤鹏超</t>
+  </si>
+  <si>
+    <t>Pengchao Feng</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/凤鹏超.jpg</t>
+  </si>
+  <si>
+    <t>李亚霖</t>
+  </si>
+  <si>
+    <t>Yalin Li</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/李亚霖.jpg</t>
+  </si>
+  <si>
+    <t>杨子旭</t>
+  </si>
+  <si>
+    <t>Zixu Yang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/杨子旭.jpg</t>
+  </si>
+  <si>
+    <t>Zhenyi Jiang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>张志龙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhilong Zhang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>离开</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2025,6 +2262,7 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2377,13 +2615,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F249"/>
+  <dimension ref="A1:F273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="M231" sqref="M231"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="E281" sqref="E281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
+    <col min="5" max="5" width="86.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -6196,7 +6438,7 @@
         <v>195</v>
       </c>
       <c r="D191" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E191" t="s">
         <v>503</v>
@@ -6307,16 +6549,19 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>517</v>
+        <v>728</v>
       </c>
       <c r="B197" t="s">
-        <v>518</v>
+        <v>729</v>
+      </c>
+      <c r="C197">
+        <v>202</v>
       </c>
       <c r="D197" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="E197" t="s">
-        <v>519</v>
+        <v>730</v>
       </c>
       <c r="F197" t="s">
         <v>228</v>
@@ -6324,16 +6569,19 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>520</v>
+        <v>554</v>
       </c>
       <c r="B198" t="s">
-        <v>521</v>
+        <v>555</v>
+      </c>
+      <c r="C198">
+        <v>203</v>
       </c>
       <c r="D198" t="s">
-        <v>8</v>
+        <v>732</v>
       </c>
       <c r="E198" t="s">
-        <v>13</v>
+        <v>556</v>
       </c>
       <c r="F198" t="s">
         <v>228</v>
@@ -6341,16 +6589,19 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>522</v>
+        <v>536</v>
       </c>
       <c r="B199" t="s">
-        <v>523</v>
+        <v>537</v>
+      </c>
+      <c r="C199">
+        <v>204</v>
       </c>
       <c r="D199" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E199" t="s">
-        <v>524</v>
+        <v>538</v>
       </c>
       <c r="F199" t="s">
         <v>228</v>
@@ -6358,16 +6609,19 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>525</v>
+        <v>663</v>
       </c>
       <c r="B200" t="s">
-        <v>526</v>
+        <v>664</v>
+      </c>
+      <c r="C200">
+        <v>205</v>
       </c>
       <c r="D200" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E200" t="s">
-        <v>527</v>
+        <v>665</v>
       </c>
       <c r="F200" t="s">
         <v>228</v>
@@ -6375,16 +6629,19 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="B201" t="s">
-        <v>529</v>
+        <v>523</v>
+      </c>
+      <c r="C201">
+        <v>206</v>
       </c>
       <c r="D201" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E201" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="F201" t="s">
         <v>228</v>
@@ -6392,16 +6649,19 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>531</v>
+        <v>651</v>
       </c>
       <c r="B202" t="s">
-        <v>532</v>
+        <v>652</v>
+      </c>
+      <c r="C202">
+        <v>208</v>
       </c>
       <c r="D202" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E202" t="s">
-        <v>13</v>
+        <v>653</v>
       </c>
       <c r="F202" t="s">
         <v>228</v>
@@ -6409,16 +6669,19 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>533</v>
+        <v>705</v>
       </c>
       <c r="B203" t="s">
-        <v>534</v>
+        <v>706</v>
+      </c>
+      <c r="C203">
+        <v>209</v>
       </c>
       <c r="D203" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E203" t="s">
-        <v>535</v>
+        <v>707</v>
       </c>
       <c r="F203" t="s">
         <v>228</v>
@@ -6426,16 +6689,19 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>536</v>
+        <v>716</v>
       </c>
       <c r="B204" t="s">
-        <v>537</v>
+        <v>717</v>
+      </c>
+      <c r="C204">
+        <v>210</v>
       </c>
       <c r="D204" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="E204" t="s">
-        <v>538</v>
+        <v>718</v>
       </c>
       <c r="F204" t="s">
         <v>228</v>
@@ -6443,16 +6709,19 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>539</v>
+        <v>654</v>
       </c>
       <c r="B205" t="s">
-        <v>540</v>
+        <v>655</v>
+      </c>
+      <c r="C205">
+        <v>213</v>
       </c>
       <c r="D205" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E205" t="s">
-        <v>541</v>
+        <v>656</v>
       </c>
       <c r="F205" t="s">
         <v>228</v>
@@ -6460,16 +6729,19 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>542</v>
+        <v>608</v>
       </c>
       <c r="B206" t="s">
-        <v>543</v>
+        <v>609</v>
+      </c>
+      <c r="C206">
+        <v>214</v>
       </c>
       <c r="D206" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E206" t="s">
-        <v>13</v>
+        <v>610</v>
       </c>
       <c r="F206" t="s">
         <v>228</v>
@@ -6477,16 +6749,19 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>544</v>
+        <v>559</v>
       </c>
       <c r="B207" t="s">
-        <v>545</v>
+        <v>560</v>
+      </c>
+      <c r="C207">
+        <v>215</v>
       </c>
       <c r="D207" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E207" t="s">
-        <v>546</v>
+        <v>561</v>
       </c>
       <c r="F207" t="s">
         <v>228</v>
@@ -6494,16 +6769,19 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>547</v>
+        <v>710</v>
       </c>
       <c r="B208" t="s">
-        <v>548</v>
+        <v>711</v>
+      </c>
+      <c r="C208">
+        <v>216</v>
       </c>
       <c r="D208" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E208" t="s">
-        <v>13</v>
+        <v>712</v>
       </c>
       <c r="F208" t="s">
         <v>228</v>
@@ -6511,16 +6789,19 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>549</v>
+        <v>642</v>
       </c>
       <c r="B209" t="s">
-        <v>550</v>
+        <v>643</v>
+      </c>
+      <c r="C209">
+        <v>217</v>
       </c>
       <c r="D209" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E209" t="s">
-        <v>13</v>
+        <v>644</v>
       </c>
       <c r="F209" t="s">
         <v>228</v>
@@ -6528,16 +6809,19 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>551</v>
+        <v>645</v>
       </c>
       <c r="B210" t="s">
-        <v>552</v>
+        <v>646</v>
+      </c>
+      <c r="C210">
+        <v>218</v>
       </c>
       <c r="D210" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E210" t="s">
-        <v>553</v>
+        <v>647</v>
       </c>
       <c r="F210" t="s">
         <v>228</v>
@@ -6545,16 +6829,19 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>554</v>
+        <v>611</v>
       </c>
       <c r="B211" t="s">
-        <v>555</v>
+        <v>612</v>
+      </c>
+      <c r="C211">
+        <v>219</v>
       </c>
       <c r="D211" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E211" t="s">
-        <v>13</v>
+        <v>613</v>
       </c>
       <c r="F211" t="s">
         <v>228</v>
@@ -6562,16 +6849,16 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>556</v>
+        <v>517</v>
       </c>
       <c r="B212" t="s">
-        <v>557</v>
+        <v>518</v>
       </c>
       <c r="D212" t="s">
         <v>8</v>
       </c>
       <c r="E212" t="s">
-        <v>13</v>
+        <v>519</v>
       </c>
       <c r="F212" t="s">
         <v>228</v>
@@ -6579,16 +6866,16 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>558</v>
+        <v>520</v>
       </c>
       <c r="B213" t="s">
-        <v>559</v>
+        <v>521</v>
       </c>
       <c r="D213" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E213" t="s">
-        <v>560</v>
+        <v>13</v>
       </c>
       <c r="F213" t="s">
         <v>228</v>
@@ -6596,16 +6883,16 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>561</v>
+        <v>525</v>
       </c>
       <c r="B214" t="s">
-        <v>562</v>
+        <v>526</v>
       </c>
       <c r="D214" t="s">
         <v>8</v>
       </c>
       <c r="E214" t="s">
-        <v>563</v>
+        <v>527</v>
       </c>
       <c r="F214" t="s">
         <v>228</v>
@@ -6613,16 +6900,16 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>564</v>
+        <v>528</v>
       </c>
       <c r="B215" t="s">
-        <v>565</v>
+        <v>529</v>
       </c>
       <c r="D215" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="E215" t="s">
-        <v>566</v>
+        <v>530</v>
       </c>
       <c r="F215" t="s">
         <v>228</v>
@@ -6630,16 +6917,16 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>567</v>
+        <v>531</v>
       </c>
       <c r="B216" t="s">
-        <v>568</v>
+        <v>532</v>
       </c>
       <c r="D216" t="s">
         <v>8</v>
       </c>
       <c r="E216" t="s">
-        <v>569</v>
+        <v>13</v>
       </c>
       <c r="F216" t="s">
         <v>228</v>
@@ -6647,16 +6934,16 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>570</v>
+        <v>533</v>
       </c>
       <c r="B217" t="s">
-        <v>571</v>
+        <v>534</v>
       </c>
       <c r="D217" t="s">
         <v>8</v>
       </c>
       <c r="E217" t="s">
-        <v>13</v>
+        <v>535</v>
       </c>
       <c r="F217" t="s">
         <v>228</v>
@@ -6664,16 +6951,16 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>572</v>
+        <v>539</v>
       </c>
       <c r="B218" t="s">
-        <v>573</v>
+        <v>540</v>
       </c>
       <c r="D218" t="s">
         <v>8</v>
       </c>
       <c r="E218" t="s">
-        <v>574</v>
+        <v>541</v>
       </c>
       <c r="F218" t="s">
         <v>228</v>
@@ -6681,16 +6968,16 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>575</v>
+        <v>542</v>
       </c>
       <c r="B219" t="s">
-        <v>576</v>
+        <v>543</v>
       </c>
       <c r="D219" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E219" t="s">
-        <v>577</v>
+        <v>13</v>
       </c>
       <c r="F219" t="s">
         <v>228</v>
@@ -6698,16 +6985,16 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>578</v>
+        <v>544</v>
       </c>
       <c r="B220" t="s">
-        <v>579</v>
+        <v>545</v>
       </c>
       <c r="D220" t="s">
         <v>8</v>
       </c>
       <c r="E220" t="s">
-        <v>580</v>
+        <v>546</v>
       </c>
       <c r="F220" t="s">
         <v>228</v>
@@ -6715,27 +7002,27 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>581</v>
+        <v>547</v>
       </c>
       <c r="B221" t="s">
-        <v>582</v>
+        <v>548</v>
       </c>
       <c r="D221" t="s">
         <v>8</v>
       </c>
       <c r="E221" t="s">
-        <v>583</v>
+        <v>13</v>
       </c>
       <c r="F221" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>584</v>
+        <v>549</v>
       </c>
       <c r="B222" t="s">
-        <v>585</v>
+        <v>550</v>
       </c>
       <c r="D222" t="s">
         <v>8</v>
@@ -6744,21 +7031,21 @@
         <v>13</v>
       </c>
       <c r="F222" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>586</v>
+        <v>551</v>
       </c>
       <c r="B223" t="s">
-        <v>587</v>
+        <v>552</v>
       </c>
       <c r="D223" t="s">
         <v>8</v>
       </c>
       <c r="E223" t="s">
-        <v>588</v>
+        <v>553</v>
       </c>
       <c r="F223" t="s">
         <v>228</v>
@@ -6766,16 +7053,16 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>589</v>
+        <v>557</v>
       </c>
       <c r="B224" t="s">
-        <v>590</v>
+        <v>558</v>
       </c>
       <c r="D224" t="s">
         <v>8</v>
       </c>
       <c r="E224" t="s">
-        <v>591</v>
+        <v>13</v>
       </c>
       <c r="F224" t="s">
         <v>228</v>
@@ -6783,33 +7070,36 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>592</v>
+        <v>562</v>
       </c>
       <c r="B225" t="s">
-        <v>593</v>
+        <v>563</v>
+      </c>
+      <c r="C225">
+        <v>212</v>
       </c>
       <c r="D225" t="s">
-        <v>8</v>
+        <v>733</v>
       </c>
       <c r="E225" t="s">
-        <v>594</v>
+        <v>564</v>
       </c>
       <c r="F225" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>595</v>
+        <v>565</v>
       </c>
       <c r="B226" t="s">
-        <v>596</v>
+        <v>566</v>
       </c>
       <c r="D226" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E226" t="s">
-        <v>597</v>
+        <v>567</v>
       </c>
       <c r="F226" t="s">
         <v>228</v>
@@ -6817,16 +7107,16 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>598</v>
+        <v>568</v>
       </c>
       <c r="B227" t="s">
-        <v>599</v>
+        <v>569</v>
       </c>
       <c r="D227" t="s">
         <v>8</v>
       </c>
       <c r="E227" t="s">
-        <v>13</v>
+        <v>570</v>
       </c>
       <c r="F227" t="s">
         <v>228</v>
@@ -6834,16 +7124,16 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>600</v>
+        <v>571</v>
       </c>
       <c r="B228" t="s">
-        <v>601</v>
+        <v>572</v>
       </c>
       <c r="D228" t="s">
         <v>8</v>
       </c>
       <c r="E228" t="s">
-        <v>602</v>
+        <v>13</v>
       </c>
       <c r="F228" t="s">
         <v>228</v>
@@ -6851,16 +7141,16 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>603</v>
+        <v>573</v>
       </c>
       <c r="B229" t="s">
-        <v>604</v>
+        <v>574</v>
       </c>
       <c r="D229" t="s">
         <v>8</v>
       </c>
       <c r="E229" t="s">
-        <v>13</v>
+        <v>575</v>
       </c>
       <c r="F229" t="s">
         <v>228</v>
@@ -6868,16 +7158,16 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>605</v>
+        <v>576</v>
       </c>
       <c r="B230" t="s">
-        <v>606</v>
+        <v>577</v>
       </c>
       <c r="D230" t="s">
         <v>8</v>
       </c>
       <c r="E230" t="s">
-        <v>13</v>
+        <v>578</v>
       </c>
       <c r="F230" t="s">
         <v>228</v>
@@ -6885,16 +7175,16 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>607</v>
+        <v>579</v>
       </c>
       <c r="B231" t="s">
-        <v>608</v>
+        <v>580</v>
       </c>
       <c r="D231" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E231" t="s">
-        <v>609</v>
+        <v>581</v>
       </c>
       <c r="F231" t="s">
         <v>228</v>
@@ -6902,27 +7192,27 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>610</v>
+        <v>582</v>
       </c>
       <c r="B232" t="s">
-        <v>611</v>
+        <v>583</v>
       </c>
       <c r="D232" t="s">
         <v>8</v>
       </c>
       <c r="E232" t="s">
-        <v>612</v>
+        <v>584</v>
       </c>
       <c r="F232" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>613</v>
+        <v>585</v>
       </c>
       <c r="B233" t="s">
-        <v>614</v>
+        <v>586</v>
       </c>
       <c r="D233" t="s">
         <v>8</v>
@@ -6931,21 +7221,24 @@
         <v>13</v>
       </c>
       <c r="F233" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>615</v>
+        <v>587</v>
       </c>
       <c r="B234" t="s">
-        <v>616</v>
+        <v>588</v>
+      </c>
+      <c r="C234">
+        <v>201</v>
       </c>
       <c r="D234" t="s">
-        <v>8</v>
+        <v>733</v>
       </c>
       <c r="E234" t="s">
-        <v>617</v>
+        <v>589</v>
       </c>
       <c r="F234" t="s">
         <v>228</v>
@@ -6953,16 +7246,16 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>618</v>
+        <v>590</v>
       </c>
       <c r="B235" t="s">
-        <v>619</v>
+        <v>591</v>
       </c>
       <c r="D235" t="s">
         <v>8</v>
       </c>
       <c r="E235" t="s">
-        <v>620</v>
+        <v>592</v>
       </c>
       <c r="F235" t="s">
         <v>228</v>
@@ -6970,33 +7263,33 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>621</v>
+        <v>593</v>
       </c>
       <c r="B236" t="s">
-        <v>288</v>
+        <v>594</v>
       </c>
       <c r="D236" t="s">
         <v>8</v>
       </c>
       <c r="E236" t="s">
-        <v>622</v>
+        <v>595</v>
       </c>
       <c r="F236" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>623</v>
+        <v>596</v>
       </c>
       <c r="B237" t="s">
-        <v>624</v>
+        <v>597</v>
       </c>
       <c r="D237" t="s">
         <v>8</v>
       </c>
       <c r="E237" t="s">
-        <v>625</v>
+        <v>598</v>
       </c>
       <c r="F237" t="s">
         <v>228</v>
@@ -7004,16 +7297,16 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>626</v>
+        <v>599</v>
       </c>
       <c r="B238" t="s">
-        <v>627</v>
+        <v>600</v>
       </c>
       <c r="D238" t="s">
         <v>8</v>
       </c>
       <c r="E238" t="s">
-        <v>628</v>
+        <v>13</v>
       </c>
       <c r="F238" t="s">
         <v>228</v>
@@ -7021,16 +7314,16 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>629</v>
+        <v>601</v>
       </c>
       <c r="B239" t="s">
-        <v>630</v>
+        <v>602</v>
       </c>
       <c r="D239" t="s">
         <v>8</v>
       </c>
       <c r="E239" t="s">
-        <v>631</v>
+        <v>603</v>
       </c>
       <c r="F239" t="s">
         <v>228</v>
@@ -7038,16 +7331,16 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>632</v>
+        <v>604</v>
       </c>
       <c r="B240" t="s">
-        <v>633</v>
+        <v>605</v>
       </c>
       <c r="D240" t="s">
         <v>8</v>
       </c>
       <c r="E240" t="s">
-        <v>634</v>
+        <v>13</v>
       </c>
       <c r="F240" t="s">
         <v>228</v>
@@ -7055,33 +7348,33 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>635</v>
+        <v>606</v>
       </c>
       <c r="B241" t="s">
-        <v>636</v>
+        <v>607</v>
       </c>
       <c r="D241" t="s">
         <v>8</v>
       </c>
       <c r="E241" t="s">
-        <v>637</v>
+        <v>13</v>
       </c>
       <c r="F241" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>638</v>
+        <v>614</v>
       </c>
       <c r="B242" t="s">
-        <v>639</v>
+        <v>615</v>
       </c>
       <c r="D242" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E242" t="s">
-        <v>640</v>
+        <v>13</v>
       </c>
       <c r="F242" t="s">
         <v>228</v>
@@ -7089,16 +7382,16 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>641</v>
+        <v>616</v>
       </c>
       <c r="B243" t="s">
-        <v>642</v>
+        <v>617</v>
       </c>
       <c r="D243" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E243" t="s">
-        <v>643</v>
+        <v>618</v>
       </c>
       <c r="F243" t="s">
         <v>228</v>
@@ -7106,16 +7399,16 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>644</v>
+        <v>619</v>
       </c>
       <c r="B244" t="s">
-        <v>645</v>
+        <v>620</v>
       </c>
       <c r="D244" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E244" t="s">
-        <v>646</v>
+        <v>621</v>
       </c>
       <c r="F244" t="s">
         <v>228</v>
@@ -7123,16 +7416,16 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>647</v>
+        <v>622</v>
       </c>
       <c r="B245" t="s">
-        <v>648</v>
+        <v>288</v>
       </c>
       <c r="D245" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E245" t="s">
-        <v>649</v>
+        <v>623</v>
       </c>
       <c r="F245" t="s">
         <v>228</v>
@@ -7140,16 +7433,16 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>661</v>
+        <v>624</v>
       </c>
       <c r="B246" t="s">
-        <v>650</v>
+        <v>625</v>
       </c>
       <c r="D246" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E246" t="s">
-        <v>651</v>
+        <v>626</v>
       </c>
       <c r="F246" t="s">
         <v>228</v>
@@ -7157,16 +7450,16 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>652</v>
+        <v>627</v>
       </c>
       <c r="B247" t="s">
-        <v>653</v>
+        <v>628</v>
       </c>
       <c r="D247" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E247" t="s">
-        <v>654</v>
+        <v>629</v>
       </c>
       <c r="F247" t="s">
         <v>228</v>
@@ -7174,16 +7467,16 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>655</v>
+        <v>630</v>
       </c>
       <c r="B248" t="s">
-        <v>656</v>
+        <v>631</v>
       </c>
       <c r="D248" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E248" t="s">
-        <v>657</v>
+        <v>632</v>
       </c>
       <c r="F248" t="s">
         <v>228</v>
@@ -7191,22 +7484,444 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
+        <v>633</v>
+      </c>
+      <c r="B249" t="s">
+        <v>634</v>
+      </c>
+      <c r="D249" t="s">
+        <v>8</v>
+      </c>
+      <c r="E249" t="s">
+        <v>635</v>
+      </c>
+      <c r="F249" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>636</v>
+      </c>
+      <c r="B250" t="s">
+        <v>637</v>
+      </c>
+      <c r="D250" t="s">
+        <v>8</v>
+      </c>
+      <c r="E250" t="s">
+        <v>638</v>
+      </c>
+      <c r="F250" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>639</v>
+      </c>
+      <c r="B251" t="s">
+        <v>640</v>
+      </c>
+      <c r="C251">
+        <v>207</v>
+      </c>
+      <c r="D251" t="s">
+        <v>52</v>
+      </c>
+      <c r="E251" t="s">
+        <v>641</v>
+      </c>
+      <c r="F251" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>648</v>
+      </c>
+      <c r="B252" t="s">
+        <v>649</v>
+      </c>
+      <c r="D252" t="s">
+        <v>16</v>
+      </c>
+      <c r="E252" t="s">
+        <v>650</v>
+      </c>
+      <c r="F252" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>657</v>
+      </c>
+      <c r="B253" t="s">
         <v>658</v>
       </c>
-      <c r="B249" t="s">
+      <c r="C253">
+        <v>211</v>
+      </c>
+      <c r="D253" t="s">
+        <v>16</v>
+      </c>
+      <c r="E253" t="s">
         <v>659</v>
       </c>
-      <c r="D249" t="s">
-        <v>8</v>
-      </c>
-      <c r="E249" t="s">
+      <c r="F253" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
         <v>660</v>
       </c>
-      <c r="F249" t="s">
-        <v>228</v>
+      <c r="B254" t="s">
+        <v>661</v>
+      </c>
+      <c r="D254" t="s">
+        <v>8</v>
+      </c>
+      <c r="E254" t="s">
+        <v>662</v>
+      </c>
+      <c r="F254" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>666</v>
+      </c>
+      <c r="B255" t="s">
+        <v>667</v>
+      </c>
+      <c r="D255" t="s">
+        <v>52</v>
+      </c>
+      <c r="E255" t="s">
+        <v>668</v>
+      </c>
+      <c r="F255" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>669</v>
+      </c>
+      <c r="B256" t="s">
+        <v>670</v>
+      </c>
+      <c r="D256" t="s">
+        <v>8</v>
+      </c>
+      <c r="E256" t="s">
+        <v>671</v>
+      </c>
+      <c r="F256" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>672</v>
+      </c>
+      <c r="B257" t="s">
+        <v>673</v>
+      </c>
+      <c r="D257" t="s">
+        <v>52</v>
+      </c>
+      <c r="E257" t="s">
+        <v>674</v>
+      </c>
+      <c r="F257" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>675</v>
+      </c>
+      <c r="B258" t="s">
+        <v>676</v>
+      </c>
+      <c r="D258" t="s">
+        <v>8</v>
+      </c>
+      <c r="E258" t="s">
+        <v>677</v>
+      </c>
+      <c r="F258" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>678</v>
+      </c>
+      <c r="B259" t="s">
+        <v>679</v>
+      </c>
+      <c r="D259" t="s">
+        <v>8</v>
+      </c>
+      <c r="E259" t="s">
+        <v>680</v>
+      </c>
+      <c r="F259" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>681</v>
+      </c>
+      <c r="B260" t="s">
+        <v>682</v>
+      </c>
+      <c r="D260" t="s">
+        <v>8</v>
+      </c>
+      <c r="E260" t="s">
+        <v>683</v>
+      </c>
+      <c r="F260" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>684</v>
+      </c>
+      <c r="B261" t="s">
+        <v>685</v>
+      </c>
+      <c r="D261" t="s">
+        <v>8</v>
+      </c>
+      <c r="E261" t="s">
+        <v>686</v>
+      </c>
+      <c r="F261" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>687</v>
+      </c>
+      <c r="B262" t="s">
+        <v>688</v>
+      </c>
+      <c r="D262" t="s">
+        <v>8</v>
+      </c>
+      <c r="E262" t="s">
+        <v>689</v>
+      </c>
+      <c r="F262" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>690</v>
+      </c>
+      <c r="B263" t="s">
+        <v>691</v>
+      </c>
+      <c r="D263" t="s">
+        <v>8</v>
+      </c>
+      <c r="E263" t="s">
+        <v>692</v>
+      </c>
+      <c r="F263" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>693</v>
+      </c>
+      <c r="B264" t="s">
+        <v>694</v>
+      </c>
+      <c r="D264" t="s">
+        <v>8</v>
+      </c>
+      <c r="E264" t="s">
+        <v>695</v>
+      </c>
+      <c r="F264" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>696</v>
+      </c>
+      <c r="B265" t="s">
+        <v>697</v>
+      </c>
+      <c r="D265" t="s">
+        <v>8</v>
+      </c>
+      <c r="E265" t="s">
+        <v>698</v>
+      </c>
+      <c r="F265" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>699</v>
+      </c>
+      <c r="B266" t="s">
+        <v>700</v>
+      </c>
+      <c r="D266" t="s">
+        <v>8</v>
+      </c>
+      <c r="E266" t="s">
+        <v>701</v>
+      </c>
+      <c r="F266" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>702</v>
+      </c>
+      <c r="B267" t="s">
+        <v>703</v>
+      </c>
+      <c r="D267" t="s">
+        <v>16</v>
+      </c>
+      <c r="E267" t="s">
+        <v>704</v>
+      </c>
+      <c r="F267" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>708</v>
+      </c>
+      <c r="B268" t="s">
+        <v>731</v>
+      </c>
+      <c r="D268" t="s">
+        <v>8</v>
+      </c>
+      <c r="E268" t="s">
+        <v>709</v>
+      </c>
+      <c r="F268" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>713</v>
+      </c>
+      <c r="B269" t="s">
+        <v>714</v>
+      </c>
+      <c r="D269" t="s">
+        <v>8</v>
+      </c>
+      <c r="E269" t="s">
+        <v>715</v>
+      </c>
+      <c r="F269" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>719</v>
+      </c>
+      <c r="B270" t="s">
+        <v>720</v>
+      </c>
+      <c r="D270" t="s">
+        <v>8</v>
+      </c>
+      <c r="E270" t="s">
+        <v>721</v>
+      </c>
+      <c r="F270" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>722</v>
+      </c>
+      <c r="B271" t="s">
+        <v>723</v>
+      </c>
+      <c r="D271" t="s">
+        <v>8</v>
+      </c>
+      <c r="E271" t="s">
+        <v>724</v>
+      </c>
+      <c r="F271" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>725</v>
+      </c>
+      <c r="B272" t="s">
+        <v>726</v>
+      </c>
+      <c r="D272" t="s">
+        <v>8</v>
+      </c>
+      <c r="E272" t="s">
+        <v>727</v>
+      </c>
+      <c r="F272" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>734</v>
+      </c>
+      <c r="B273" t="s">
+        <v>735</v>
+      </c>
+      <c r="C273">
+        <v>220</v>
+      </c>
+      <c r="D273" t="s">
+        <v>736</v>
+      </c>
+      <c r="E273" t="s">
+        <v>698</v>
+      </c>
+      <c r="F273" t="s">
+        <v>737</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F272">
+      <sortCondition ref="C1"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@ffc48296f794a3144403110d9c54b50d6be61054 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465F157A-1BB7-4AF0-BF35-00D9D75DE064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C60FA30-4F1D-4CB4-A209-36FE1C679EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="738">
   <si>
     <t>name</t>
   </si>
@@ -1690,6 +1693,9 @@
     <t>Yuzhe Liang</t>
   </si>
   <si>
+    <t>/assets/img/members/student/梁宇哲.jpg</t>
+  </si>
+  <si>
     <t>刘轩丞</t>
   </si>
   <si>
@@ -1957,7 +1963,7 @@
     <t>吴媚</t>
   </si>
   <si>
-    <t>WuMei</t>
+    <t>Mei Wu</t>
   </si>
   <si>
     <t>/assets/img/members/student/吴媚.jpg</t>
@@ -1972,6 +1978,9 @@
     <t>/assets/img/members/student/王哲祥.jpg</t>
   </si>
   <si>
+    <t>蔡崇皓</t>
+  </si>
+  <si>
     <t>Chonghao Cai</t>
   </si>
   <si>
@@ -1981,7 +1990,7 @@
     <t>朱轩宇</t>
   </si>
   <si>
-    <t>Xuanyu Zhu</t>
+    <t>Zhu Xuanyu</t>
   </si>
   <si>
     <t>/assets/img/members/student/朱轩宇.jpg</t>
@@ -2005,7 +2014,235 @@
     <t>/assets/img/members/student/刘峻希.jpg</t>
   </si>
   <si>
-    <t>蔡崇皓</t>
+    <t>孙文杰</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wenjie Sun </t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/孙文杰.jpg</t>
+  </si>
+  <si>
+    <t>刘展勋</t>
+  </si>
+  <si>
+    <t>Zhanxun Liu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/刘展勋.jpg</t>
+  </si>
+  <si>
+    <t>李师萌</t>
+  </si>
+  <si>
+    <t>Shimeng Li</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/李师萌.jpg</t>
+  </si>
+  <si>
+    <t>韩晨烨</t>
+  </si>
+  <si>
+    <t>Chenye Han</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/韩晨烨.jpg</t>
+  </si>
+  <si>
+    <t>涂宇清</t>
+  </si>
+  <si>
+    <t>Yuqing Tu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/涂宇清.jpg</t>
+  </si>
+  <si>
+    <t>张锦维</t>
+  </si>
+  <si>
+    <t>Jinwei Zhang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/张锦维.jpg</t>
+  </si>
+  <si>
+    <t>黄文宾</t>
+  </si>
+  <si>
+    <t>Wenbin Huang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/黄文宾.jpg</t>
+  </si>
+  <si>
+    <t>徐世奇</t>
+  </si>
+  <si>
+    <t>Shiqi Xu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/徐世奇.jpg</t>
+  </si>
+  <si>
+    <t>尹志强</t>
+  </si>
+  <si>
+    <t>zhiqiangyin</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/尹志强.jpg</t>
+  </si>
+  <si>
+    <t>张书畅</t>
+  </si>
+  <si>
+    <t>Shuchang Zhang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/张书畅.jpg</t>
+  </si>
+  <si>
+    <t>陈沛宁</t>
+  </si>
+  <si>
+    <t>Peining Chen</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/陈沛宁.jpg</t>
+  </si>
+  <si>
+    <t>刘翔</t>
+  </si>
+  <si>
+    <t>Xiang Liu</t>
+  </si>
+  <si>
+    <t>../../assets/img/octocat.png</t>
+  </si>
+  <si>
+    <t>王金文</t>
+  </si>
+  <si>
+    <t>JinWen Wang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/王金文.jpg</t>
+  </si>
+  <si>
+    <t>顾笑与</t>
+  </si>
+  <si>
+    <t>Xiaoyu Gu</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/顾笑与.jpg</t>
+  </si>
+  <si>
+    <t>杨子董</t>
+  </si>
+  <si>
+    <t>Zidong Yang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/杨子董.jpg</t>
+  </si>
+  <si>
+    <t>姜振宇</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/姜振宇.jpg</t>
+  </si>
+  <si>
+    <t>渡边翔太</t>
+  </si>
+  <si>
+    <t>WATANABE SHOTA</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/渡边翔太.jpg</t>
+  </si>
+  <si>
+    <t>王梓鉴</t>
+  </si>
+  <si>
+    <t>Zijian Wang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/王梓鉴.jpg</t>
+  </si>
+  <si>
+    <t>孙天翼</t>
+  </si>
+  <si>
+    <t>Tianyi Sun</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/孙天翼.jpg</t>
+  </si>
+  <si>
+    <t>罗予</t>
+  </si>
+  <si>
+    <t>Yu Luo</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/罗予.jpg</t>
+  </si>
+  <si>
+    <t>凤鹏超</t>
+  </si>
+  <si>
+    <t>Pengchao Feng</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/凤鹏超.jpg</t>
+  </si>
+  <si>
+    <t>李亚霖</t>
+  </si>
+  <si>
+    <t>Yalin Li</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/李亚霖.jpg</t>
+  </si>
+  <si>
+    <t>杨子旭</t>
+  </si>
+  <si>
+    <t>Zixu Yang</t>
+  </si>
+  <si>
+    <t>/assets/img/members/student/杨子旭.jpg</t>
+  </si>
+  <si>
+    <t>Zhenyi Jiang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>张志龙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zhilong Zhang</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>离开</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2025,6 +2262,7 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2377,13 +2615,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F249"/>
+  <dimension ref="A1:F273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" workbookViewId="0">
-      <selection activeCell="M231" sqref="M231"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
+      <selection activeCell="E281" sqref="E281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.7265625" customWidth="1"/>
+    <col min="5" max="5" width="86.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -6196,7 +6438,7 @@
         <v>195</v>
       </c>
       <c r="D191" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E191" t="s">
         <v>503</v>
@@ -6307,16 +6549,19 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>517</v>
+        <v>728</v>
       </c>
       <c r="B197" t="s">
-        <v>518</v>
+        <v>729</v>
+      </c>
+      <c r="C197">
+        <v>202</v>
       </c>
       <c r="D197" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="E197" t="s">
-        <v>519</v>
+        <v>730</v>
       </c>
       <c r="F197" t="s">
         <v>228</v>
@@ -6324,16 +6569,19 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>520</v>
+        <v>554</v>
       </c>
       <c r="B198" t="s">
-        <v>521</v>
+        <v>555</v>
+      </c>
+      <c r="C198">
+        <v>203</v>
       </c>
       <c r="D198" t="s">
-        <v>8</v>
+        <v>732</v>
       </c>
       <c r="E198" t="s">
-        <v>13</v>
+        <v>556</v>
       </c>
       <c r="F198" t="s">
         <v>228</v>
@@ -6341,16 +6589,19 @@
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>522</v>
+        <v>536</v>
       </c>
       <c r="B199" t="s">
-        <v>523</v>
+        <v>537</v>
+      </c>
+      <c r="C199">
+        <v>204</v>
       </c>
       <c r="D199" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E199" t="s">
-        <v>524</v>
+        <v>538</v>
       </c>
       <c r="F199" t="s">
         <v>228</v>
@@ -6358,16 +6609,19 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>525</v>
+        <v>663</v>
       </c>
       <c r="B200" t="s">
-        <v>526</v>
+        <v>664</v>
+      </c>
+      <c r="C200">
+        <v>205</v>
       </c>
       <c r="D200" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E200" t="s">
-        <v>527</v>
+        <v>665</v>
       </c>
       <c r="F200" t="s">
         <v>228</v>
@@ -6375,16 +6629,19 @@
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="B201" t="s">
-        <v>529</v>
+        <v>523</v>
+      </c>
+      <c r="C201">
+        <v>206</v>
       </c>
       <c r="D201" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="E201" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="F201" t="s">
         <v>228</v>
@@ -6392,16 +6649,19 @@
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>531</v>
+        <v>651</v>
       </c>
       <c r="B202" t="s">
-        <v>532</v>
+        <v>652</v>
+      </c>
+      <c r="C202">
+        <v>208</v>
       </c>
       <c r="D202" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E202" t="s">
-        <v>13</v>
+        <v>653</v>
       </c>
       <c r="F202" t="s">
         <v>228</v>
@@ -6409,16 +6669,19 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>533</v>
+        <v>705</v>
       </c>
       <c r="B203" t="s">
-        <v>534</v>
+        <v>706</v>
+      </c>
+      <c r="C203">
+        <v>209</v>
       </c>
       <c r="D203" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E203" t="s">
-        <v>535</v>
+        <v>707</v>
       </c>
       <c r="F203" t="s">
         <v>228</v>
@@ -6426,16 +6689,19 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>536</v>
+        <v>716</v>
       </c>
       <c r="B204" t="s">
-        <v>537</v>
+        <v>717</v>
+      </c>
+      <c r="C204">
+        <v>210</v>
       </c>
       <c r="D204" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="E204" t="s">
-        <v>538</v>
+        <v>718</v>
       </c>
       <c r="F204" t="s">
         <v>228</v>
@@ -6443,16 +6709,19 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>539</v>
+        <v>654</v>
       </c>
       <c r="B205" t="s">
-        <v>540</v>
+        <v>655</v>
+      </c>
+      <c r="C205">
+        <v>213</v>
       </c>
       <c r="D205" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E205" t="s">
-        <v>541</v>
+        <v>656</v>
       </c>
       <c r="F205" t="s">
         <v>228</v>
@@ -6460,16 +6729,19 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>542</v>
+        <v>608</v>
       </c>
       <c r="B206" t="s">
-        <v>543</v>
+        <v>609</v>
+      </c>
+      <c r="C206">
+        <v>214</v>
       </c>
       <c r="D206" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E206" t="s">
-        <v>13</v>
+        <v>610</v>
       </c>
       <c r="F206" t="s">
         <v>228</v>
@@ -6477,16 +6749,19 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>544</v>
+        <v>559</v>
       </c>
       <c r="B207" t="s">
-        <v>545</v>
+        <v>560</v>
+      </c>
+      <c r="C207">
+        <v>215</v>
       </c>
       <c r="D207" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E207" t="s">
-        <v>546</v>
+        <v>561</v>
       </c>
       <c r="F207" t="s">
         <v>228</v>
@@ -6494,16 +6769,19 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>547</v>
+        <v>710</v>
       </c>
       <c r="B208" t="s">
-        <v>548</v>
+        <v>711</v>
+      </c>
+      <c r="C208">
+        <v>216</v>
       </c>
       <c r="D208" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E208" t="s">
-        <v>13</v>
+        <v>712</v>
       </c>
       <c r="F208" t="s">
         <v>228</v>
@@ -6511,16 +6789,19 @@
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>549</v>
+        <v>642</v>
       </c>
       <c r="B209" t="s">
-        <v>550</v>
+        <v>643</v>
+      </c>
+      <c r="C209">
+        <v>217</v>
       </c>
       <c r="D209" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E209" t="s">
-        <v>13</v>
+        <v>644</v>
       </c>
       <c r="F209" t="s">
         <v>228</v>
@@ -6528,16 +6809,19 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>551</v>
+        <v>645</v>
       </c>
       <c r="B210" t="s">
-        <v>552</v>
+        <v>646</v>
+      </c>
+      <c r="C210">
+        <v>218</v>
       </c>
       <c r="D210" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E210" t="s">
-        <v>553</v>
+        <v>647</v>
       </c>
       <c r="F210" t="s">
         <v>228</v>
@@ -6545,16 +6829,19 @@
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>554</v>
+        <v>611</v>
       </c>
       <c r="B211" t="s">
-        <v>555</v>
+        <v>612</v>
+      </c>
+      <c r="C211">
+        <v>219</v>
       </c>
       <c r="D211" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E211" t="s">
-        <v>13</v>
+        <v>613</v>
       </c>
       <c r="F211" t="s">
         <v>228</v>
@@ -6562,16 +6849,16 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>556</v>
+        <v>517</v>
       </c>
       <c r="B212" t="s">
-        <v>557</v>
+        <v>518</v>
       </c>
       <c r="D212" t="s">
         <v>8</v>
       </c>
       <c r="E212" t="s">
-        <v>13</v>
+        <v>519</v>
       </c>
       <c r="F212" t="s">
         <v>228</v>
@@ -6579,16 +6866,16 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>558</v>
+        <v>520</v>
       </c>
       <c r="B213" t="s">
-        <v>559</v>
+        <v>521</v>
       </c>
       <c r="D213" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E213" t="s">
-        <v>560</v>
+        <v>13</v>
       </c>
       <c r="F213" t="s">
         <v>228</v>
@@ -6596,16 +6883,16 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>561</v>
+        <v>525</v>
       </c>
       <c r="B214" t="s">
-        <v>562</v>
+        <v>526</v>
       </c>
       <c r="D214" t="s">
         <v>8</v>
       </c>
       <c r="E214" t="s">
-        <v>563</v>
+        <v>527</v>
       </c>
       <c r="F214" t="s">
         <v>228</v>
@@ -6613,16 +6900,16 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>564</v>
+        <v>528</v>
       </c>
       <c r="B215" t="s">
-        <v>565</v>
+        <v>529</v>
       </c>
       <c r="D215" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="E215" t="s">
-        <v>566</v>
+        <v>530</v>
       </c>
       <c r="F215" t="s">
         <v>228</v>
@@ -6630,16 +6917,16 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>567</v>
+        <v>531</v>
       </c>
       <c r="B216" t="s">
-        <v>568</v>
+        <v>532</v>
       </c>
       <c r="D216" t="s">
         <v>8</v>
       </c>
       <c r="E216" t="s">
-        <v>569</v>
+        <v>13</v>
       </c>
       <c r="F216" t="s">
         <v>228</v>
@@ -6647,16 +6934,16 @@
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>570</v>
+        <v>533</v>
       </c>
       <c r="B217" t="s">
-        <v>571</v>
+        <v>534</v>
       </c>
       <c r="D217" t="s">
         <v>8</v>
       </c>
       <c r="E217" t="s">
-        <v>13</v>
+        <v>535</v>
       </c>
       <c r="F217" t="s">
         <v>228</v>
@@ -6664,16 +6951,16 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>572</v>
+        <v>539</v>
       </c>
       <c r="B218" t="s">
-        <v>573</v>
+        <v>540</v>
       </c>
       <c r="D218" t="s">
         <v>8</v>
       </c>
       <c r="E218" t="s">
-        <v>574</v>
+        <v>541</v>
       </c>
       <c r="F218" t="s">
         <v>228</v>
@@ -6681,16 +6968,16 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>575</v>
+        <v>542</v>
       </c>
       <c r="B219" t="s">
-        <v>576</v>
+        <v>543</v>
       </c>
       <c r="D219" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E219" t="s">
-        <v>577</v>
+        <v>13</v>
       </c>
       <c r="F219" t="s">
         <v>228</v>
@@ -6698,16 +6985,16 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>578</v>
+        <v>544</v>
       </c>
       <c r="B220" t="s">
-        <v>579</v>
+        <v>545</v>
       </c>
       <c r="D220" t="s">
         <v>8</v>
       </c>
       <c r="E220" t="s">
-        <v>580</v>
+        <v>546</v>
       </c>
       <c r="F220" t="s">
         <v>228</v>
@@ -6715,27 +7002,27 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>581</v>
+        <v>547</v>
       </c>
       <c r="B221" t="s">
-        <v>582</v>
+        <v>548</v>
       </c>
       <c r="D221" t="s">
         <v>8</v>
       </c>
       <c r="E221" t="s">
-        <v>583</v>
+        <v>13</v>
       </c>
       <c r="F221" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>584</v>
+        <v>549</v>
       </c>
       <c r="B222" t="s">
-        <v>585</v>
+        <v>550</v>
       </c>
       <c r="D222" t="s">
         <v>8</v>
@@ -6744,21 +7031,21 @@
         <v>13</v>
       </c>
       <c r="F222" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>586</v>
+        <v>551</v>
       </c>
       <c r="B223" t="s">
-        <v>587</v>
+        <v>552</v>
       </c>
       <c r="D223" t="s">
         <v>8</v>
       </c>
       <c r="E223" t="s">
-        <v>588</v>
+        <v>553</v>
       </c>
       <c r="F223" t="s">
         <v>228</v>
@@ -6766,16 +7053,16 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>589</v>
+        <v>557</v>
       </c>
       <c r="B224" t="s">
-        <v>590</v>
+        <v>558</v>
       </c>
       <c r="D224" t="s">
         <v>8</v>
       </c>
       <c r="E224" t="s">
-        <v>591</v>
+        <v>13</v>
       </c>
       <c r="F224" t="s">
         <v>228</v>
@@ -6783,33 +7070,36 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>592</v>
+        <v>562</v>
       </c>
       <c r="B225" t="s">
-        <v>593</v>
+        <v>563</v>
+      </c>
+      <c r="C225">
+        <v>212</v>
       </c>
       <c r="D225" t="s">
-        <v>8</v>
+        <v>733</v>
       </c>
       <c r="E225" t="s">
-        <v>594</v>
+        <v>564</v>
       </c>
       <c r="F225" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>595</v>
+        <v>565</v>
       </c>
       <c r="B226" t="s">
-        <v>596</v>
+        <v>566</v>
       </c>
       <c r="D226" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E226" t="s">
-        <v>597</v>
+        <v>567</v>
       </c>
       <c r="F226" t="s">
         <v>228</v>
@@ -6817,16 +7107,16 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>598</v>
+        <v>568</v>
       </c>
       <c r="B227" t="s">
-        <v>599</v>
+        <v>569</v>
       </c>
       <c r="D227" t="s">
         <v>8</v>
       </c>
       <c r="E227" t="s">
-        <v>13</v>
+        <v>570</v>
       </c>
       <c r="F227" t="s">
         <v>228</v>
@@ -6834,16 +7124,16 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>600</v>
+        <v>571</v>
       </c>
       <c r="B228" t="s">
-        <v>601</v>
+        <v>572</v>
       </c>
       <c r="D228" t="s">
         <v>8</v>
       </c>
       <c r="E228" t="s">
-        <v>602</v>
+        <v>13</v>
       </c>
       <c r="F228" t="s">
         <v>228</v>
@@ -6851,16 +7141,16 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>603</v>
+        <v>573</v>
       </c>
       <c r="B229" t="s">
-        <v>604</v>
+        <v>574</v>
       </c>
       <c r="D229" t="s">
         <v>8</v>
       </c>
       <c r="E229" t="s">
-        <v>13</v>
+        <v>575</v>
       </c>
       <c r="F229" t="s">
         <v>228</v>
@@ -6868,16 +7158,16 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>605</v>
+        <v>576</v>
       </c>
       <c r="B230" t="s">
-        <v>606</v>
+        <v>577</v>
       </c>
       <c r="D230" t="s">
         <v>8</v>
       </c>
       <c r="E230" t="s">
-        <v>13</v>
+        <v>578</v>
       </c>
       <c r="F230" t="s">
         <v>228</v>
@@ -6885,16 +7175,16 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>607</v>
+        <v>579</v>
       </c>
       <c r="B231" t="s">
-        <v>608</v>
+        <v>580</v>
       </c>
       <c r="D231" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E231" t="s">
-        <v>609</v>
+        <v>581</v>
       </c>
       <c r="F231" t="s">
         <v>228</v>
@@ -6902,27 +7192,27 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>610</v>
+        <v>582</v>
       </c>
       <c r="B232" t="s">
-        <v>611</v>
+        <v>583</v>
       </c>
       <c r="D232" t="s">
         <v>8</v>
       </c>
       <c r="E232" t="s">
-        <v>612</v>
+        <v>584</v>
       </c>
       <c r="F232" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>613</v>
+        <v>585</v>
       </c>
       <c r="B233" t="s">
-        <v>614</v>
+        <v>586</v>
       </c>
       <c r="D233" t="s">
         <v>8</v>
@@ -6931,21 +7221,24 @@
         <v>13</v>
       </c>
       <c r="F233" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>615</v>
+        <v>587</v>
       </c>
       <c r="B234" t="s">
-        <v>616</v>
+        <v>588</v>
+      </c>
+      <c r="C234">
+        <v>201</v>
       </c>
       <c r="D234" t="s">
-        <v>8</v>
+        <v>733</v>
       </c>
       <c r="E234" t="s">
-        <v>617</v>
+        <v>589</v>
       </c>
       <c r="F234" t="s">
         <v>228</v>
@@ -6953,16 +7246,16 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>618</v>
+        <v>590</v>
       </c>
       <c r="B235" t="s">
-        <v>619</v>
+        <v>591</v>
       </c>
       <c r="D235" t="s">
         <v>8</v>
       </c>
       <c r="E235" t="s">
-        <v>620</v>
+        <v>592</v>
       </c>
       <c r="F235" t="s">
         <v>228</v>
@@ -6970,33 +7263,33 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>621</v>
+        <v>593</v>
       </c>
       <c r="B236" t="s">
-        <v>288</v>
+        <v>594</v>
       </c>
       <c r="D236" t="s">
         <v>8</v>
       </c>
       <c r="E236" t="s">
-        <v>622</v>
+        <v>595</v>
       </c>
       <c r="F236" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>623</v>
+        <v>596</v>
       </c>
       <c r="B237" t="s">
-        <v>624</v>
+        <v>597</v>
       </c>
       <c r="D237" t="s">
         <v>8</v>
       </c>
       <c r="E237" t="s">
-        <v>625</v>
+        <v>598</v>
       </c>
       <c r="F237" t="s">
         <v>228</v>
@@ -7004,16 +7297,16 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>626</v>
+        <v>599</v>
       </c>
       <c r="B238" t="s">
-        <v>627</v>
+        <v>600</v>
       </c>
       <c r="D238" t="s">
         <v>8</v>
       </c>
       <c r="E238" t="s">
-        <v>628</v>
+        <v>13</v>
       </c>
       <c r="F238" t="s">
         <v>228</v>
@@ -7021,16 +7314,16 @@
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>629</v>
+        <v>601</v>
       </c>
       <c r="B239" t="s">
-        <v>630</v>
+        <v>602</v>
       </c>
       <c r="D239" t="s">
         <v>8</v>
       </c>
       <c r="E239" t="s">
-        <v>631</v>
+        <v>603</v>
       </c>
       <c r="F239" t="s">
         <v>228</v>
@@ -7038,16 +7331,16 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>632</v>
+        <v>604</v>
       </c>
       <c r="B240" t="s">
-        <v>633</v>
+        <v>605</v>
       </c>
       <c r="D240" t="s">
         <v>8</v>
       </c>
       <c r="E240" t="s">
-        <v>634</v>
+        <v>13</v>
       </c>
       <c r="F240" t="s">
         <v>228</v>
@@ -7055,33 +7348,33 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>635</v>
+        <v>606</v>
       </c>
       <c r="B241" t="s">
-        <v>636</v>
+        <v>607</v>
       </c>
       <c r="D241" t="s">
         <v>8</v>
       </c>
       <c r="E241" t="s">
-        <v>637</v>
+        <v>13</v>
       </c>
       <c r="F241" t="s">
-        <v>10</v>
+        <v>228</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>638</v>
+        <v>614</v>
       </c>
       <c r="B242" t="s">
-        <v>639</v>
+        <v>615</v>
       </c>
       <c r="D242" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E242" t="s">
-        <v>640</v>
+        <v>13</v>
       </c>
       <c r="F242" t="s">
         <v>228</v>
@@ -7089,16 +7382,16 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>641</v>
+        <v>616</v>
       </c>
       <c r="B243" t="s">
-        <v>642</v>
+        <v>617</v>
       </c>
       <c r="D243" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E243" t="s">
-        <v>643</v>
+        <v>618</v>
       </c>
       <c r="F243" t="s">
         <v>228</v>
@@ -7106,16 +7399,16 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>644</v>
+        <v>619</v>
       </c>
       <c r="B244" t="s">
-        <v>645</v>
+        <v>620</v>
       </c>
       <c r="D244" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E244" t="s">
-        <v>646</v>
+        <v>621</v>
       </c>
       <c r="F244" t="s">
         <v>228</v>
@@ -7123,16 +7416,16 @@
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>647</v>
+        <v>622</v>
       </c>
       <c r="B245" t="s">
-        <v>648</v>
+        <v>288</v>
       </c>
       <c r="D245" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E245" t="s">
-        <v>649</v>
+        <v>623</v>
       </c>
       <c r="F245" t="s">
         <v>228</v>
@@ -7140,16 +7433,16 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>661</v>
+        <v>624</v>
       </c>
       <c r="B246" t="s">
-        <v>650</v>
+        <v>625</v>
       </c>
       <c r="D246" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E246" t="s">
-        <v>651</v>
+        <v>626</v>
       </c>
       <c r="F246" t="s">
         <v>228</v>
@@ -7157,16 +7450,16 @@
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>652</v>
+        <v>627</v>
       </c>
       <c r="B247" t="s">
-        <v>653</v>
+        <v>628</v>
       </c>
       <c r="D247" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="E247" t="s">
-        <v>654</v>
+        <v>629</v>
       </c>
       <c r="F247" t="s">
         <v>228</v>
@@ -7174,16 +7467,16 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>655</v>
+        <v>630</v>
       </c>
       <c r="B248" t="s">
-        <v>656</v>
+        <v>631</v>
       </c>
       <c r="D248" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E248" t="s">
-        <v>657</v>
+        <v>632</v>
       </c>
       <c r="F248" t="s">
         <v>228</v>
@@ -7191,22 +7484,444 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
+        <v>633</v>
+      </c>
+      <c r="B249" t="s">
+        <v>634</v>
+      </c>
+      <c r="D249" t="s">
+        <v>8</v>
+      </c>
+      <c r="E249" t="s">
+        <v>635</v>
+      </c>
+      <c r="F249" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>636</v>
+      </c>
+      <c r="B250" t="s">
+        <v>637</v>
+      </c>
+      <c r="D250" t="s">
+        <v>8</v>
+      </c>
+      <c r="E250" t="s">
+        <v>638</v>
+      </c>
+      <c r="F250" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>639</v>
+      </c>
+      <c r="B251" t="s">
+        <v>640</v>
+      </c>
+      <c r="C251">
+        <v>207</v>
+      </c>
+      <c r="D251" t="s">
+        <v>52</v>
+      </c>
+      <c r="E251" t="s">
+        <v>641</v>
+      </c>
+      <c r="F251" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>648</v>
+      </c>
+      <c r="B252" t="s">
+        <v>649</v>
+      </c>
+      <c r="D252" t="s">
+        <v>16</v>
+      </c>
+      <c r="E252" t="s">
+        <v>650</v>
+      </c>
+      <c r="F252" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>657</v>
+      </c>
+      <c r="B253" t="s">
         <v>658</v>
       </c>
-      <c r="B249" t="s">
+      <c r="C253">
+        <v>211</v>
+      </c>
+      <c r="D253" t="s">
+        <v>16</v>
+      </c>
+      <c r="E253" t="s">
         <v>659</v>
       </c>
-      <c r="D249" t="s">
-        <v>8</v>
-      </c>
-      <c r="E249" t="s">
+      <c r="F253" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
         <v>660</v>
       </c>
-      <c r="F249" t="s">
-        <v>228</v>
+      <c r="B254" t="s">
+        <v>661</v>
+      </c>
+      <c r="D254" t="s">
+        <v>8</v>
+      </c>
+      <c r="E254" t="s">
+        <v>662</v>
+      </c>
+      <c r="F254" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>666</v>
+      </c>
+      <c r="B255" t="s">
+        <v>667</v>
+      </c>
+      <c r="D255" t="s">
+        <v>52</v>
+      </c>
+      <c r="E255" t="s">
+        <v>668</v>
+      </c>
+      <c r="F255" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>669</v>
+      </c>
+      <c r="B256" t="s">
+        <v>670</v>
+      </c>
+      <c r="D256" t="s">
+        <v>8</v>
+      </c>
+      <c r="E256" t="s">
+        <v>671</v>
+      </c>
+      <c r="F256" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>672</v>
+      </c>
+      <c r="B257" t="s">
+        <v>673</v>
+      </c>
+      <c r="D257" t="s">
+        <v>52</v>
+      </c>
+      <c r="E257" t="s">
+        <v>674</v>
+      </c>
+      <c r="F257" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>675</v>
+      </c>
+      <c r="B258" t="s">
+        <v>676</v>
+      </c>
+      <c r="D258" t="s">
+        <v>8</v>
+      </c>
+      <c r="E258" t="s">
+        <v>677</v>
+      </c>
+      <c r="F258" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>678</v>
+      </c>
+      <c r="B259" t="s">
+        <v>679</v>
+      </c>
+      <c r="D259" t="s">
+        <v>8</v>
+      </c>
+      <c r="E259" t="s">
+        <v>680</v>
+      </c>
+      <c r="F259" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>681</v>
+      </c>
+      <c r="B260" t="s">
+        <v>682</v>
+      </c>
+      <c r="D260" t="s">
+        <v>8</v>
+      </c>
+      <c r="E260" t="s">
+        <v>683</v>
+      </c>
+      <c r="F260" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>684</v>
+      </c>
+      <c r="B261" t="s">
+        <v>685</v>
+      </c>
+      <c r="D261" t="s">
+        <v>8</v>
+      </c>
+      <c r="E261" t="s">
+        <v>686</v>
+      </c>
+      <c r="F261" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>687</v>
+      </c>
+      <c r="B262" t="s">
+        <v>688</v>
+      </c>
+      <c r="D262" t="s">
+        <v>8</v>
+      </c>
+      <c r="E262" t="s">
+        <v>689</v>
+      </c>
+      <c r="F262" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>690</v>
+      </c>
+      <c r="B263" t="s">
+        <v>691</v>
+      </c>
+      <c r="D263" t="s">
+        <v>8</v>
+      </c>
+      <c r="E263" t="s">
+        <v>692</v>
+      </c>
+      <c r="F263" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>693</v>
+      </c>
+      <c r="B264" t="s">
+        <v>694</v>
+      </c>
+      <c r="D264" t="s">
+        <v>8</v>
+      </c>
+      <c r="E264" t="s">
+        <v>695</v>
+      </c>
+      <c r="F264" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>696</v>
+      </c>
+      <c r="B265" t="s">
+        <v>697</v>
+      </c>
+      <c r="D265" t="s">
+        <v>8</v>
+      </c>
+      <c r="E265" t="s">
+        <v>698</v>
+      </c>
+      <c r="F265" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>699</v>
+      </c>
+      <c r="B266" t="s">
+        <v>700</v>
+      </c>
+      <c r="D266" t="s">
+        <v>8</v>
+      </c>
+      <c r="E266" t="s">
+        <v>701</v>
+      </c>
+      <c r="F266" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>702</v>
+      </c>
+      <c r="B267" t="s">
+        <v>703</v>
+      </c>
+      <c r="D267" t="s">
+        <v>16</v>
+      </c>
+      <c r="E267" t="s">
+        <v>704</v>
+      </c>
+      <c r="F267" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>708</v>
+      </c>
+      <c r="B268" t="s">
+        <v>731</v>
+      </c>
+      <c r="D268" t="s">
+        <v>8</v>
+      </c>
+      <c r="E268" t="s">
+        <v>709</v>
+      </c>
+      <c r="F268" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>713</v>
+      </c>
+      <c r="B269" t="s">
+        <v>714</v>
+      </c>
+      <c r="D269" t="s">
+        <v>8</v>
+      </c>
+      <c r="E269" t="s">
+        <v>715</v>
+      </c>
+      <c r="F269" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>719</v>
+      </c>
+      <c r="B270" t="s">
+        <v>720</v>
+      </c>
+      <c r="D270" t="s">
+        <v>8</v>
+      </c>
+      <c r="E270" t="s">
+        <v>721</v>
+      </c>
+      <c r="F270" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>722</v>
+      </c>
+      <c r="B271" t="s">
+        <v>723</v>
+      </c>
+      <c r="D271" t="s">
+        <v>8</v>
+      </c>
+      <c r="E271" t="s">
+        <v>724</v>
+      </c>
+      <c r="F271" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>725</v>
+      </c>
+      <c r="B272" t="s">
+        <v>726</v>
+      </c>
+      <c r="D272" t="s">
+        <v>8</v>
+      </c>
+      <c r="E272" t="s">
+        <v>727</v>
+      </c>
+      <c r="F272" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>734</v>
+      </c>
+      <c r="B273" t="s">
+        <v>735</v>
+      </c>
+      <c r="C273">
+        <v>220</v>
+      </c>
+      <c r="D273" t="s">
+        <v>736</v>
+      </c>
+      <c r="E273" t="s">
+        <v>698</v>
+      </c>
+      <c r="F273" t="s">
+        <v>737</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F272">
+      <sortCondition ref="C1"/>
+    </sortState>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
update: 1. member status
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C60FA30-4F1D-4CB4-A209-36FE1C679EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA3CE71-4C74-4AE2-BED3-C120D40CFCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$273</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="742">
   <si>
     <t>name</t>
   </si>
@@ -2239,6 +2239,22 @@
   </si>
   <si>
     <t>M</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>离开</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>马文杰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wenjie Ma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -2615,10 +2631,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F273"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="E281" sqref="E281"/>
+    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
+      <selection activeCell="E276" sqref="E276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -2647,7 +2664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2667,7 +2684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2687,7 +2704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2707,7 +2724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2727,7 +2744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2747,7 +2764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -2767,7 +2784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2787,7 +2804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -2807,7 +2824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2827,7 +2844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -2847,7 +2864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -2867,7 +2884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2887,7 +2904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -2907,7 +2924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -2927,7 +2944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -2947,7 +2964,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -2967,7 +2984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -2987,7 +3004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>57</v>
       </c>
@@ -3007,7 +3024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>59</v>
       </c>
@@ -3027,7 +3044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -3047,7 +3064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -3067,7 +3084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -3087,7 +3104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -3107,7 +3124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -3127,7 +3144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -3147,7 +3164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -3167,7 +3184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -3187,7 +3204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -3207,7 +3224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -3227,7 +3244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>87</v>
       </c>
@@ -3247,7 +3264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -3267,7 +3284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>92</v>
       </c>
@@ -3287,7 +3304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -3307,7 +3324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -3327,7 +3344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>99</v>
       </c>
@@ -3347,7 +3364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>101</v>
       </c>
@@ -3367,7 +3384,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>103</v>
       </c>
@@ -3387,7 +3404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>106</v>
       </c>
@@ -3407,7 +3424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>108</v>
       </c>
@@ -3427,7 +3444,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>110</v>
       </c>
@@ -3447,7 +3464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>113</v>
       </c>
@@ -3467,7 +3484,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>116</v>
       </c>
@@ -3487,7 +3504,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>118</v>
       </c>
@@ -3507,7 +3524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>120</v>
       </c>
@@ -3527,7 +3544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>123</v>
       </c>
@@ -3547,7 +3564,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>125</v>
       </c>
@@ -3567,7 +3584,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>127</v>
       </c>
@@ -3587,7 +3604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>130</v>
       </c>
@@ -3607,7 +3624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>132</v>
       </c>
@@ -3627,7 +3644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>134</v>
       </c>
@@ -3647,7 +3664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>136</v>
       </c>
@@ -3667,7 +3684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>138</v>
       </c>
@@ -3687,7 +3704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>141</v>
       </c>
@@ -3707,7 +3724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>143</v>
       </c>
@@ -3727,7 +3744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>146</v>
       </c>
@@ -3747,7 +3764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>148</v>
       </c>
@@ -3767,7 +3784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>150</v>
       </c>
@@ -3787,7 +3804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>153</v>
       </c>
@@ -3807,7 +3824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>155</v>
       </c>
@@ -3827,7 +3844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>157</v>
       </c>
@@ -3847,7 +3864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>160</v>
       </c>
@@ -3867,7 +3884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>163</v>
       </c>
@@ -3887,7 +3904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>165</v>
       </c>
@@ -3907,7 +3924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>167</v>
       </c>
@@ -3927,7 +3944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>170</v>
       </c>
@@ -3947,7 +3964,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>170</v>
       </c>
@@ -3967,7 +3984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>173</v>
       </c>
@@ -3987,7 +4004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>175</v>
       </c>
@@ -4007,7 +4024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>177</v>
       </c>
@@ -4027,7 +4044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>179</v>
       </c>
@@ -4047,7 +4064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>182</v>
       </c>
@@ -4067,7 +4084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>184</v>
       </c>
@@ -4087,7 +4104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>186</v>
       </c>
@@ -4107,7 +4124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>188</v>
       </c>
@@ -4127,7 +4144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>190</v>
       </c>
@@ -4147,7 +4164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>193</v>
       </c>
@@ -4167,7 +4184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -4187,7 +4204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>199</v>
       </c>
@@ -4207,7 +4224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>202</v>
       </c>
@@ -4227,7 +4244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>204</v>
       </c>
@@ -4247,7 +4264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>206</v>
       </c>
@@ -4267,7 +4284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>208</v>
       </c>
@@ -4287,7 +4304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>211</v>
       </c>
@@ -4307,7 +4324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>214</v>
       </c>
@@ -4327,7 +4344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>216</v>
       </c>
@@ -4347,7 +4364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>218</v>
       </c>
@@ -4367,7 +4384,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>220</v>
       </c>
@@ -4387,7 +4404,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>222</v>
       </c>
@@ -4427,7 +4444,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>229</v>
       </c>
@@ -4447,7 +4464,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>232</v>
       </c>
@@ -4487,7 +4504,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>238</v>
       </c>
@@ -4507,7 +4524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>241</v>
       </c>
@@ -4527,7 +4544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>243</v>
       </c>
@@ -4564,10 +4581,10 @@
         <v>247</v>
       </c>
       <c r="F97" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>248</v>
       </c>
@@ -4587,7 +4604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>250</v>
       </c>
@@ -4607,7 +4624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>253</v>
       </c>
@@ -4627,7 +4644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>255</v>
       </c>
@@ -4647,7 +4664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>257</v>
       </c>
@@ -4667,7 +4684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>259</v>
       </c>
@@ -4687,7 +4704,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>261</v>
       </c>
@@ -4747,7 +4764,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>270</v>
       </c>
@@ -4767,7 +4784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>273</v>
       </c>
@@ -4787,7 +4804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>276</v>
       </c>
@@ -4807,7 +4824,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>279</v>
       </c>
@@ -4847,7 +4864,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>285</v>
       </c>
@@ -4867,7 +4884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>287</v>
       </c>
@@ -4887,7 +4904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>289</v>
       </c>
@@ -4907,7 +4924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>291</v>
       </c>
@@ -4927,7 +4944,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>293</v>
       </c>
@@ -4947,7 +4964,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>295</v>
       </c>
@@ -4967,7 +4984,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>297</v>
       </c>
@@ -4987,7 +5004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>299</v>
       </c>
@@ -5007,7 +5024,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>301</v>
       </c>
@@ -5027,7 +5044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>303</v>
       </c>
@@ -5047,7 +5064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>305</v>
       </c>
@@ -5067,7 +5084,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>308</v>
       </c>
@@ -5087,7 +5104,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>310</v>
       </c>
@@ -5107,7 +5124,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>313</v>
       </c>
@@ -5127,7 +5144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>315</v>
       </c>
@@ -5167,7 +5184,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>321</v>
       </c>
@@ -5207,7 +5224,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>327</v>
       </c>
@@ -5227,7 +5244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>329</v>
       </c>
@@ -5247,7 +5264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>332</v>
       </c>
@@ -5267,7 +5284,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>335</v>
       </c>
@@ -5287,7 +5304,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>338</v>
       </c>
@@ -5307,7 +5324,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>341</v>
       </c>
@@ -5524,10 +5541,10 @@
         <v>372</v>
       </c>
       <c r="F145" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>373</v>
       </c>
@@ -5627,7 +5644,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>387</v>
       </c>
@@ -5647,7 +5664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>390</v>
       </c>
@@ -5847,7 +5864,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>420</v>
       </c>
@@ -5907,7 +5924,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>429</v>
       </c>
@@ -5947,7 +5964,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>435</v>
       </c>
@@ -5987,7 +6004,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>441</v>
       </c>
@@ -6067,7 +6084,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>452</v>
       </c>
@@ -6127,7 +6144,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>460</v>
       </c>
@@ -6147,7 +6164,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>463</v>
       </c>
@@ -6167,7 +6184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>465</v>
       </c>
@@ -6187,7 +6204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>467</v>
       </c>
@@ -6227,7 +6244,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>473</v>
       </c>
@@ -6327,7 +6344,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>50</v>
       </c>
@@ -6347,7 +6364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>489</v>
       </c>
@@ -6464,7 +6481,7 @@
         <v>13</v>
       </c>
       <c r="F192" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -6507,7 +6524,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>512</v>
       </c>
@@ -7119,7 +7136,7 @@
         <v>570</v>
       </c>
       <c r="F227" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -7190,7 +7207,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>582</v>
       </c>
@@ -7207,7 +7224,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>585</v>
       </c>
@@ -7261,7 +7278,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>593</v>
       </c>
@@ -7309,7 +7326,7 @@
         <v>13</v>
       </c>
       <c r="F238" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
@@ -7326,7 +7343,7 @@
         <v>603</v>
       </c>
       <c r="F239" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
@@ -7499,7 +7516,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>636</v>
       </c>
@@ -7896,7 +7913,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>734</v>
       </c>
@@ -7916,8 +7933,30 @@
         <v>737</v>
       </c>
     </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>738</v>
+      </c>
+      <c r="B274" t="s">
+        <v>739</v>
+      </c>
+      <c r="D274" t="s">
+        <v>740</v>
+      </c>
+      <c r="E274" t="s">
+        <v>698</v>
+      </c>
+      <c r="F274" t="s">
+        <v>741</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:F273" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="在读"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F272">
       <sortCondition ref="C1"/>
     </sortState>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@1a53047681d18d14f5e0ca717b9f09a511109334 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C60FA30-4F1D-4CB4-A209-36FE1C679EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69FA9C4-3142-4925-B8F9-00D054FA1664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$274</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="745">
   <si>
     <t>name</t>
   </si>
@@ -2243,6 +2243,34 @@
   </si>
   <si>
     <t>离开</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>马文杰</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wenjie Ma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>U</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>离开</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/assets/img/members/student/马文杰.jpg</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2615,10 +2643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F273"/>
+  <dimension ref="A1:F274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="E281" sqref="E281"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="E274" sqref="E274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -4564,7 +4592,7 @@
         <v>247</v>
       </c>
       <c r="F97" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -5524,7 +5552,7 @@
         <v>372</v>
       </c>
       <c r="F145" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -6378,7 +6406,7 @@
         <v>192</v>
       </c>
       <c r="D188" t="s">
-        <v>8</v>
+        <v>743</v>
       </c>
       <c r="E188" t="s">
         <v>494</v>
@@ -6398,7 +6426,7 @@
         <v>193</v>
       </c>
       <c r="D189" t="s">
-        <v>8</v>
+        <v>742</v>
       </c>
       <c r="E189" t="s">
         <v>497</v>
@@ -6418,7 +6446,7 @@
         <v>194</v>
       </c>
       <c r="D190" t="s">
-        <v>8</v>
+        <v>742</v>
       </c>
       <c r="E190" t="s">
         <v>500</v>
@@ -6464,7 +6492,7 @@
         <v>13</v>
       </c>
       <c r="F192" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -6889,7 +6917,7 @@
         <v>526</v>
       </c>
       <c r="D214" t="s">
-        <v>8</v>
+        <v>742</v>
       </c>
       <c r="E214" t="s">
         <v>527</v>
@@ -6957,7 +6985,7 @@
         <v>540</v>
       </c>
       <c r="D218" t="s">
-        <v>8</v>
+        <v>742</v>
       </c>
       <c r="E218" t="s">
         <v>541</v>
@@ -6974,7 +7002,7 @@
         <v>543</v>
       </c>
       <c r="D219" t="s">
-        <v>16</v>
+        <v>742</v>
       </c>
       <c r="E219" t="s">
         <v>13</v>
@@ -7025,7 +7053,7 @@
         <v>550</v>
       </c>
       <c r="D222" t="s">
-        <v>8</v>
+        <v>742</v>
       </c>
       <c r="E222" t="s">
         <v>13</v>
@@ -7119,7 +7147,7 @@
         <v>570</v>
       </c>
       <c r="F227" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -7309,7 +7337,7 @@
         <v>13</v>
       </c>
       <c r="F238" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
@@ -7326,7 +7354,7 @@
         <v>603</v>
       </c>
       <c r="F239" t="s">
-        <v>228</v>
+        <v>10</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
@@ -7916,8 +7944,25 @@
         <v>737</v>
       </c>
     </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>738</v>
+      </c>
+      <c r="B274" t="s">
+        <v>739</v>
+      </c>
+      <c r="D274" t="s">
+        <v>740</v>
+      </c>
+      <c r="E274" t="s">
+        <v>744</v>
+      </c>
+      <c r="F274" t="s">
+        <v>741</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A1:F274" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F272">
       <sortCondition ref="C1"/>
     </sortState>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@f651cb0466a4ea6cfdd5887ff7105b3b627e193a 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69FA9C4-3142-4925-B8F9-00D054FA1664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3253C1F-4C66-4BE2-A2E5-C83310495E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="747">
   <si>
     <t>name</t>
   </si>
@@ -2271,6 +2271,14 @@
   </si>
   <si>
     <t>/assets/img/members/student/马文杰.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2645,8 +2653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
-      <selection activeCell="E274" sqref="E274"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -5986,7 +5994,7 @@
         <v>170</v>
       </c>
       <c r="D167" t="s">
-        <v>16</v>
+        <v>745</v>
       </c>
       <c r="E167" t="s">
         <v>437</v>
@@ -6326,7 +6334,7 @@
         <v>187</v>
       </c>
       <c r="D184" t="s">
-        <v>16</v>
+        <v>745</v>
       </c>
       <c r="E184" t="s">
         <v>484</v>
@@ -6346,7 +6354,7 @@
         <v>189</v>
       </c>
       <c r="D185" t="s">
-        <v>16</v>
+        <v>746</v>
       </c>
       <c r="E185" t="s">
         <v>487</v>
@@ -6466,7 +6474,7 @@
         <v>195</v>
       </c>
       <c r="D191" t="s">
-        <v>16</v>
+        <v>745</v>
       </c>
       <c r="E191" t="s">
         <v>503</v>
@@ -6866,7 +6874,7 @@
         <v>219</v>
       </c>
       <c r="D211" t="s">
-        <v>16</v>
+        <v>745</v>
       </c>
       <c r="E211" t="s">
         <v>613</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@b88bc79678ca8d56e4c22b3524a8f12482a632dc 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3253C1F-4C66-4BE2-A2E5-C83310495E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606379D0-627D-4E7D-8292-56E8C8F6F99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="746">
   <si>
     <t>name</t>
   </si>
@@ -2117,9 +2117,6 @@
   </si>
   <si>
     <t>Xiang Liu</t>
-  </si>
-  <si>
-    <t>../../assets/img/octocat.png</t>
   </si>
   <si>
     <t>王金文</t>
@@ -2653,8 +2650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="D173" sqref="D173"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="E279" sqref="E279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -5994,7 +5991,7 @@
         <v>170</v>
       </c>
       <c r="D167" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E167" t="s">
         <v>437</v>
@@ -6334,7 +6331,7 @@
         <v>187</v>
       </c>
       <c r="D184" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E184" t="s">
         <v>484</v>
@@ -6354,7 +6351,7 @@
         <v>189</v>
       </c>
       <c r="D185" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E185" t="s">
         <v>487</v>
@@ -6414,7 +6411,7 @@
         <v>192</v>
       </c>
       <c r="D188" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E188" t="s">
         <v>494</v>
@@ -6434,7 +6431,7 @@
         <v>193</v>
       </c>
       <c r="D189" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E189" t="s">
         <v>497</v>
@@ -6454,7 +6451,7 @@
         <v>194</v>
       </c>
       <c r="D190" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E190" t="s">
         <v>500</v>
@@ -6474,7 +6471,7 @@
         <v>195</v>
       </c>
       <c r="D191" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E191" t="s">
         <v>503</v>
@@ -6585,10 +6582,10 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
+        <v>727</v>
+      </c>
+      <c r="B197" t="s">
         <v>728</v>
-      </c>
-      <c r="B197" t="s">
-        <v>729</v>
       </c>
       <c r="C197">
         <v>202</v>
@@ -6597,7 +6594,7 @@
         <v>42</v>
       </c>
       <c r="E197" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="F197" t="s">
         <v>228</v>
@@ -6614,7 +6611,7 @@
         <v>203</v>
       </c>
       <c r="D198" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E198" t="s">
         <v>556</v>
@@ -6705,10 +6702,10 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
+        <v>704</v>
+      </c>
+      <c r="B203" t="s">
         <v>705</v>
-      </c>
-      <c r="B203" t="s">
-        <v>706</v>
       </c>
       <c r="C203">
         <v>209</v>
@@ -6717,7 +6714,7 @@
         <v>52</v>
       </c>
       <c r="E203" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F203" t="s">
         <v>228</v>
@@ -6725,10 +6722,10 @@
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
+        <v>715</v>
+      </c>
+      <c r="B204" t="s">
         <v>716</v>
-      </c>
-      <c r="B204" t="s">
-        <v>717</v>
       </c>
       <c r="C204">
         <v>210</v>
@@ -6737,7 +6734,7 @@
         <v>42</v>
       </c>
       <c r="E204" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F204" t="s">
         <v>228</v>
@@ -6805,10 +6802,10 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
+        <v>709</v>
+      </c>
+      <c r="B208" t="s">
         <v>710</v>
-      </c>
-      <c r="B208" t="s">
-        <v>711</v>
       </c>
       <c r="C208">
         <v>216</v>
@@ -6817,7 +6814,7 @@
         <v>20</v>
       </c>
       <c r="E208" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F208" t="s">
         <v>228</v>
@@ -6874,7 +6871,7 @@
         <v>219</v>
       </c>
       <c r="D211" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E211" t="s">
         <v>613</v>
@@ -6925,7 +6922,7 @@
         <v>526</v>
       </c>
       <c r="D214" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E214" t="s">
         <v>527</v>
@@ -6993,7 +6990,7 @@
         <v>540</v>
       </c>
       <c r="D218" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E218" t="s">
         <v>541</v>
@@ -7010,7 +7007,7 @@
         <v>543</v>
       </c>
       <c r="D219" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E219" t="s">
         <v>13</v>
@@ -7061,7 +7058,7 @@
         <v>550</v>
       </c>
       <c r="D222" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E222" t="s">
         <v>13</v>
@@ -7115,7 +7112,7 @@
         <v>212</v>
       </c>
       <c r="D225" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E225" t="s">
         <v>564</v>
@@ -7271,7 +7268,7 @@
         <v>201</v>
       </c>
       <c r="D234" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E234" t="s">
         <v>589</v>
@@ -7807,7 +7804,7 @@
         <v>8</v>
       </c>
       <c r="E265" t="s">
-        <v>698</v>
+        <v>13</v>
       </c>
       <c r="F265" t="s">
         <v>228</v>
@@ -7815,16 +7812,16 @@
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
+        <v>698</v>
+      </c>
+      <c r="B266" t="s">
         <v>699</v>
       </c>
-      <c r="B266" t="s">
+      <c r="D266" t="s">
+        <v>8</v>
+      </c>
+      <c r="E266" t="s">
         <v>700</v>
-      </c>
-      <c r="D266" t="s">
-        <v>8</v>
-      </c>
-      <c r="E266" t="s">
-        <v>701</v>
       </c>
       <c r="F266" t="s">
         <v>228</v>
@@ -7832,16 +7829,16 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
+        <v>701</v>
+      </c>
+      <c r="B267" t="s">
         <v>702</v>
-      </c>
-      <c r="B267" t="s">
-        <v>703</v>
       </c>
       <c r="D267" t="s">
         <v>16</v>
       </c>
       <c r="E267" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F267" t="s">
         <v>228</v>
@@ -7849,16 +7846,16 @@
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
+        <v>707</v>
+      </c>
+      <c r="B268" t="s">
+        <v>730</v>
+      </c>
+      <c r="D268" t="s">
+        <v>8</v>
+      </c>
+      <c r="E268" t="s">
         <v>708</v>
-      </c>
-      <c r="B268" t="s">
-        <v>731</v>
-      </c>
-      <c r="D268" t="s">
-        <v>8</v>
-      </c>
-      <c r="E268" t="s">
-        <v>709</v>
       </c>
       <c r="F268" t="s">
         <v>228</v>
@@ -7866,16 +7863,16 @@
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
+        <v>712</v>
+      </c>
+      <c r="B269" t="s">
         <v>713</v>
       </c>
-      <c r="B269" t="s">
+      <c r="D269" t="s">
+        <v>8</v>
+      </c>
+      <c r="E269" t="s">
         <v>714</v>
-      </c>
-      <c r="D269" t="s">
-        <v>8</v>
-      </c>
-      <c r="E269" t="s">
-        <v>715</v>
       </c>
       <c r="F269" t="s">
         <v>228</v>
@@ -7883,16 +7880,16 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
+        <v>718</v>
+      </c>
+      <c r="B270" t="s">
         <v>719</v>
       </c>
-      <c r="B270" t="s">
+      <c r="D270" t="s">
+        <v>8</v>
+      </c>
+      <c r="E270" t="s">
         <v>720</v>
-      </c>
-      <c r="D270" t="s">
-        <v>8</v>
-      </c>
-      <c r="E270" t="s">
-        <v>721</v>
       </c>
       <c r="F270" t="s">
         <v>228</v>
@@ -7900,16 +7897,16 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
+        <v>721</v>
+      </c>
+      <c r="B271" t="s">
         <v>722</v>
       </c>
-      <c r="B271" t="s">
+      <c r="D271" t="s">
+        <v>8</v>
+      </c>
+      <c r="E271" t="s">
         <v>723</v>
-      </c>
-      <c r="D271" t="s">
-        <v>8</v>
-      </c>
-      <c r="E271" t="s">
-        <v>724</v>
       </c>
       <c r="F271" t="s">
         <v>228</v>
@@ -7917,16 +7914,16 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
+        <v>724</v>
+      </c>
+      <c r="B272" t="s">
         <v>725</v>
       </c>
-      <c r="B272" t="s">
+      <c r="D272" t="s">
+        <v>8</v>
+      </c>
+      <c r="E272" t="s">
         <v>726</v>
-      </c>
-      <c r="D272" t="s">
-        <v>8</v>
-      </c>
-      <c r="E272" t="s">
-        <v>727</v>
       </c>
       <c r="F272" t="s">
         <v>228</v>
@@ -7934,39 +7931,39 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
+        <v>733</v>
+      </c>
+      <c r="B273" t="s">
         <v>734</v>
-      </c>
-      <c r="B273" t="s">
-        <v>735</v>
       </c>
       <c r="C273">
         <v>220</v>
       </c>
       <c r="D273" t="s">
+        <v>735</v>
+      </c>
+      <c r="E273" t="s">
+        <v>13</v>
+      </c>
+      <c r="F273" t="s">
         <v>736</v>
-      </c>
-      <c r="E273" t="s">
-        <v>698</v>
-      </c>
-      <c r="F273" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
+        <v>737</v>
+      </c>
+      <c r="B274" t="s">
         <v>738</v>
       </c>
-      <c r="B274" t="s">
+      <c r="D274" t="s">
         <v>739</v>
       </c>
-      <c r="D274" t="s">
+      <c r="E274" t="s">
+        <v>743</v>
+      </c>
+      <c r="F274" t="s">
         <v>740</v>
-      </c>
-      <c r="E274" t="s">
-        <v>744</v>
-      </c>
-      <c r="F274" t="s">
-        <v>741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: 1. add new members 2. add webpage links
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3EF4F7-73B4-4964-9BD4-2AEF5C911FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABEF13D-FCF5-4F49-864F-2789856418C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2738,8 +2738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="F238" sqref="F238"/>
+    <sheetView tabSelected="1" topLeftCell="A247" workbookViewId="0">
+      <selection activeCell="A257" sqref="A257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -7983,7 +7983,7 @@
         <v>729</v>
       </c>
       <c r="D269" t="s">
-        <v>53</v>
+        <v>778</v>
       </c>
       <c r="E269" t="s">
         <v>730</v>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ X-LANCE/x-lance.github.io@d93e3ad6ff9d58053edb7d4c87811586c1130443 🚀
</commit_message>
<xml_diff>
--- a/process_avatar/final.xlsx
+++ b/process_avatar/final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SJTU\X-LANCE\宣传委员\xlance.github.io\process_avatar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3EF4F7-73B4-4964-9BD4-2AEF5C911FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA4E359-E4D3-45DF-92DA-DD3435AF2F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1438" uniqueCount="784">
   <si>
     <t>name</t>
   </si>
@@ -2315,9 +2315,6 @@
   </si>
   <si>
     <t>Mingxuan Zhu</t>
-  </si>
-  <si>
-    <t>../../assets/img/octocat.png</t>
   </si>
   <si>
     <t>郑时捷</t>
@@ -2365,6 +2362,22 @@
   </si>
   <si>
     <t>/assets/img/members/student/陈博_2.jpg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>王宇飞</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yufei Wang</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2736,10 +2749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G284"/>
+  <dimension ref="A1:G285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="F238" sqref="F238"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="E287" sqref="E287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -4547,7 +4560,7 @@
         <v>228</v>
       </c>
       <c r="F90" t="s">
-        <v>229</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -5290,7 +5303,7 @@
         <v>322</v>
       </c>
       <c r="F127" t="s">
-        <v>229</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -5613,7 +5626,7 @@
         <v>229</v>
       </c>
       <c r="G143" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
@@ -5950,7 +5963,7 @@
         <v>163</v>
       </c>
       <c r="D160" t="s">
-        <v>17</v>
+        <v>781</v>
       </c>
       <c r="E160" t="s">
         <v>419</v>
@@ -6030,7 +6043,7 @@
         <v>167</v>
       </c>
       <c r="D164" t="s">
-        <v>17</v>
+        <v>780</v>
       </c>
       <c r="E164" t="s">
         <v>431</v>
@@ -6482,7 +6495,7 @@
         <v>53</v>
       </c>
       <c r="E186" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F186" t="s">
         <v>11</v>
@@ -7121,7 +7134,7 @@
         <v>14</v>
       </c>
       <c r="F219" t="s">
-        <v>229</v>
+        <v>11</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
@@ -7132,7 +7145,7 @@
         <v>590</v>
       </c>
       <c r="D220" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E220" t="s">
         <v>591</v>
@@ -7983,7 +7996,7 @@
         <v>729</v>
       </c>
       <c r="D269" t="s">
-        <v>53</v>
+        <v>777</v>
       </c>
       <c r="E269" t="s">
         <v>730</v>
@@ -8188,7 +8201,7 @@
         <v>9</v>
       </c>
       <c r="E280" t="s">
-        <v>765</v>
+        <v>14</v>
       </c>
       <c r="F280" t="s">
         <v>229</v>
@@ -8196,16 +8209,16 @@
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
+        <v>765</v>
+      </c>
+      <c r="B281" t="s">
         <v>766</v>
       </c>
-      <c r="B281" t="s">
+      <c r="D281" t="s">
+        <v>9</v>
+      </c>
+      <c r="E281" t="s">
         <v>767</v>
-      </c>
-      <c r="D281" t="s">
-        <v>9</v>
-      </c>
-      <c r="E281" t="s">
-        <v>768</v>
       </c>
       <c r="F281" t="s">
         <v>229</v>
@@ -8213,16 +8226,16 @@
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
+        <v>768</v>
+      </c>
+      <c r="B282" t="s">
         <v>769</v>
-      </c>
-      <c r="B282" t="s">
-        <v>770</v>
       </c>
       <c r="D282" t="s">
         <v>17</v>
       </c>
       <c r="E282" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F282" t="s">
         <v>229</v>
@@ -8230,16 +8243,16 @@
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
+        <v>771</v>
+      </c>
+      <c r="B283" t="s">
         <v>772</v>
       </c>
-      <c r="B283" t="s">
+      <c r="D283" t="s">
+        <v>9</v>
+      </c>
+      <c r="E283" t="s">
         <v>773</v>
-      </c>
-      <c r="D283" t="s">
-        <v>9</v>
-      </c>
-      <c r="E283" t="s">
-        <v>774</v>
       </c>
       <c r="F283" t="s">
         <v>229</v>
@@ -8247,19 +8260,36 @@
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
+        <v>774</v>
+      </c>
+      <c r="B284" t="s">
         <v>775</v>
       </c>
-      <c r="B284" t="s">
+      <c r="D284" t="s">
+        <v>9</v>
+      </c>
+      <c r="E284" t="s">
         <v>776</v>
       </c>
-      <c r="D284" t="s">
-        <v>9</v>
-      </c>
-      <c r="E284" t="s">
-        <v>777</v>
-      </c>
       <c r="F284" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>782</v>
+      </c>
+      <c r="B285" t="s">
+        <v>783</v>
+      </c>
+      <c r="D285" t="s">
+        <v>781</v>
+      </c>
+      <c r="E285" t="s">
+        <v>14</v>
+      </c>
+      <c r="F285" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>